<commit_message>
Add Case Shiller page
</commit_message>
<xml_diff>
--- a/layouts.xlsx
+++ b/layouts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/046b73b793af0aea/PAMGMT/projects/tamarac/economic-market-commentary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="331" documentId="8_{16FB9176-5700-CA44-8DDA-ADDCE61D2EC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C8200912-01EB-F04D-BAFC-72935C49BB62}"/>
+  <xr:revisionPtr revIDLastSave="342" documentId="8_{16FB9176-5700-CA44-8DDA-ADDCE61D2EC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CA9BDEAF-3996-FB4E-8771-876C4E8F7577}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="1600" windowWidth="28040" windowHeight="18100" activeTab="10" xr2:uid="{7344E464-CEB7-A74D-A529-F1BDE3AF96EC}"/>
+    <workbookView xWindow="3900" yWindow="1600" windowWidth="28040" windowHeight="18100" activeTab="11" xr2:uid="{7344E464-CEB7-A74D-A529-F1BDE3AF96EC}"/>
   </bookViews>
   <sheets>
     <sheet name="lay-1" sheetId="2" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="lay-9" sheetId="11" r:id="rId9"/>
     <sheet name="lay-10" sheetId="12" r:id="rId10"/>
     <sheet name="lay-11" sheetId="13" r:id="rId11"/>
+    <sheet name="lay-12" sheetId="14" r:id="rId12"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="41">
   <si>
     <t>a</t>
   </si>
@@ -181,7 +182,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -251,6 +252,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -347,7 +360,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -373,6 +386,8 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7440,7 +7455,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA7830CE-41DB-244E-BF33-1B0680A4704E}">
   <dimension ref="A1:AN28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
@@ -10863,6 +10878,3440 @@
       </c>
       <c r="AN28" s="24">
         <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88058F12-8899-DA4C-9FD4-20DF326DCD54}">
+  <dimension ref="A1:AN28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AR25" sqref="AR25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="40" width="3.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>40</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1">
+        <v>1</v>
+      </c>
+      <c r="I2" s="1">
+        <v>1</v>
+      </c>
+      <c r="J2" s="1">
+        <v>1</v>
+      </c>
+      <c r="K2" s="1">
+        <v>1</v>
+      </c>
+      <c r="L2" s="1">
+        <v>1</v>
+      </c>
+      <c r="M2" s="1">
+        <v>1</v>
+      </c>
+      <c r="N2" s="1">
+        <v>1</v>
+      </c>
+      <c r="O2" s="1">
+        <v>1</v>
+      </c>
+      <c r="P2" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>1</v>
+      </c>
+      <c r="R2" s="1">
+        <v>1</v>
+      </c>
+      <c r="S2" s="1">
+        <v>1</v>
+      </c>
+      <c r="T2" s="1">
+        <v>1</v>
+      </c>
+      <c r="U2" s="1">
+        <v>1</v>
+      </c>
+      <c r="V2" s="1">
+        <v>1</v>
+      </c>
+      <c r="W2" s="1">
+        <v>1</v>
+      </c>
+      <c r="X2" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AM2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1">
+        <v>1</v>
+      </c>
+      <c r="J3" s="1">
+        <v>1</v>
+      </c>
+      <c r="K3" s="1">
+        <v>1</v>
+      </c>
+      <c r="L3" s="1">
+        <v>1</v>
+      </c>
+      <c r="M3" s="1">
+        <v>1</v>
+      </c>
+      <c r="N3" s="1">
+        <v>1</v>
+      </c>
+      <c r="O3" s="1">
+        <v>1</v>
+      </c>
+      <c r="P3" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>1</v>
+      </c>
+      <c r="R3" s="1">
+        <v>1</v>
+      </c>
+      <c r="S3" s="1">
+        <v>1</v>
+      </c>
+      <c r="T3" s="1">
+        <v>1</v>
+      </c>
+      <c r="U3" s="1">
+        <v>1</v>
+      </c>
+      <c r="V3" s="1">
+        <v>1</v>
+      </c>
+      <c r="W3" s="1">
+        <v>1</v>
+      </c>
+      <c r="X3" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y3" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AM3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1</v>
+      </c>
+      <c r="I4" s="1">
+        <v>1</v>
+      </c>
+      <c r="J4" s="1">
+        <v>1</v>
+      </c>
+      <c r="K4" s="1">
+        <v>1</v>
+      </c>
+      <c r="L4" s="1">
+        <v>1</v>
+      </c>
+      <c r="M4" s="1">
+        <v>1</v>
+      </c>
+      <c r="N4" s="1">
+        <v>1</v>
+      </c>
+      <c r="O4" s="1">
+        <v>1</v>
+      </c>
+      <c r="P4" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>1</v>
+      </c>
+      <c r="R4" s="1">
+        <v>1</v>
+      </c>
+      <c r="S4" s="1">
+        <v>1</v>
+      </c>
+      <c r="T4" s="1">
+        <v>1</v>
+      </c>
+      <c r="U4" s="1">
+        <v>1</v>
+      </c>
+      <c r="V4" s="1">
+        <v>1</v>
+      </c>
+      <c r="W4" s="1">
+        <v>1</v>
+      </c>
+      <c r="X4" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y4" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AM4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="18">
+        <v>2</v>
+      </c>
+      <c r="B5" s="18">
+        <v>2</v>
+      </c>
+      <c r="C5" s="18">
+        <v>2</v>
+      </c>
+      <c r="D5" s="18">
+        <v>2</v>
+      </c>
+      <c r="E5" s="18">
+        <v>2</v>
+      </c>
+      <c r="F5" s="18">
+        <v>2</v>
+      </c>
+      <c r="G5" s="18">
+        <v>2</v>
+      </c>
+      <c r="H5" s="18">
+        <v>2</v>
+      </c>
+      <c r="I5" s="18">
+        <v>2</v>
+      </c>
+      <c r="J5" s="18">
+        <v>2</v>
+      </c>
+      <c r="K5" s="18">
+        <v>2</v>
+      </c>
+      <c r="L5" s="18">
+        <v>2</v>
+      </c>
+      <c r="M5" s="18">
+        <v>2</v>
+      </c>
+      <c r="N5" s="18">
+        <v>2</v>
+      </c>
+      <c r="O5" s="18">
+        <v>2</v>
+      </c>
+      <c r="P5" s="18">
+        <v>2</v>
+      </c>
+      <c r="Q5" s="18">
+        <v>2</v>
+      </c>
+      <c r="R5" s="18">
+        <v>2</v>
+      </c>
+      <c r="S5" s="18">
+        <v>2</v>
+      </c>
+      <c r="T5" s="18">
+        <v>2</v>
+      </c>
+      <c r="U5" s="25">
+        <v>3</v>
+      </c>
+      <c r="V5" s="25">
+        <v>3</v>
+      </c>
+      <c r="W5" s="25">
+        <v>3</v>
+      </c>
+      <c r="X5" s="25">
+        <v>3</v>
+      </c>
+      <c r="Y5" s="25">
+        <v>3</v>
+      </c>
+      <c r="Z5" s="25">
+        <v>3</v>
+      </c>
+      <c r="AA5" s="25">
+        <v>3</v>
+      </c>
+      <c r="AB5" s="25">
+        <v>3</v>
+      </c>
+      <c r="AC5" s="25">
+        <v>3</v>
+      </c>
+      <c r="AD5" s="25">
+        <v>3</v>
+      </c>
+      <c r="AE5" s="25">
+        <v>3</v>
+      </c>
+      <c r="AF5" s="25">
+        <v>3</v>
+      </c>
+      <c r="AG5" s="25">
+        <v>3</v>
+      </c>
+      <c r="AH5" s="25">
+        <v>3</v>
+      </c>
+      <c r="AI5" s="25">
+        <v>3</v>
+      </c>
+      <c r="AJ5" s="25">
+        <v>3</v>
+      </c>
+      <c r="AK5" s="25">
+        <v>3</v>
+      </c>
+      <c r="AL5" s="25">
+        <v>3</v>
+      </c>
+      <c r="AM5" s="25">
+        <v>3</v>
+      </c>
+      <c r="AN5" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="18">
+        <v>2</v>
+      </c>
+      <c r="B6" s="18">
+        <v>2</v>
+      </c>
+      <c r="C6" s="18">
+        <v>2</v>
+      </c>
+      <c r="D6" s="18">
+        <v>2</v>
+      </c>
+      <c r="E6" s="18">
+        <v>2</v>
+      </c>
+      <c r="F6" s="18">
+        <v>2</v>
+      </c>
+      <c r="G6" s="18">
+        <v>2</v>
+      </c>
+      <c r="H6" s="18">
+        <v>2</v>
+      </c>
+      <c r="I6" s="18">
+        <v>2</v>
+      </c>
+      <c r="J6" s="18">
+        <v>2</v>
+      </c>
+      <c r="K6" s="18">
+        <v>2</v>
+      </c>
+      <c r="L6" s="18">
+        <v>2</v>
+      </c>
+      <c r="M6" s="18">
+        <v>2</v>
+      </c>
+      <c r="N6" s="18">
+        <v>2</v>
+      </c>
+      <c r="O6" s="18">
+        <v>2</v>
+      </c>
+      <c r="P6" s="18">
+        <v>2</v>
+      </c>
+      <c r="Q6" s="18">
+        <v>2</v>
+      </c>
+      <c r="R6" s="18">
+        <v>2</v>
+      </c>
+      <c r="S6" s="18">
+        <v>2</v>
+      </c>
+      <c r="T6" s="18">
+        <v>2</v>
+      </c>
+      <c r="U6" s="25">
+        <v>3</v>
+      </c>
+      <c r="V6" s="25">
+        <v>3</v>
+      </c>
+      <c r="W6" s="25">
+        <v>3</v>
+      </c>
+      <c r="X6" s="25">
+        <v>3</v>
+      </c>
+      <c r="Y6" s="25">
+        <v>3</v>
+      </c>
+      <c r="Z6" s="25">
+        <v>3</v>
+      </c>
+      <c r="AA6" s="25">
+        <v>3</v>
+      </c>
+      <c r="AB6" s="25">
+        <v>3</v>
+      </c>
+      <c r="AC6" s="25">
+        <v>3</v>
+      </c>
+      <c r="AD6" s="25">
+        <v>3</v>
+      </c>
+      <c r="AE6" s="25">
+        <v>3</v>
+      </c>
+      <c r="AF6" s="25">
+        <v>3</v>
+      </c>
+      <c r="AG6" s="25">
+        <v>3</v>
+      </c>
+      <c r="AH6" s="25">
+        <v>3</v>
+      </c>
+      <c r="AI6" s="25">
+        <v>3</v>
+      </c>
+      <c r="AJ6" s="25">
+        <v>3</v>
+      </c>
+      <c r="AK6" s="25">
+        <v>3</v>
+      </c>
+      <c r="AL6" s="25">
+        <v>3</v>
+      </c>
+      <c r="AM6" s="25">
+        <v>3</v>
+      </c>
+      <c r="AN6" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="18">
+        <v>2</v>
+      </c>
+      <c r="B7" s="18">
+        <v>2</v>
+      </c>
+      <c r="C7" s="18">
+        <v>2</v>
+      </c>
+      <c r="D7" s="18">
+        <v>2</v>
+      </c>
+      <c r="E7" s="18">
+        <v>2</v>
+      </c>
+      <c r="F7" s="18">
+        <v>2</v>
+      </c>
+      <c r="G7" s="18">
+        <v>2</v>
+      </c>
+      <c r="H7" s="18">
+        <v>2</v>
+      </c>
+      <c r="I7" s="18">
+        <v>2</v>
+      </c>
+      <c r="J7" s="18">
+        <v>2</v>
+      </c>
+      <c r="K7" s="18">
+        <v>2</v>
+      </c>
+      <c r="L7" s="18">
+        <v>2</v>
+      </c>
+      <c r="M7" s="18">
+        <v>2</v>
+      </c>
+      <c r="N7" s="18">
+        <v>2</v>
+      </c>
+      <c r="O7" s="18">
+        <v>2</v>
+      </c>
+      <c r="P7" s="18">
+        <v>2</v>
+      </c>
+      <c r="Q7" s="18">
+        <v>2</v>
+      </c>
+      <c r="R7" s="18">
+        <v>2</v>
+      </c>
+      <c r="S7" s="18">
+        <v>2</v>
+      </c>
+      <c r="T7" s="18">
+        <v>2</v>
+      </c>
+      <c r="U7" s="25">
+        <v>3</v>
+      </c>
+      <c r="V7" s="25">
+        <v>3</v>
+      </c>
+      <c r="W7" s="25">
+        <v>3</v>
+      </c>
+      <c r="X7" s="25">
+        <v>3</v>
+      </c>
+      <c r="Y7" s="25">
+        <v>3</v>
+      </c>
+      <c r="Z7" s="25">
+        <v>3</v>
+      </c>
+      <c r="AA7" s="25">
+        <v>3</v>
+      </c>
+      <c r="AB7" s="25">
+        <v>3</v>
+      </c>
+      <c r="AC7" s="25">
+        <v>3</v>
+      </c>
+      <c r="AD7" s="25">
+        <v>3</v>
+      </c>
+      <c r="AE7" s="25">
+        <v>3</v>
+      </c>
+      <c r="AF7" s="25">
+        <v>3</v>
+      </c>
+      <c r="AG7" s="25">
+        <v>3</v>
+      </c>
+      <c r="AH7" s="25">
+        <v>3</v>
+      </c>
+      <c r="AI7" s="25">
+        <v>3</v>
+      </c>
+      <c r="AJ7" s="25">
+        <v>3</v>
+      </c>
+      <c r="AK7" s="25">
+        <v>3</v>
+      </c>
+      <c r="AL7" s="25">
+        <v>3</v>
+      </c>
+      <c r="AM7" s="25">
+        <v>3</v>
+      </c>
+      <c r="AN7" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="18">
+        <v>2</v>
+      </c>
+      <c r="B8" s="18">
+        <v>2</v>
+      </c>
+      <c r="C8" s="18">
+        <v>2</v>
+      </c>
+      <c r="D8" s="18">
+        <v>2</v>
+      </c>
+      <c r="E8" s="18">
+        <v>2</v>
+      </c>
+      <c r="F8" s="18">
+        <v>2</v>
+      </c>
+      <c r="G8" s="18">
+        <v>2</v>
+      </c>
+      <c r="H8" s="18">
+        <v>2</v>
+      </c>
+      <c r="I8" s="18">
+        <v>2</v>
+      </c>
+      <c r="J8" s="18">
+        <v>2</v>
+      </c>
+      <c r="K8" s="18">
+        <v>2</v>
+      </c>
+      <c r="L8" s="18">
+        <v>2</v>
+      </c>
+      <c r="M8" s="18">
+        <v>2</v>
+      </c>
+      <c r="N8" s="18">
+        <v>2</v>
+      </c>
+      <c r="O8" s="18">
+        <v>2</v>
+      </c>
+      <c r="P8" s="18">
+        <v>2</v>
+      </c>
+      <c r="Q8" s="18">
+        <v>2</v>
+      </c>
+      <c r="R8" s="18">
+        <v>2</v>
+      </c>
+      <c r="S8" s="18">
+        <v>2</v>
+      </c>
+      <c r="T8" s="18">
+        <v>2</v>
+      </c>
+      <c r="U8" s="25">
+        <v>3</v>
+      </c>
+      <c r="V8" s="25">
+        <v>3</v>
+      </c>
+      <c r="W8" s="25">
+        <v>3</v>
+      </c>
+      <c r="X8" s="25">
+        <v>3</v>
+      </c>
+      <c r="Y8" s="25">
+        <v>3</v>
+      </c>
+      <c r="Z8" s="25">
+        <v>3</v>
+      </c>
+      <c r="AA8" s="25">
+        <v>3</v>
+      </c>
+      <c r="AB8" s="25">
+        <v>3</v>
+      </c>
+      <c r="AC8" s="25">
+        <v>3</v>
+      </c>
+      <c r="AD8" s="25">
+        <v>3</v>
+      </c>
+      <c r="AE8" s="25">
+        <v>3</v>
+      </c>
+      <c r="AF8" s="25">
+        <v>3</v>
+      </c>
+      <c r="AG8" s="25">
+        <v>3</v>
+      </c>
+      <c r="AH8" s="25">
+        <v>3</v>
+      </c>
+      <c r="AI8" s="25">
+        <v>3</v>
+      </c>
+      <c r="AJ8" s="25">
+        <v>3</v>
+      </c>
+      <c r="AK8" s="25">
+        <v>3</v>
+      </c>
+      <c r="AL8" s="25">
+        <v>3</v>
+      </c>
+      <c r="AM8" s="25">
+        <v>3</v>
+      </c>
+      <c r="AN8" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="18">
+        <v>2</v>
+      </c>
+      <c r="B9" s="18">
+        <v>2</v>
+      </c>
+      <c r="C9" s="18">
+        <v>2</v>
+      </c>
+      <c r="D9" s="18">
+        <v>2</v>
+      </c>
+      <c r="E9" s="18">
+        <v>2</v>
+      </c>
+      <c r="F9" s="18">
+        <v>2</v>
+      </c>
+      <c r="G9" s="18">
+        <v>2</v>
+      </c>
+      <c r="H9" s="18">
+        <v>2</v>
+      </c>
+      <c r="I9" s="18">
+        <v>2</v>
+      </c>
+      <c r="J9" s="18">
+        <v>2</v>
+      </c>
+      <c r="K9" s="18">
+        <v>2</v>
+      </c>
+      <c r="L9" s="18">
+        <v>2</v>
+      </c>
+      <c r="M9" s="18">
+        <v>2</v>
+      </c>
+      <c r="N9" s="18">
+        <v>2</v>
+      </c>
+      <c r="O9" s="18">
+        <v>2</v>
+      </c>
+      <c r="P9" s="18">
+        <v>2</v>
+      </c>
+      <c r="Q9" s="18">
+        <v>2</v>
+      </c>
+      <c r="R9" s="18">
+        <v>2</v>
+      </c>
+      <c r="S9" s="18">
+        <v>2</v>
+      </c>
+      <c r="T9" s="18">
+        <v>2</v>
+      </c>
+      <c r="U9" s="25">
+        <v>3</v>
+      </c>
+      <c r="V9" s="25">
+        <v>3</v>
+      </c>
+      <c r="W9" s="25">
+        <v>3</v>
+      </c>
+      <c r="X9" s="25">
+        <v>3</v>
+      </c>
+      <c r="Y9" s="25">
+        <v>3</v>
+      </c>
+      <c r="Z9" s="25">
+        <v>3</v>
+      </c>
+      <c r="AA9" s="25">
+        <v>3</v>
+      </c>
+      <c r="AB9" s="25">
+        <v>3</v>
+      </c>
+      <c r="AC9" s="25">
+        <v>3</v>
+      </c>
+      <c r="AD9" s="25">
+        <v>3</v>
+      </c>
+      <c r="AE9" s="25">
+        <v>3</v>
+      </c>
+      <c r="AF9" s="25">
+        <v>3</v>
+      </c>
+      <c r="AG9" s="25">
+        <v>3</v>
+      </c>
+      <c r="AH9" s="25">
+        <v>3</v>
+      </c>
+      <c r="AI9" s="25">
+        <v>3</v>
+      </c>
+      <c r="AJ9" s="25">
+        <v>3</v>
+      </c>
+      <c r="AK9" s="25">
+        <v>3</v>
+      </c>
+      <c r="AL9" s="25">
+        <v>3</v>
+      </c>
+      <c r="AM9" s="25">
+        <v>3</v>
+      </c>
+      <c r="AN9" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="18">
+        <v>2</v>
+      </c>
+      <c r="B10" s="18">
+        <v>2</v>
+      </c>
+      <c r="C10" s="18">
+        <v>2</v>
+      </c>
+      <c r="D10" s="18">
+        <v>2</v>
+      </c>
+      <c r="E10" s="18">
+        <v>2</v>
+      </c>
+      <c r="F10" s="18">
+        <v>2</v>
+      </c>
+      <c r="G10" s="18">
+        <v>2</v>
+      </c>
+      <c r="H10" s="18">
+        <v>2</v>
+      </c>
+      <c r="I10" s="18">
+        <v>2</v>
+      </c>
+      <c r="J10" s="18">
+        <v>2</v>
+      </c>
+      <c r="K10" s="18">
+        <v>2</v>
+      </c>
+      <c r="L10" s="18">
+        <v>2</v>
+      </c>
+      <c r="M10" s="18">
+        <v>2</v>
+      </c>
+      <c r="N10" s="18">
+        <v>2</v>
+      </c>
+      <c r="O10" s="18">
+        <v>2</v>
+      </c>
+      <c r="P10" s="18">
+        <v>2</v>
+      </c>
+      <c r="Q10" s="18">
+        <v>2</v>
+      </c>
+      <c r="R10" s="18">
+        <v>2</v>
+      </c>
+      <c r="S10" s="18">
+        <v>2</v>
+      </c>
+      <c r="T10" s="18">
+        <v>2</v>
+      </c>
+      <c r="U10" s="25">
+        <v>3</v>
+      </c>
+      <c r="V10" s="25">
+        <v>3</v>
+      </c>
+      <c r="W10" s="25">
+        <v>3</v>
+      </c>
+      <c r="X10" s="25">
+        <v>3</v>
+      </c>
+      <c r="Y10" s="25">
+        <v>3</v>
+      </c>
+      <c r="Z10" s="25">
+        <v>3</v>
+      </c>
+      <c r="AA10" s="25">
+        <v>3</v>
+      </c>
+      <c r="AB10" s="25">
+        <v>3</v>
+      </c>
+      <c r="AC10" s="25">
+        <v>3</v>
+      </c>
+      <c r="AD10" s="25">
+        <v>3</v>
+      </c>
+      <c r="AE10" s="25">
+        <v>3</v>
+      </c>
+      <c r="AF10" s="25">
+        <v>3</v>
+      </c>
+      <c r="AG10" s="25">
+        <v>3</v>
+      </c>
+      <c r="AH10" s="25">
+        <v>3</v>
+      </c>
+      <c r="AI10" s="25">
+        <v>3</v>
+      </c>
+      <c r="AJ10" s="25">
+        <v>3</v>
+      </c>
+      <c r="AK10" s="25">
+        <v>3</v>
+      </c>
+      <c r="AL10" s="25">
+        <v>3</v>
+      </c>
+      <c r="AM10" s="25">
+        <v>3</v>
+      </c>
+      <c r="AN10" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="18">
+        <v>2</v>
+      </c>
+      <c r="B11" s="18">
+        <v>2</v>
+      </c>
+      <c r="C11" s="18">
+        <v>2</v>
+      </c>
+      <c r="D11" s="18">
+        <v>2</v>
+      </c>
+      <c r="E11" s="18">
+        <v>2</v>
+      </c>
+      <c r="F11" s="18">
+        <v>2</v>
+      </c>
+      <c r="G11" s="18">
+        <v>2</v>
+      </c>
+      <c r="H11" s="18">
+        <v>2</v>
+      </c>
+      <c r="I11" s="18">
+        <v>2</v>
+      </c>
+      <c r="J11" s="18">
+        <v>2</v>
+      </c>
+      <c r="K11" s="18">
+        <v>2</v>
+      </c>
+      <c r="L11" s="18">
+        <v>2</v>
+      </c>
+      <c r="M11" s="18">
+        <v>2</v>
+      </c>
+      <c r="N11" s="18">
+        <v>2</v>
+      </c>
+      <c r="O11" s="18">
+        <v>2</v>
+      </c>
+      <c r="P11" s="18">
+        <v>2</v>
+      </c>
+      <c r="Q11" s="18">
+        <v>2</v>
+      </c>
+      <c r="R11" s="18">
+        <v>2</v>
+      </c>
+      <c r="S11" s="18">
+        <v>2</v>
+      </c>
+      <c r="T11" s="18">
+        <v>2</v>
+      </c>
+      <c r="U11" s="25">
+        <v>3</v>
+      </c>
+      <c r="V11" s="25">
+        <v>3</v>
+      </c>
+      <c r="W11" s="25">
+        <v>3</v>
+      </c>
+      <c r="X11" s="25">
+        <v>3</v>
+      </c>
+      <c r="Y11" s="25">
+        <v>3</v>
+      </c>
+      <c r="Z11" s="25">
+        <v>3</v>
+      </c>
+      <c r="AA11" s="25">
+        <v>3</v>
+      </c>
+      <c r="AB11" s="25">
+        <v>3</v>
+      </c>
+      <c r="AC11" s="25">
+        <v>3</v>
+      </c>
+      <c r="AD11" s="25">
+        <v>3</v>
+      </c>
+      <c r="AE11" s="25">
+        <v>3</v>
+      </c>
+      <c r="AF11" s="25">
+        <v>3</v>
+      </c>
+      <c r="AG11" s="25">
+        <v>3</v>
+      </c>
+      <c r="AH11" s="25">
+        <v>3</v>
+      </c>
+      <c r="AI11" s="25">
+        <v>3</v>
+      </c>
+      <c r="AJ11" s="25">
+        <v>3</v>
+      </c>
+      <c r="AK11" s="25">
+        <v>3</v>
+      </c>
+      <c r="AL11" s="25">
+        <v>3</v>
+      </c>
+      <c r="AM11" s="25">
+        <v>3</v>
+      </c>
+      <c r="AN11" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="18">
+        <v>2</v>
+      </c>
+      <c r="B12" s="18">
+        <v>2</v>
+      </c>
+      <c r="C12" s="18">
+        <v>2</v>
+      </c>
+      <c r="D12" s="18">
+        <v>2</v>
+      </c>
+      <c r="E12" s="18">
+        <v>2</v>
+      </c>
+      <c r="F12" s="18">
+        <v>2</v>
+      </c>
+      <c r="G12" s="18">
+        <v>2</v>
+      </c>
+      <c r="H12" s="18">
+        <v>2</v>
+      </c>
+      <c r="I12" s="18">
+        <v>2</v>
+      </c>
+      <c r="J12" s="18">
+        <v>2</v>
+      </c>
+      <c r="K12" s="18">
+        <v>2</v>
+      </c>
+      <c r="L12" s="18">
+        <v>2</v>
+      </c>
+      <c r="M12" s="18">
+        <v>2</v>
+      </c>
+      <c r="N12" s="18">
+        <v>2</v>
+      </c>
+      <c r="O12" s="18">
+        <v>2</v>
+      </c>
+      <c r="P12" s="18">
+        <v>2</v>
+      </c>
+      <c r="Q12" s="18">
+        <v>2</v>
+      </c>
+      <c r="R12" s="18">
+        <v>2</v>
+      </c>
+      <c r="S12" s="18">
+        <v>2</v>
+      </c>
+      <c r="T12" s="18">
+        <v>2</v>
+      </c>
+      <c r="U12" s="25">
+        <v>3</v>
+      </c>
+      <c r="V12" s="25">
+        <v>3</v>
+      </c>
+      <c r="W12" s="25">
+        <v>3</v>
+      </c>
+      <c r="X12" s="25">
+        <v>3</v>
+      </c>
+      <c r="Y12" s="25">
+        <v>3</v>
+      </c>
+      <c r="Z12" s="25">
+        <v>3</v>
+      </c>
+      <c r="AA12" s="25">
+        <v>3</v>
+      </c>
+      <c r="AB12" s="25">
+        <v>3</v>
+      </c>
+      <c r="AC12" s="25">
+        <v>3</v>
+      </c>
+      <c r="AD12" s="25">
+        <v>3</v>
+      </c>
+      <c r="AE12" s="25">
+        <v>3</v>
+      </c>
+      <c r="AF12" s="25">
+        <v>3</v>
+      </c>
+      <c r="AG12" s="25">
+        <v>3</v>
+      </c>
+      <c r="AH12" s="25">
+        <v>3</v>
+      </c>
+      <c r="AI12" s="25">
+        <v>3</v>
+      </c>
+      <c r="AJ12" s="25">
+        <v>3</v>
+      </c>
+      <c r="AK12" s="25">
+        <v>3</v>
+      </c>
+      <c r="AL12" s="25">
+        <v>3</v>
+      </c>
+      <c r="AM12" s="25">
+        <v>3</v>
+      </c>
+      <c r="AN12" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="18">
+        <v>2</v>
+      </c>
+      <c r="B13" s="18">
+        <v>2</v>
+      </c>
+      <c r="C13" s="18">
+        <v>2</v>
+      </c>
+      <c r="D13" s="18">
+        <v>2</v>
+      </c>
+      <c r="E13" s="18">
+        <v>2</v>
+      </c>
+      <c r="F13" s="18">
+        <v>2</v>
+      </c>
+      <c r="G13" s="18">
+        <v>2</v>
+      </c>
+      <c r="H13" s="18">
+        <v>2</v>
+      </c>
+      <c r="I13" s="18">
+        <v>2</v>
+      </c>
+      <c r="J13" s="18">
+        <v>2</v>
+      </c>
+      <c r="K13" s="18">
+        <v>2</v>
+      </c>
+      <c r="L13" s="18">
+        <v>2</v>
+      </c>
+      <c r="M13" s="18">
+        <v>2</v>
+      </c>
+      <c r="N13" s="18">
+        <v>2</v>
+      </c>
+      <c r="O13" s="18">
+        <v>2</v>
+      </c>
+      <c r="P13" s="18">
+        <v>2</v>
+      </c>
+      <c r="Q13" s="18">
+        <v>2</v>
+      </c>
+      <c r="R13" s="18">
+        <v>2</v>
+      </c>
+      <c r="S13" s="18">
+        <v>2</v>
+      </c>
+      <c r="T13" s="18">
+        <v>2</v>
+      </c>
+      <c r="U13" s="25">
+        <v>3</v>
+      </c>
+      <c r="V13" s="25">
+        <v>3</v>
+      </c>
+      <c r="W13" s="25">
+        <v>3</v>
+      </c>
+      <c r="X13" s="25">
+        <v>3</v>
+      </c>
+      <c r="Y13" s="25">
+        <v>3</v>
+      </c>
+      <c r="Z13" s="25">
+        <v>3</v>
+      </c>
+      <c r="AA13" s="25">
+        <v>3</v>
+      </c>
+      <c r="AB13" s="25">
+        <v>3</v>
+      </c>
+      <c r="AC13" s="25">
+        <v>3</v>
+      </c>
+      <c r="AD13" s="25">
+        <v>3</v>
+      </c>
+      <c r="AE13" s="25">
+        <v>3</v>
+      </c>
+      <c r="AF13" s="25">
+        <v>3</v>
+      </c>
+      <c r="AG13" s="25">
+        <v>3</v>
+      </c>
+      <c r="AH13" s="25">
+        <v>3</v>
+      </c>
+      <c r="AI13" s="25">
+        <v>3</v>
+      </c>
+      <c r="AJ13" s="25">
+        <v>3</v>
+      </c>
+      <c r="AK13" s="25">
+        <v>3</v>
+      </c>
+      <c r="AL13" s="25">
+        <v>3</v>
+      </c>
+      <c r="AM13" s="25">
+        <v>3</v>
+      </c>
+      <c r="AN13" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="18">
+        <v>2</v>
+      </c>
+      <c r="B14" s="18">
+        <v>2</v>
+      </c>
+      <c r="C14" s="18">
+        <v>2</v>
+      </c>
+      <c r="D14" s="18">
+        <v>2</v>
+      </c>
+      <c r="E14" s="18">
+        <v>2</v>
+      </c>
+      <c r="F14" s="18">
+        <v>2</v>
+      </c>
+      <c r="G14" s="18">
+        <v>2</v>
+      </c>
+      <c r="H14" s="18">
+        <v>2</v>
+      </c>
+      <c r="I14" s="18">
+        <v>2</v>
+      </c>
+      <c r="J14" s="18">
+        <v>2</v>
+      </c>
+      <c r="K14" s="18">
+        <v>2</v>
+      </c>
+      <c r="L14" s="18">
+        <v>2</v>
+      </c>
+      <c r="M14" s="18">
+        <v>2</v>
+      </c>
+      <c r="N14" s="18">
+        <v>2</v>
+      </c>
+      <c r="O14" s="18">
+        <v>2</v>
+      </c>
+      <c r="P14" s="18">
+        <v>2</v>
+      </c>
+      <c r="Q14" s="18">
+        <v>2</v>
+      </c>
+      <c r="R14" s="18">
+        <v>2</v>
+      </c>
+      <c r="S14" s="18">
+        <v>2</v>
+      </c>
+      <c r="T14" s="18">
+        <v>2</v>
+      </c>
+      <c r="U14" s="25">
+        <v>3</v>
+      </c>
+      <c r="V14" s="25">
+        <v>3</v>
+      </c>
+      <c r="W14" s="25">
+        <v>3</v>
+      </c>
+      <c r="X14" s="25">
+        <v>3</v>
+      </c>
+      <c r="Y14" s="25">
+        <v>3</v>
+      </c>
+      <c r="Z14" s="25">
+        <v>3</v>
+      </c>
+      <c r="AA14" s="25">
+        <v>3</v>
+      </c>
+      <c r="AB14" s="25">
+        <v>3</v>
+      </c>
+      <c r="AC14" s="25">
+        <v>3</v>
+      </c>
+      <c r="AD14" s="25">
+        <v>3</v>
+      </c>
+      <c r="AE14" s="25">
+        <v>3</v>
+      </c>
+      <c r="AF14" s="25">
+        <v>3</v>
+      </c>
+      <c r="AG14" s="25">
+        <v>3</v>
+      </c>
+      <c r="AH14" s="25">
+        <v>3</v>
+      </c>
+      <c r="AI14" s="25">
+        <v>3</v>
+      </c>
+      <c r="AJ14" s="25">
+        <v>3</v>
+      </c>
+      <c r="AK14" s="25">
+        <v>3</v>
+      </c>
+      <c r="AL14" s="25">
+        <v>3</v>
+      </c>
+      <c r="AM14" s="25">
+        <v>3</v>
+      </c>
+      <c r="AN14" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="18">
+        <v>2</v>
+      </c>
+      <c r="B15" s="18">
+        <v>2</v>
+      </c>
+      <c r="C15" s="18">
+        <v>2</v>
+      </c>
+      <c r="D15" s="18">
+        <v>2</v>
+      </c>
+      <c r="E15" s="18">
+        <v>2</v>
+      </c>
+      <c r="F15" s="18">
+        <v>2</v>
+      </c>
+      <c r="G15" s="18">
+        <v>2</v>
+      </c>
+      <c r="H15" s="18">
+        <v>2</v>
+      </c>
+      <c r="I15" s="18">
+        <v>2</v>
+      </c>
+      <c r="J15" s="18">
+        <v>2</v>
+      </c>
+      <c r="K15" s="18">
+        <v>2</v>
+      </c>
+      <c r="L15" s="18">
+        <v>2</v>
+      </c>
+      <c r="M15" s="18">
+        <v>2</v>
+      </c>
+      <c r="N15" s="18">
+        <v>2</v>
+      </c>
+      <c r="O15" s="18">
+        <v>2</v>
+      </c>
+      <c r="P15" s="18">
+        <v>2</v>
+      </c>
+      <c r="Q15" s="18">
+        <v>2</v>
+      </c>
+      <c r="R15" s="18">
+        <v>2</v>
+      </c>
+      <c r="S15" s="18">
+        <v>2</v>
+      </c>
+      <c r="T15" s="18">
+        <v>2</v>
+      </c>
+      <c r="U15" s="25">
+        <v>3</v>
+      </c>
+      <c r="V15" s="25">
+        <v>3</v>
+      </c>
+      <c r="W15" s="25">
+        <v>3</v>
+      </c>
+      <c r="X15" s="25">
+        <v>3</v>
+      </c>
+      <c r="Y15" s="25">
+        <v>3</v>
+      </c>
+      <c r="Z15" s="25">
+        <v>3</v>
+      </c>
+      <c r="AA15" s="25">
+        <v>3</v>
+      </c>
+      <c r="AB15" s="25">
+        <v>3</v>
+      </c>
+      <c r="AC15" s="25">
+        <v>3</v>
+      </c>
+      <c r="AD15" s="25">
+        <v>3</v>
+      </c>
+      <c r="AE15" s="25">
+        <v>3</v>
+      </c>
+      <c r="AF15" s="25">
+        <v>3</v>
+      </c>
+      <c r="AG15" s="25">
+        <v>3</v>
+      </c>
+      <c r="AH15" s="25">
+        <v>3</v>
+      </c>
+      <c r="AI15" s="25">
+        <v>3</v>
+      </c>
+      <c r="AJ15" s="25">
+        <v>3</v>
+      </c>
+      <c r="AK15" s="25">
+        <v>3</v>
+      </c>
+      <c r="AL15" s="25">
+        <v>3</v>
+      </c>
+      <c r="AM15" s="25">
+        <v>3</v>
+      </c>
+      <c r="AN15" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="18">
+        <v>2</v>
+      </c>
+      <c r="B16" s="18">
+        <v>2</v>
+      </c>
+      <c r="C16" s="18">
+        <v>2</v>
+      </c>
+      <c r="D16" s="18">
+        <v>2</v>
+      </c>
+      <c r="E16" s="18">
+        <v>2</v>
+      </c>
+      <c r="F16" s="18">
+        <v>2</v>
+      </c>
+      <c r="G16" s="18">
+        <v>2</v>
+      </c>
+      <c r="H16" s="18">
+        <v>2</v>
+      </c>
+      <c r="I16" s="18">
+        <v>2</v>
+      </c>
+      <c r="J16" s="18">
+        <v>2</v>
+      </c>
+      <c r="K16" s="18">
+        <v>2</v>
+      </c>
+      <c r="L16" s="18">
+        <v>2</v>
+      </c>
+      <c r="M16" s="18">
+        <v>2</v>
+      </c>
+      <c r="N16" s="18">
+        <v>2</v>
+      </c>
+      <c r="O16" s="18">
+        <v>2</v>
+      </c>
+      <c r="P16" s="18">
+        <v>2</v>
+      </c>
+      <c r="Q16" s="18">
+        <v>2</v>
+      </c>
+      <c r="R16" s="18">
+        <v>2</v>
+      </c>
+      <c r="S16" s="18">
+        <v>2</v>
+      </c>
+      <c r="T16" s="18">
+        <v>2</v>
+      </c>
+      <c r="U16" s="25">
+        <v>3</v>
+      </c>
+      <c r="V16" s="25">
+        <v>3</v>
+      </c>
+      <c r="W16" s="25">
+        <v>3</v>
+      </c>
+      <c r="X16" s="25">
+        <v>3</v>
+      </c>
+      <c r="Y16" s="25">
+        <v>3</v>
+      </c>
+      <c r="Z16" s="25">
+        <v>3</v>
+      </c>
+      <c r="AA16" s="25">
+        <v>3</v>
+      </c>
+      <c r="AB16" s="25">
+        <v>3</v>
+      </c>
+      <c r="AC16" s="25">
+        <v>3</v>
+      </c>
+      <c r="AD16" s="25">
+        <v>3</v>
+      </c>
+      <c r="AE16" s="25">
+        <v>3</v>
+      </c>
+      <c r="AF16" s="25">
+        <v>3</v>
+      </c>
+      <c r="AG16" s="25">
+        <v>3</v>
+      </c>
+      <c r="AH16" s="25">
+        <v>3</v>
+      </c>
+      <c r="AI16" s="25">
+        <v>3</v>
+      </c>
+      <c r="AJ16" s="25">
+        <v>3</v>
+      </c>
+      <c r="AK16" s="25">
+        <v>3</v>
+      </c>
+      <c r="AL16" s="25">
+        <v>3</v>
+      </c>
+      <c r="AM16" s="25">
+        <v>3</v>
+      </c>
+      <c r="AN16" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="18">
+        <v>2</v>
+      </c>
+      <c r="B17" s="18">
+        <v>2</v>
+      </c>
+      <c r="C17" s="18">
+        <v>2</v>
+      </c>
+      <c r="D17" s="18">
+        <v>2</v>
+      </c>
+      <c r="E17" s="18">
+        <v>2</v>
+      </c>
+      <c r="F17" s="18">
+        <v>2</v>
+      </c>
+      <c r="G17" s="18">
+        <v>2</v>
+      </c>
+      <c r="H17" s="18">
+        <v>2</v>
+      </c>
+      <c r="I17" s="18">
+        <v>2</v>
+      </c>
+      <c r="J17" s="18">
+        <v>2</v>
+      </c>
+      <c r="K17" s="18">
+        <v>2</v>
+      </c>
+      <c r="L17" s="18">
+        <v>2</v>
+      </c>
+      <c r="M17" s="18">
+        <v>2</v>
+      </c>
+      <c r="N17" s="18">
+        <v>2</v>
+      </c>
+      <c r="O17" s="18">
+        <v>2</v>
+      </c>
+      <c r="P17" s="18">
+        <v>2</v>
+      </c>
+      <c r="Q17" s="18">
+        <v>2</v>
+      </c>
+      <c r="R17" s="18">
+        <v>2</v>
+      </c>
+      <c r="S17" s="18">
+        <v>2</v>
+      </c>
+      <c r="T17" s="18">
+        <v>2</v>
+      </c>
+      <c r="U17" s="25">
+        <v>3</v>
+      </c>
+      <c r="V17" s="25">
+        <v>3</v>
+      </c>
+      <c r="W17" s="25">
+        <v>3</v>
+      </c>
+      <c r="X17" s="25">
+        <v>3</v>
+      </c>
+      <c r="Y17" s="25">
+        <v>3</v>
+      </c>
+      <c r="Z17" s="25">
+        <v>3</v>
+      </c>
+      <c r="AA17" s="25">
+        <v>3</v>
+      </c>
+      <c r="AB17" s="25">
+        <v>3</v>
+      </c>
+      <c r="AC17" s="25">
+        <v>3</v>
+      </c>
+      <c r="AD17" s="25">
+        <v>3</v>
+      </c>
+      <c r="AE17" s="25">
+        <v>3</v>
+      </c>
+      <c r="AF17" s="25">
+        <v>3</v>
+      </c>
+      <c r="AG17" s="25">
+        <v>3</v>
+      </c>
+      <c r="AH17" s="25">
+        <v>3</v>
+      </c>
+      <c r="AI17" s="25">
+        <v>3</v>
+      </c>
+      <c r="AJ17" s="25">
+        <v>3</v>
+      </c>
+      <c r="AK17" s="25">
+        <v>3</v>
+      </c>
+      <c r="AL17" s="25">
+        <v>3</v>
+      </c>
+      <c r="AM17" s="25">
+        <v>3</v>
+      </c>
+      <c r="AN17" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="21">
+        <v>4</v>
+      </c>
+      <c r="B18" s="21">
+        <v>4</v>
+      </c>
+      <c r="C18" s="21">
+        <v>4</v>
+      </c>
+      <c r="D18" s="21">
+        <v>4</v>
+      </c>
+      <c r="E18" s="21">
+        <v>4</v>
+      </c>
+      <c r="F18" s="21">
+        <v>4</v>
+      </c>
+      <c r="G18" s="21">
+        <v>4</v>
+      </c>
+      <c r="H18" s="21">
+        <v>4</v>
+      </c>
+      <c r="I18" s="21">
+        <v>4</v>
+      </c>
+      <c r="J18" s="21">
+        <v>4</v>
+      </c>
+      <c r="K18" s="20">
+        <v>5</v>
+      </c>
+      <c r="L18" s="20">
+        <v>5</v>
+      </c>
+      <c r="M18" s="20">
+        <v>5</v>
+      </c>
+      <c r="N18" s="20">
+        <v>5</v>
+      </c>
+      <c r="O18" s="20">
+        <v>5</v>
+      </c>
+      <c r="P18" s="20">
+        <v>5</v>
+      </c>
+      <c r="Q18" s="20">
+        <v>5</v>
+      </c>
+      <c r="R18" s="20">
+        <v>5</v>
+      </c>
+      <c r="S18" s="20">
+        <v>5</v>
+      </c>
+      <c r="T18" s="20">
+        <v>5</v>
+      </c>
+      <c r="U18" s="24">
+        <v>6</v>
+      </c>
+      <c r="V18" s="24">
+        <v>6</v>
+      </c>
+      <c r="W18" s="24">
+        <v>6</v>
+      </c>
+      <c r="X18" s="24">
+        <v>6</v>
+      </c>
+      <c r="Y18" s="24">
+        <v>6</v>
+      </c>
+      <c r="Z18" s="24">
+        <v>6</v>
+      </c>
+      <c r="AA18" s="24">
+        <v>6</v>
+      </c>
+      <c r="AB18" s="24">
+        <v>6</v>
+      </c>
+      <c r="AC18" s="24">
+        <v>6</v>
+      </c>
+      <c r="AD18" s="24">
+        <v>6</v>
+      </c>
+      <c r="AE18" s="26">
+        <v>7</v>
+      </c>
+      <c r="AF18" s="26">
+        <v>7</v>
+      </c>
+      <c r="AG18" s="26">
+        <v>7</v>
+      </c>
+      <c r="AH18" s="26">
+        <v>7</v>
+      </c>
+      <c r="AI18" s="26">
+        <v>7</v>
+      </c>
+      <c r="AJ18" s="26">
+        <v>7</v>
+      </c>
+      <c r="AK18" s="26">
+        <v>7</v>
+      </c>
+      <c r="AL18" s="26">
+        <v>7</v>
+      </c>
+      <c r="AM18" s="26">
+        <v>7</v>
+      </c>
+      <c r="AN18" s="26">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="21">
+        <v>4</v>
+      </c>
+      <c r="B19" s="21">
+        <v>4</v>
+      </c>
+      <c r="C19" s="21">
+        <v>4</v>
+      </c>
+      <c r="D19" s="21">
+        <v>4</v>
+      </c>
+      <c r="E19" s="21">
+        <v>4</v>
+      </c>
+      <c r="F19" s="21">
+        <v>4</v>
+      </c>
+      <c r="G19" s="21">
+        <v>4</v>
+      </c>
+      <c r="H19" s="21">
+        <v>4</v>
+      </c>
+      <c r="I19" s="21">
+        <v>4</v>
+      </c>
+      <c r="J19" s="21">
+        <v>4</v>
+      </c>
+      <c r="K19" s="20">
+        <v>5</v>
+      </c>
+      <c r="L19" s="20">
+        <v>5</v>
+      </c>
+      <c r="M19" s="20">
+        <v>5</v>
+      </c>
+      <c r="N19" s="20">
+        <v>5</v>
+      </c>
+      <c r="O19" s="20">
+        <v>5</v>
+      </c>
+      <c r="P19" s="20">
+        <v>5</v>
+      </c>
+      <c r="Q19" s="20">
+        <v>5</v>
+      </c>
+      <c r="R19" s="20">
+        <v>5</v>
+      </c>
+      <c r="S19" s="20">
+        <v>5</v>
+      </c>
+      <c r="T19" s="20">
+        <v>5</v>
+      </c>
+      <c r="U19" s="24">
+        <v>6</v>
+      </c>
+      <c r="V19" s="24">
+        <v>6</v>
+      </c>
+      <c r="W19" s="24">
+        <v>6</v>
+      </c>
+      <c r="X19" s="24">
+        <v>6</v>
+      </c>
+      <c r="Y19" s="24">
+        <v>6</v>
+      </c>
+      <c r="Z19" s="24">
+        <v>6</v>
+      </c>
+      <c r="AA19" s="24">
+        <v>6</v>
+      </c>
+      <c r="AB19" s="24">
+        <v>6</v>
+      </c>
+      <c r="AC19" s="24">
+        <v>6</v>
+      </c>
+      <c r="AD19" s="24">
+        <v>6</v>
+      </c>
+      <c r="AE19" s="26">
+        <v>7</v>
+      </c>
+      <c r="AF19" s="26">
+        <v>7</v>
+      </c>
+      <c r="AG19" s="26">
+        <v>7</v>
+      </c>
+      <c r="AH19" s="26">
+        <v>7</v>
+      </c>
+      <c r="AI19" s="26">
+        <v>7</v>
+      </c>
+      <c r="AJ19" s="26">
+        <v>7</v>
+      </c>
+      <c r="AK19" s="26">
+        <v>7</v>
+      </c>
+      <c r="AL19" s="26">
+        <v>7</v>
+      </c>
+      <c r="AM19" s="26">
+        <v>7</v>
+      </c>
+      <c r="AN19" s="26">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="21">
+        <v>4</v>
+      </c>
+      <c r="B20" s="21">
+        <v>4</v>
+      </c>
+      <c r="C20" s="21">
+        <v>4</v>
+      </c>
+      <c r="D20" s="21">
+        <v>4</v>
+      </c>
+      <c r="E20" s="21">
+        <v>4</v>
+      </c>
+      <c r="F20" s="21">
+        <v>4</v>
+      </c>
+      <c r="G20" s="21">
+        <v>4</v>
+      </c>
+      <c r="H20" s="21">
+        <v>4</v>
+      </c>
+      <c r="I20" s="21">
+        <v>4</v>
+      </c>
+      <c r="J20" s="21">
+        <v>4</v>
+      </c>
+      <c r="K20" s="20">
+        <v>5</v>
+      </c>
+      <c r="L20" s="20">
+        <v>5</v>
+      </c>
+      <c r="M20" s="20">
+        <v>5</v>
+      </c>
+      <c r="N20" s="20">
+        <v>5</v>
+      </c>
+      <c r="O20" s="20">
+        <v>5</v>
+      </c>
+      <c r="P20" s="20">
+        <v>5</v>
+      </c>
+      <c r="Q20" s="20">
+        <v>5</v>
+      </c>
+      <c r="R20" s="20">
+        <v>5</v>
+      </c>
+      <c r="S20" s="20">
+        <v>5</v>
+      </c>
+      <c r="T20" s="20">
+        <v>5</v>
+      </c>
+      <c r="U20" s="24">
+        <v>6</v>
+      </c>
+      <c r="V20" s="24">
+        <v>6</v>
+      </c>
+      <c r="W20" s="24">
+        <v>6</v>
+      </c>
+      <c r="X20" s="24">
+        <v>6</v>
+      </c>
+      <c r="Y20" s="24">
+        <v>6</v>
+      </c>
+      <c r="Z20" s="24">
+        <v>6</v>
+      </c>
+      <c r="AA20" s="24">
+        <v>6</v>
+      </c>
+      <c r="AB20" s="24">
+        <v>6</v>
+      </c>
+      <c r="AC20" s="24">
+        <v>6</v>
+      </c>
+      <c r="AD20" s="24">
+        <v>6</v>
+      </c>
+      <c r="AE20" s="26">
+        <v>7</v>
+      </c>
+      <c r="AF20" s="26">
+        <v>7</v>
+      </c>
+      <c r="AG20" s="26">
+        <v>7</v>
+      </c>
+      <c r="AH20" s="26">
+        <v>7</v>
+      </c>
+      <c r="AI20" s="26">
+        <v>7</v>
+      </c>
+      <c r="AJ20" s="26">
+        <v>7</v>
+      </c>
+      <c r="AK20" s="26">
+        <v>7</v>
+      </c>
+      <c r="AL20" s="26">
+        <v>7</v>
+      </c>
+      <c r="AM20" s="26">
+        <v>7</v>
+      </c>
+      <c r="AN20" s="26">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="21">
+        <v>4</v>
+      </c>
+      <c r="B21" s="21">
+        <v>4</v>
+      </c>
+      <c r="C21" s="21">
+        <v>4</v>
+      </c>
+      <c r="D21" s="21">
+        <v>4</v>
+      </c>
+      <c r="E21" s="21">
+        <v>4</v>
+      </c>
+      <c r="F21" s="21">
+        <v>4</v>
+      </c>
+      <c r="G21" s="21">
+        <v>4</v>
+      </c>
+      <c r="H21" s="21">
+        <v>4</v>
+      </c>
+      <c r="I21" s="21">
+        <v>4</v>
+      </c>
+      <c r="J21" s="21">
+        <v>4</v>
+      </c>
+      <c r="K21" s="20">
+        <v>5</v>
+      </c>
+      <c r="L21" s="20">
+        <v>5</v>
+      </c>
+      <c r="M21" s="20">
+        <v>5</v>
+      </c>
+      <c r="N21" s="20">
+        <v>5</v>
+      </c>
+      <c r="O21" s="20">
+        <v>5</v>
+      </c>
+      <c r="P21" s="20">
+        <v>5</v>
+      </c>
+      <c r="Q21" s="20">
+        <v>5</v>
+      </c>
+      <c r="R21" s="20">
+        <v>5</v>
+      </c>
+      <c r="S21" s="20">
+        <v>5</v>
+      </c>
+      <c r="T21" s="20">
+        <v>5</v>
+      </c>
+      <c r="U21" s="24">
+        <v>6</v>
+      </c>
+      <c r="V21" s="24">
+        <v>6</v>
+      </c>
+      <c r="W21" s="24">
+        <v>6</v>
+      </c>
+      <c r="X21" s="24">
+        <v>6</v>
+      </c>
+      <c r="Y21" s="24">
+        <v>6</v>
+      </c>
+      <c r="Z21" s="24">
+        <v>6</v>
+      </c>
+      <c r="AA21" s="24">
+        <v>6</v>
+      </c>
+      <c r="AB21" s="24">
+        <v>6</v>
+      </c>
+      <c r="AC21" s="24">
+        <v>6</v>
+      </c>
+      <c r="AD21" s="24">
+        <v>6</v>
+      </c>
+      <c r="AE21" s="26">
+        <v>7</v>
+      </c>
+      <c r="AF21" s="26">
+        <v>7</v>
+      </c>
+      <c r="AG21" s="26">
+        <v>7</v>
+      </c>
+      <c r="AH21" s="26">
+        <v>7</v>
+      </c>
+      <c r="AI21" s="26">
+        <v>7</v>
+      </c>
+      <c r="AJ21" s="26">
+        <v>7</v>
+      </c>
+      <c r="AK21" s="26">
+        <v>7</v>
+      </c>
+      <c r="AL21" s="26">
+        <v>7</v>
+      </c>
+      <c r="AM21" s="26">
+        <v>7</v>
+      </c>
+      <c r="AN21" s="26">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="21">
+        <v>4</v>
+      </c>
+      <c r="B22" s="21">
+        <v>4</v>
+      </c>
+      <c r="C22" s="21">
+        <v>4</v>
+      </c>
+      <c r="D22" s="21">
+        <v>4</v>
+      </c>
+      <c r="E22" s="21">
+        <v>4</v>
+      </c>
+      <c r="F22" s="21">
+        <v>4</v>
+      </c>
+      <c r="G22" s="21">
+        <v>4</v>
+      </c>
+      <c r="H22" s="21">
+        <v>4</v>
+      </c>
+      <c r="I22" s="21">
+        <v>4</v>
+      </c>
+      <c r="J22" s="21">
+        <v>4</v>
+      </c>
+      <c r="K22" s="20">
+        <v>5</v>
+      </c>
+      <c r="L22" s="20">
+        <v>5</v>
+      </c>
+      <c r="M22" s="20">
+        <v>5</v>
+      </c>
+      <c r="N22" s="20">
+        <v>5</v>
+      </c>
+      <c r="O22" s="20">
+        <v>5</v>
+      </c>
+      <c r="P22" s="20">
+        <v>5</v>
+      </c>
+      <c r="Q22" s="20">
+        <v>5</v>
+      </c>
+      <c r="R22" s="20">
+        <v>5</v>
+      </c>
+      <c r="S22" s="20">
+        <v>5</v>
+      </c>
+      <c r="T22" s="20">
+        <v>5</v>
+      </c>
+      <c r="U22" s="24">
+        <v>6</v>
+      </c>
+      <c r="V22" s="24">
+        <v>6</v>
+      </c>
+      <c r="W22" s="24">
+        <v>6</v>
+      </c>
+      <c r="X22" s="24">
+        <v>6</v>
+      </c>
+      <c r="Y22" s="24">
+        <v>6</v>
+      </c>
+      <c r="Z22" s="24">
+        <v>6</v>
+      </c>
+      <c r="AA22" s="24">
+        <v>6</v>
+      </c>
+      <c r="AB22" s="24">
+        <v>6</v>
+      </c>
+      <c r="AC22" s="24">
+        <v>6</v>
+      </c>
+      <c r="AD22" s="24">
+        <v>6</v>
+      </c>
+      <c r="AE22" s="26">
+        <v>7</v>
+      </c>
+      <c r="AF22" s="26">
+        <v>7</v>
+      </c>
+      <c r="AG22" s="26">
+        <v>7</v>
+      </c>
+      <c r="AH22" s="26">
+        <v>7</v>
+      </c>
+      <c r="AI22" s="26">
+        <v>7</v>
+      </c>
+      <c r="AJ22" s="26">
+        <v>7</v>
+      </c>
+      <c r="AK22" s="26">
+        <v>7</v>
+      </c>
+      <c r="AL22" s="26">
+        <v>7</v>
+      </c>
+      <c r="AM22" s="26">
+        <v>7</v>
+      </c>
+      <c r="AN22" s="26">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="21">
+        <v>4</v>
+      </c>
+      <c r="B23" s="21">
+        <v>4</v>
+      </c>
+      <c r="C23" s="21">
+        <v>4</v>
+      </c>
+      <c r="D23" s="21">
+        <v>4</v>
+      </c>
+      <c r="E23" s="21">
+        <v>4</v>
+      </c>
+      <c r="F23" s="21">
+        <v>4</v>
+      </c>
+      <c r="G23" s="21">
+        <v>4</v>
+      </c>
+      <c r="H23" s="21">
+        <v>4</v>
+      </c>
+      <c r="I23" s="21">
+        <v>4</v>
+      </c>
+      <c r="J23" s="21">
+        <v>4</v>
+      </c>
+      <c r="K23" s="20">
+        <v>5</v>
+      </c>
+      <c r="L23" s="20">
+        <v>5</v>
+      </c>
+      <c r="M23" s="20">
+        <v>5</v>
+      </c>
+      <c r="N23" s="20">
+        <v>5</v>
+      </c>
+      <c r="O23" s="20">
+        <v>5</v>
+      </c>
+      <c r="P23" s="20">
+        <v>5</v>
+      </c>
+      <c r="Q23" s="20">
+        <v>5</v>
+      </c>
+      <c r="R23" s="20">
+        <v>5</v>
+      </c>
+      <c r="S23" s="20">
+        <v>5</v>
+      </c>
+      <c r="T23" s="20">
+        <v>5</v>
+      </c>
+      <c r="U23" s="24">
+        <v>6</v>
+      </c>
+      <c r="V23" s="24">
+        <v>6</v>
+      </c>
+      <c r="W23" s="24">
+        <v>6</v>
+      </c>
+      <c r="X23" s="24">
+        <v>6</v>
+      </c>
+      <c r="Y23" s="24">
+        <v>6</v>
+      </c>
+      <c r="Z23" s="24">
+        <v>6</v>
+      </c>
+      <c r="AA23" s="24">
+        <v>6</v>
+      </c>
+      <c r="AB23" s="24">
+        <v>6</v>
+      </c>
+      <c r="AC23" s="24">
+        <v>6</v>
+      </c>
+      <c r="AD23" s="24">
+        <v>6</v>
+      </c>
+      <c r="AE23" s="26">
+        <v>7</v>
+      </c>
+      <c r="AF23" s="26">
+        <v>7</v>
+      </c>
+      <c r="AG23" s="26">
+        <v>7</v>
+      </c>
+      <c r="AH23" s="26">
+        <v>7</v>
+      </c>
+      <c r="AI23" s="26">
+        <v>7</v>
+      </c>
+      <c r="AJ23" s="26">
+        <v>7</v>
+      </c>
+      <c r="AK23" s="26">
+        <v>7</v>
+      </c>
+      <c r="AL23" s="26">
+        <v>7</v>
+      </c>
+      <c r="AM23" s="26">
+        <v>7</v>
+      </c>
+      <c r="AN23" s="26">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="21">
+        <v>4</v>
+      </c>
+      <c r="B24" s="21">
+        <v>4</v>
+      </c>
+      <c r="C24" s="21">
+        <v>4</v>
+      </c>
+      <c r="D24" s="21">
+        <v>4</v>
+      </c>
+      <c r="E24" s="21">
+        <v>4</v>
+      </c>
+      <c r="F24" s="21">
+        <v>4</v>
+      </c>
+      <c r="G24" s="21">
+        <v>4</v>
+      </c>
+      <c r="H24" s="21">
+        <v>4</v>
+      </c>
+      <c r="I24" s="21">
+        <v>4</v>
+      </c>
+      <c r="J24" s="21">
+        <v>4</v>
+      </c>
+      <c r="K24" s="20">
+        <v>5</v>
+      </c>
+      <c r="L24" s="20">
+        <v>5</v>
+      </c>
+      <c r="M24" s="20">
+        <v>5</v>
+      </c>
+      <c r="N24" s="20">
+        <v>5</v>
+      </c>
+      <c r="O24" s="20">
+        <v>5</v>
+      </c>
+      <c r="P24" s="20">
+        <v>5</v>
+      </c>
+      <c r="Q24" s="20">
+        <v>5</v>
+      </c>
+      <c r="R24" s="20">
+        <v>5</v>
+      </c>
+      <c r="S24" s="20">
+        <v>5</v>
+      </c>
+      <c r="T24" s="20">
+        <v>5</v>
+      </c>
+      <c r="U24" s="24">
+        <v>6</v>
+      </c>
+      <c r="V24" s="24">
+        <v>6</v>
+      </c>
+      <c r="W24" s="24">
+        <v>6</v>
+      </c>
+      <c r="X24" s="24">
+        <v>6</v>
+      </c>
+      <c r="Y24" s="24">
+        <v>6</v>
+      </c>
+      <c r="Z24" s="24">
+        <v>6</v>
+      </c>
+      <c r="AA24" s="24">
+        <v>6</v>
+      </c>
+      <c r="AB24" s="24">
+        <v>6</v>
+      </c>
+      <c r="AC24" s="24">
+        <v>6</v>
+      </c>
+      <c r="AD24" s="24">
+        <v>6</v>
+      </c>
+      <c r="AE24" s="26">
+        <v>7</v>
+      </c>
+      <c r="AF24" s="26">
+        <v>7</v>
+      </c>
+      <c r="AG24" s="26">
+        <v>7</v>
+      </c>
+      <c r="AH24" s="26">
+        <v>7</v>
+      </c>
+      <c r="AI24" s="26">
+        <v>7</v>
+      </c>
+      <c r="AJ24" s="26">
+        <v>7</v>
+      </c>
+      <c r="AK24" s="26">
+        <v>7</v>
+      </c>
+      <c r="AL24" s="26">
+        <v>7</v>
+      </c>
+      <c r="AM24" s="26">
+        <v>7</v>
+      </c>
+      <c r="AN24" s="26">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="21">
+        <v>4</v>
+      </c>
+      <c r="B25" s="21">
+        <v>4</v>
+      </c>
+      <c r="C25" s="21">
+        <v>4</v>
+      </c>
+      <c r="D25" s="21">
+        <v>4</v>
+      </c>
+      <c r="E25" s="21">
+        <v>4</v>
+      </c>
+      <c r="F25" s="21">
+        <v>4</v>
+      </c>
+      <c r="G25" s="21">
+        <v>4</v>
+      </c>
+      <c r="H25" s="21">
+        <v>4</v>
+      </c>
+      <c r="I25" s="21">
+        <v>4</v>
+      </c>
+      <c r="J25" s="21">
+        <v>4</v>
+      </c>
+      <c r="K25" s="20">
+        <v>5</v>
+      </c>
+      <c r="L25" s="20">
+        <v>5</v>
+      </c>
+      <c r="M25" s="20">
+        <v>5</v>
+      </c>
+      <c r="N25" s="20">
+        <v>5</v>
+      </c>
+      <c r="O25" s="20">
+        <v>5</v>
+      </c>
+      <c r="P25" s="20">
+        <v>5</v>
+      </c>
+      <c r="Q25" s="20">
+        <v>5</v>
+      </c>
+      <c r="R25" s="20">
+        <v>5</v>
+      </c>
+      <c r="S25" s="20">
+        <v>5</v>
+      </c>
+      <c r="T25" s="20">
+        <v>5</v>
+      </c>
+      <c r="U25" s="24">
+        <v>6</v>
+      </c>
+      <c r="V25" s="24">
+        <v>6</v>
+      </c>
+      <c r="W25" s="24">
+        <v>6</v>
+      </c>
+      <c r="X25" s="24">
+        <v>6</v>
+      </c>
+      <c r="Y25" s="24">
+        <v>6</v>
+      </c>
+      <c r="Z25" s="24">
+        <v>6</v>
+      </c>
+      <c r="AA25" s="24">
+        <v>6</v>
+      </c>
+      <c r="AB25" s="24">
+        <v>6</v>
+      </c>
+      <c r="AC25" s="24">
+        <v>6</v>
+      </c>
+      <c r="AD25" s="24">
+        <v>6</v>
+      </c>
+      <c r="AE25" s="26">
+        <v>7</v>
+      </c>
+      <c r="AF25" s="26">
+        <v>7</v>
+      </c>
+      <c r="AG25" s="26">
+        <v>7</v>
+      </c>
+      <c r="AH25" s="26">
+        <v>7</v>
+      </c>
+      <c r="AI25" s="26">
+        <v>7</v>
+      </c>
+      <c r="AJ25" s="26">
+        <v>7</v>
+      </c>
+      <c r="AK25" s="26">
+        <v>7</v>
+      </c>
+      <c r="AL25" s="26">
+        <v>7</v>
+      </c>
+      <c r="AM25" s="26">
+        <v>7</v>
+      </c>
+      <c r="AN25" s="26">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="21">
+        <v>4</v>
+      </c>
+      <c r="B26" s="21">
+        <v>4</v>
+      </c>
+      <c r="C26" s="21">
+        <v>4</v>
+      </c>
+      <c r="D26" s="21">
+        <v>4</v>
+      </c>
+      <c r="E26" s="21">
+        <v>4</v>
+      </c>
+      <c r="F26" s="21">
+        <v>4</v>
+      </c>
+      <c r="G26" s="21">
+        <v>4</v>
+      </c>
+      <c r="H26" s="21">
+        <v>4</v>
+      </c>
+      <c r="I26" s="21">
+        <v>4</v>
+      </c>
+      <c r="J26" s="21">
+        <v>4</v>
+      </c>
+      <c r="K26" s="20">
+        <v>5</v>
+      </c>
+      <c r="L26" s="20">
+        <v>5</v>
+      </c>
+      <c r="M26" s="20">
+        <v>5</v>
+      </c>
+      <c r="N26" s="20">
+        <v>5</v>
+      </c>
+      <c r="O26" s="20">
+        <v>5</v>
+      </c>
+      <c r="P26" s="20">
+        <v>5</v>
+      </c>
+      <c r="Q26" s="20">
+        <v>5</v>
+      </c>
+      <c r="R26" s="20">
+        <v>5</v>
+      </c>
+      <c r="S26" s="20">
+        <v>5</v>
+      </c>
+      <c r="T26" s="20">
+        <v>5</v>
+      </c>
+      <c r="U26" s="24">
+        <v>6</v>
+      </c>
+      <c r="V26" s="24">
+        <v>6</v>
+      </c>
+      <c r="W26" s="24">
+        <v>6</v>
+      </c>
+      <c r="X26" s="24">
+        <v>6</v>
+      </c>
+      <c r="Y26" s="24">
+        <v>6</v>
+      </c>
+      <c r="Z26" s="24">
+        <v>6</v>
+      </c>
+      <c r="AA26" s="24">
+        <v>6</v>
+      </c>
+      <c r="AB26" s="24">
+        <v>6</v>
+      </c>
+      <c r="AC26" s="24">
+        <v>6</v>
+      </c>
+      <c r="AD26" s="24">
+        <v>6</v>
+      </c>
+      <c r="AE26" s="26">
+        <v>7</v>
+      </c>
+      <c r="AF26" s="26">
+        <v>7</v>
+      </c>
+      <c r="AG26" s="26">
+        <v>7</v>
+      </c>
+      <c r="AH26" s="26">
+        <v>7</v>
+      </c>
+      <c r="AI26" s="26">
+        <v>7</v>
+      </c>
+      <c r="AJ26" s="26">
+        <v>7</v>
+      </c>
+      <c r="AK26" s="26">
+        <v>7</v>
+      </c>
+      <c r="AL26" s="26">
+        <v>7</v>
+      </c>
+      <c r="AM26" s="26">
+        <v>7</v>
+      </c>
+      <c r="AN26" s="26">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="21">
+        <v>4</v>
+      </c>
+      <c r="B27" s="21">
+        <v>4</v>
+      </c>
+      <c r="C27" s="21">
+        <v>4</v>
+      </c>
+      <c r="D27" s="21">
+        <v>4</v>
+      </c>
+      <c r="E27" s="21">
+        <v>4</v>
+      </c>
+      <c r="F27" s="21">
+        <v>4</v>
+      </c>
+      <c r="G27" s="21">
+        <v>4</v>
+      </c>
+      <c r="H27" s="21">
+        <v>4</v>
+      </c>
+      <c r="I27" s="21">
+        <v>4</v>
+      </c>
+      <c r="J27" s="21">
+        <v>4</v>
+      </c>
+      <c r="K27" s="20">
+        <v>5</v>
+      </c>
+      <c r="L27" s="20">
+        <v>5</v>
+      </c>
+      <c r="M27" s="20">
+        <v>5</v>
+      </c>
+      <c r="N27" s="20">
+        <v>5</v>
+      </c>
+      <c r="O27" s="20">
+        <v>5</v>
+      </c>
+      <c r="P27" s="20">
+        <v>5</v>
+      </c>
+      <c r="Q27" s="20">
+        <v>5</v>
+      </c>
+      <c r="R27" s="20">
+        <v>5</v>
+      </c>
+      <c r="S27" s="20">
+        <v>5</v>
+      </c>
+      <c r="T27" s="20">
+        <v>5</v>
+      </c>
+      <c r="U27" s="24">
+        <v>6</v>
+      </c>
+      <c r="V27" s="24">
+        <v>6</v>
+      </c>
+      <c r="W27" s="24">
+        <v>6</v>
+      </c>
+      <c r="X27" s="24">
+        <v>6</v>
+      </c>
+      <c r="Y27" s="24">
+        <v>6</v>
+      </c>
+      <c r="Z27" s="24">
+        <v>6</v>
+      </c>
+      <c r="AA27" s="24">
+        <v>6</v>
+      </c>
+      <c r="AB27" s="24">
+        <v>6</v>
+      </c>
+      <c r="AC27" s="24">
+        <v>6</v>
+      </c>
+      <c r="AD27" s="24">
+        <v>6</v>
+      </c>
+      <c r="AE27" s="26">
+        <v>7</v>
+      </c>
+      <c r="AF27" s="26">
+        <v>7</v>
+      </c>
+      <c r="AG27" s="26">
+        <v>7</v>
+      </c>
+      <c r="AH27" s="26">
+        <v>7</v>
+      </c>
+      <c r="AI27" s="26">
+        <v>7</v>
+      </c>
+      <c r="AJ27" s="26">
+        <v>7</v>
+      </c>
+      <c r="AK27" s="26">
+        <v>7</v>
+      </c>
+      <c r="AL27" s="26">
+        <v>7</v>
+      </c>
+      <c r="AM27" s="26">
+        <v>7</v>
+      </c>
+      <c r="AN27" s="26">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="21">
+        <v>4</v>
+      </c>
+      <c r="B28" s="21">
+        <v>4</v>
+      </c>
+      <c r="C28" s="21">
+        <v>4</v>
+      </c>
+      <c r="D28" s="21">
+        <v>4</v>
+      </c>
+      <c r="E28" s="21">
+        <v>4</v>
+      </c>
+      <c r="F28" s="21">
+        <v>4</v>
+      </c>
+      <c r="G28" s="21">
+        <v>4</v>
+      </c>
+      <c r="H28" s="21">
+        <v>4</v>
+      </c>
+      <c r="I28" s="21">
+        <v>4</v>
+      </c>
+      <c r="J28" s="21">
+        <v>4</v>
+      </c>
+      <c r="K28" s="20">
+        <v>5</v>
+      </c>
+      <c r="L28" s="20">
+        <v>5</v>
+      </c>
+      <c r="M28" s="20">
+        <v>5</v>
+      </c>
+      <c r="N28" s="20">
+        <v>5</v>
+      </c>
+      <c r="O28" s="20">
+        <v>5</v>
+      </c>
+      <c r="P28" s="20">
+        <v>5</v>
+      </c>
+      <c r="Q28" s="20">
+        <v>5</v>
+      </c>
+      <c r="R28" s="20">
+        <v>5</v>
+      </c>
+      <c r="S28" s="20">
+        <v>5</v>
+      </c>
+      <c r="T28" s="20">
+        <v>5</v>
+      </c>
+      <c r="U28" s="24">
+        <v>6</v>
+      </c>
+      <c r="V28" s="24">
+        <v>6</v>
+      </c>
+      <c r="W28" s="24">
+        <v>6</v>
+      </c>
+      <c r="X28" s="24">
+        <v>6</v>
+      </c>
+      <c r="Y28" s="24">
+        <v>6</v>
+      </c>
+      <c r="Z28" s="24">
+        <v>6</v>
+      </c>
+      <c r="AA28" s="24">
+        <v>6</v>
+      </c>
+      <c r="AB28" s="24">
+        <v>6</v>
+      </c>
+      <c r="AC28" s="24">
+        <v>6</v>
+      </c>
+      <c r="AD28" s="24">
+        <v>6</v>
+      </c>
+      <c r="AE28" s="26">
+        <v>7</v>
+      </c>
+      <c r="AF28" s="26">
+        <v>7</v>
+      </c>
+      <c r="AG28" s="26">
+        <v>7</v>
+      </c>
+      <c r="AH28" s="26">
+        <v>7</v>
+      </c>
+      <c r="AI28" s="26">
+        <v>7</v>
+      </c>
+      <c r="AJ28" s="26">
+        <v>7</v>
+      </c>
+      <c r="AK28" s="26">
+        <v>7</v>
+      </c>
+      <c r="AL28" s="26">
+        <v>7</v>
+      </c>
+      <c r="AM28" s="26">
+        <v>7</v>
+      </c>
+      <c r="AN28" s="26">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add housing affordability page
</commit_message>
<xml_diff>
--- a/layouts.xlsx
+++ b/layouts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/046b73b793af0aea/PAMGMT/projects/tamarac/economic-market-commentary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="342" documentId="8_{16FB9176-5700-CA44-8DDA-ADDCE61D2EC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CA9BDEAF-3996-FB4E-8771-876C4E8F7577}"/>
+  <xr:revisionPtr revIDLastSave="346" documentId="8_{16FB9176-5700-CA44-8DDA-ADDCE61D2EC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D8EB576D-4DBD-C44A-8070-C794031B2ACE}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="1600" windowWidth="28040" windowHeight="18100" activeTab="11" xr2:uid="{7344E464-CEB7-A74D-A529-F1BDE3AF96EC}"/>
+    <workbookView xWindow="3900" yWindow="1600" windowWidth="28040" windowHeight="18100" activeTab="12" xr2:uid="{7344E464-CEB7-A74D-A529-F1BDE3AF96EC}"/>
   </bookViews>
   <sheets>
     <sheet name="lay-1" sheetId="2" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <sheet name="lay-10" sheetId="12" r:id="rId10"/>
     <sheet name="lay-11" sheetId="13" r:id="rId11"/>
     <sheet name="lay-12" sheetId="14" r:id="rId12"/>
+    <sheet name="lay-13" sheetId="15" r:id="rId13"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="41">
   <si>
     <t>a</t>
   </si>
@@ -10889,7 +10890,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88058F12-8899-DA4C-9FD4-20DF326DCD54}">
   <dimension ref="A1:AN28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AR25" sqref="AR25"/>
     </sheetView>
   </sheetViews>
@@ -14312,6 +14313,3440 @@
       </c>
       <c r="AN28" s="26">
         <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{544EC16B-A29B-4A43-BE11-AE7567F72735}">
+  <dimension ref="A1:AN28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T31" sqref="T31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="40" width="3.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>40</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1">
+        <v>1</v>
+      </c>
+      <c r="I2" s="1">
+        <v>1</v>
+      </c>
+      <c r="J2" s="1">
+        <v>1</v>
+      </c>
+      <c r="K2" s="1">
+        <v>1</v>
+      </c>
+      <c r="L2" s="1">
+        <v>1</v>
+      </c>
+      <c r="M2" s="1">
+        <v>1</v>
+      </c>
+      <c r="N2" s="1">
+        <v>1</v>
+      </c>
+      <c r="O2" s="1">
+        <v>1</v>
+      </c>
+      <c r="P2" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>1</v>
+      </c>
+      <c r="R2" s="1">
+        <v>1</v>
+      </c>
+      <c r="S2" s="1">
+        <v>1</v>
+      </c>
+      <c r="T2" s="1">
+        <v>1</v>
+      </c>
+      <c r="U2" s="1">
+        <v>1</v>
+      </c>
+      <c r="V2" s="1">
+        <v>1</v>
+      </c>
+      <c r="W2" s="1">
+        <v>1</v>
+      </c>
+      <c r="X2" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AM2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1">
+        <v>1</v>
+      </c>
+      <c r="J3" s="1">
+        <v>1</v>
+      </c>
+      <c r="K3" s="1">
+        <v>1</v>
+      </c>
+      <c r="L3" s="1">
+        <v>1</v>
+      </c>
+      <c r="M3" s="1">
+        <v>1</v>
+      </c>
+      <c r="N3" s="1">
+        <v>1</v>
+      </c>
+      <c r="O3" s="1">
+        <v>1</v>
+      </c>
+      <c r="P3" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>1</v>
+      </c>
+      <c r="R3" s="1">
+        <v>1</v>
+      </c>
+      <c r="S3" s="1">
+        <v>1</v>
+      </c>
+      <c r="T3" s="1">
+        <v>1</v>
+      </c>
+      <c r="U3" s="1">
+        <v>1</v>
+      </c>
+      <c r="V3" s="1">
+        <v>1</v>
+      </c>
+      <c r="W3" s="1">
+        <v>1</v>
+      </c>
+      <c r="X3" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y3" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AM3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1</v>
+      </c>
+      <c r="I4" s="1">
+        <v>1</v>
+      </c>
+      <c r="J4" s="1">
+        <v>1</v>
+      </c>
+      <c r="K4" s="1">
+        <v>1</v>
+      </c>
+      <c r="L4" s="1">
+        <v>1</v>
+      </c>
+      <c r="M4" s="1">
+        <v>1</v>
+      </c>
+      <c r="N4" s="1">
+        <v>1</v>
+      </c>
+      <c r="O4" s="1">
+        <v>1</v>
+      </c>
+      <c r="P4" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>1</v>
+      </c>
+      <c r="R4" s="1">
+        <v>1</v>
+      </c>
+      <c r="S4" s="1">
+        <v>1</v>
+      </c>
+      <c r="T4" s="1">
+        <v>1</v>
+      </c>
+      <c r="U4" s="1">
+        <v>1</v>
+      </c>
+      <c r="V4" s="1">
+        <v>1</v>
+      </c>
+      <c r="W4" s="1">
+        <v>1</v>
+      </c>
+      <c r="X4" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y4" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AM4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="18">
+        <v>2</v>
+      </c>
+      <c r="B5" s="18">
+        <v>2</v>
+      </c>
+      <c r="C5" s="18">
+        <v>2</v>
+      </c>
+      <c r="D5" s="18">
+        <v>2</v>
+      </c>
+      <c r="E5" s="18">
+        <v>2</v>
+      </c>
+      <c r="F5" s="18">
+        <v>2</v>
+      </c>
+      <c r="G5" s="18">
+        <v>2</v>
+      </c>
+      <c r="H5" s="18">
+        <v>2</v>
+      </c>
+      <c r="I5" s="18">
+        <v>2</v>
+      </c>
+      <c r="J5" s="18">
+        <v>2</v>
+      </c>
+      <c r="K5" s="18">
+        <v>2</v>
+      </c>
+      <c r="L5" s="18">
+        <v>2</v>
+      </c>
+      <c r="M5" s="18">
+        <v>2</v>
+      </c>
+      <c r="N5" s="18">
+        <v>2</v>
+      </c>
+      <c r="O5" s="18">
+        <v>2</v>
+      </c>
+      <c r="P5" s="18">
+        <v>2</v>
+      </c>
+      <c r="Q5" s="18">
+        <v>2</v>
+      </c>
+      <c r="R5" s="18">
+        <v>2</v>
+      </c>
+      <c r="S5" s="18">
+        <v>2</v>
+      </c>
+      <c r="T5" s="18">
+        <v>2</v>
+      </c>
+      <c r="U5" s="25">
+        <v>3</v>
+      </c>
+      <c r="V5" s="25">
+        <v>3</v>
+      </c>
+      <c r="W5" s="25">
+        <v>3</v>
+      </c>
+      <c r="X5" s="25">
+        <v>3</v>
+      </c>
+      <c r="Y5" s="25">
+        <v>3</v>
+      </c>
+      <c r="Z5" s="25">
+        <v>3</v>
+      </c>
+      <c r="AA5" s="25">
+        <v>3</v>
+      </c>
+      <c r="AB5" s="25">
+        <v>3</v>
+      </c>
+      <c r="AC5" s="25">
+        <v>3</v>
+      </c>
+      <c r="AD5" s="25">
+        <v>3</v>
+      </c>
+      <c r="AE5" s="25">
+        <v>3</v>
+      </c>
+      <c r="AF5" s="25">
+        <v>3</v>
+      </c>
+      <c r="AG5" s="25">
+        <v>3</v>
+      </c>
+      <c r="AH5" s="25">
+        <v>3</v>
+      </c>
+      <c r="AI5" s="25">
+        <v>3</v>
+      </c>
+      <c r="AJ5" s="25">
+        <v>3</v>
+      </c>
+      <c r="AK5" s="25">
+        <v>3</v>
+      </c>
+      <c r="AL5" s="25">
+        <v>3</v>
+      </c>
+      <c r="AM5" s="25">
+        <v>3</v>
+      </c>
+      <c r="AN5" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="18">
+        <v>2</v>
+      </c>
+      <c r="B6" s="18">
+        <v>2</v>
+      </c>
+      <c r="C6" s="18">
+        <v>2</v>
+      </c>
+      <c r="D6" s="18">
+        <v>2</v>
+      </c>
+      <c r="E6" s="18">
+        <v>2</v>
+      </c>
+      <c r="F6" s="18">
+        <v>2</v>
+      </c>
+      <c r="G6" s="18">
+        <v>2</v>
+      </c>
+      <c r="H6" s="18">
+        <v>2</v>
+      </c>
+      <c r="I6" s="18">
+        <v>2</v>
+      </c>
+      <c r="J6" s="18">
+        <v>2</v>
+      </c>
+      <c r="K6" s="18">
+        <v>2</v>
+      </c>
+      <c r="L6" s="18">
+        <v>2</v>
+      </c>
+      <c r="M6" s="18">
+        <v>2</v>
+      </c>
+      <c r="N6" s="18">
+        <v>2</v>
+      </c>
+      <c r="O6" s="18">
+        <v>2</v>
+      </c>
+      <c r="P6" s="18">
+        <v>2</v>
+      </c>
+      <c r="Q6" s="18">
+        <v>2</v>
+      </c>
+      <c r="R6" s="18">
+        <v>2</v>
+      </c>
+      <c r="S6" s="18">
+        <v>2</v>
+      </c>
+      <c r="T6" s="18">
+        <v>2</v>
+      </c>
+      <c r="U6" s="25">
+        <v>3</v>
+      </c>
+      <c r="V6" s="25">
+        <v>3</v>
+      </c>
+      <c r="W6" s="25">
+        <v>3</v>
+      </c>
+      <c r="X6" s="25">
+        <v>3</v>
+      </c>
+      <c r="Y6" s="25">
+        <v>3</v>
+      </c>
+      <c r="Z6" s="25">
+        <v>3</v>
+      </c>
+      <c r="AA6" s="25">
+        <v>3</v>
+      </c>
+      <c r="AB6" s="25">
+        <v>3</v>
+      </c>
+      <c r="AC6" s="25">
+        <v>3</v>
+      </c>
+      <c r="AD6" s="25">
+        <v>3</v>
+      </c>
+      <c r="AE6" s="25">
+        <v>3</v>
+      </c>
+      <c r="AF6" s="25">
+        <v>3</v>
+      </c>
+      <c r="AG6" s="25">
+        <v>3</v>
+      </c>
+      <c r="AH6" s="25">
+        <v>3</v>
+      </c>
+      <c r="AI6" s="25">
+        <v>3</v>
+      </c>
+      <c r="AJ6" s="25">
+        <v>3</v>
+      </c>
+      <c r="AK6" s="25">
+        <v>3</v>
+      </c>
+      <c r="AL6" s="25">
+        <v>3</v>
+      </c>
+      <c r="AM6" s="25">
+        <v>3</v>
+      </c>
+      <c r="AN6" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="18">
+        <v>2</v>
+      </c>
+      <c r="B7" s="18">
+        <v>2</v>
+      </c>
+      <c r="C7" s="18">
+        <v>2</v>
+      </c>
+      <c r="D7" s="18">
+        <v>2</v>
+      </c>
+      <c r="E7" s="18">
+        <v>2</v>
+      </c>
+      <c r="F7" s="18">
+        <v>2</v>
+      </c>
+      <c r="G7" s="18">
+        <v>2</v>
+      </c>
+      <c r="H7" s="18">
+        <v>2</v>
+      </c>
+      <c r="I7" s="18">
+        <v>2</v>
+      </c>
+      <c r="J7" s="18">
+        <v>2</v>
+      </c>
+      <c r="K7" s="18">
+        <v>2</v>
+      </c>
+      <c r="L7" s="18">
+        <v>2</v>
+      </c>
+      <c r="M7" s="18">
+        <v>2</v>
+      </c>
+      <c r="N7" s="18">
+        <v>2</v>
+      </c>
+      <c r="O7" s="18">
+        <v>2</v>
+      </c>
+      <c r="P7" s="18">
+        <v>2</v>
+      </c>
+      <c r="Q7" s="18">
+        <v>2</v>
+      </c>
+      <c r="R7" s="18">
+        <v>2</v>
+      </c>
+      <c r="S7" s="18">
+        <v>2</v>
+      </c>
+      <c r="T7" s="18">
+        <v>2</v>
+      </c>
+      <c r="U7" s="25">
+        <v>3</v>
+      </c>
+      <c r="V7" s="25">
+        <v>3</v>
+      </c>
+      <c r="W7" s="25">
+        <v>3</v>
+      </c>
+      <c r="X7" s="25">
+        <v>3</v>
+      </c>
+      <c r="Y7" s="25">
+        <v>3</v>
+      </c>
+      <c r="Z7" s="25">
+        <v>3</v>
+      </c>
+      <c r="AA7" s="25">
+        <v>3</v>
+      </c>
+      <c r="AB7" s="25">
+        <v>3</v>
+      </c>
+      <c r="AC7" s="25">
+        <v>3</v>
+      </c>
+      <c r="AD7" s="25">
+        <v>3</v>
+      </c>
+      <c r="AE7" s="25">
+        <v>3</v>
+      </c>
+      <c r="AF7" s="25">
+        <v>3</v>
+      </c>
+      <c r="AG7" s="25">
+        <v>3</v>
+      </c>
+      <c r="AH7" s="25">
+        <v>3</v>
+      </c>
+      <c r="AI7" s="25">
+        <v>3</v>
+      </c>
+      <c r="AJ7" s="25">
+        <v>3</v>
+      </c>
+      <c r="AK7" s="25">
+        <v>3</v>
+      </c>
+      <c r="AL7" s="25">
+        <v>3</v>
+      </c>
+      <c r="AM7" s="25">
+        <v>3</v>
+      </c>
+      <c r="AN7" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="18">
+        <v>2</v>
+      </c>
+      <c r="B8" s="18">
+        <v>2</v>
+      </c>
+      <c r="C8" s="18">
+        <v>2</v>
+      </c>
+      <c r="D8" s="18">
+        <v>2</v>
+      </c>
+      <c r="E8" s="18">
+        <v>2</v>
+      </c>
+      <c r="F8" s="18">
+        <v>2</v>
+      </c>
+      <c r="G8" s="18">
+        <v>2</v>
+      </c>
+      <c r="H8" s="18">
+        <v>2</v>
+      </c>
+      <c r="I8" s="18">
+        <v>2</v>
+      </c>
+      <c r="J8" s="18">
+        <v>2</v>
+      </c>
+      <c r="K8" s="18">
+        <v>2</v>
+      </c>
+      <c r="L8" s="18">
+        <v>2</v>
+      </c>
+      <c r="M8" s="18">
+        <v>2</v>
+      </c>
+      <c r="N8" s="18">
+        <v>2</v>
+      </c>
+      <c r="O8" s="18">
+        <v>2</v>
+      </c>
+      <c r="P8" s="18">
+        <v>2</v>
+      </c>
+      <c r="Q8" s="18">
+        <v>2</v>
+      </c>
+      <c r="R8" s="18">
+        <v>2</v>
+      </c>
+      <c r="S8" s="18">
+        <v>2</v>
+      </c>
+      <c r="T8" s="18">
+        <v>2</v>
+      </c>
+      <c r="U8" s="25">
+        <v>3</v>
+      </c>
+      <c r="V8" s="25">
+        <v>3</v>
+      </c>
+      <c r="W8" s="25">
+        <v>3</v>
+      </c>
+      <c r="X8" s="25">
+        <v>3</v>
+      </c>
+      <c r="Y8" s="25">
+        <v>3</v>
+      </c>
+      <c r="Z8" s="25">
+        <v>3</v>
+      </c>
+      <c r="AA8" s="25">
+        <v>3</v>
+      </c>
+      <c r="AB8" s="25">
+        <v>3</v>
+      </c>
+      <c r="AC8" s="25">
+        <v>3</v>
+      </c>
+      <c r="AD8" s="25">
+        <v>3</v>
+      </c>
+      <c r="AE8" s="25">
+        <v>3</v>
+      </c>
+      <c r="AF8" s="25">
+        <v>3</v>
+      </c>
+      <c r="AG8" s="25">
+        <v>3</v>
+      </c>
+      <c r="AH8" s="25">
+        <v>3</v>
+      </c>
+      <c r="AI8" s="25">
+        <v>3</v>
+      </c>
+      <c r="AJ8" s="25">
+        <v>3</v>
+      </c>
+      <c r="AK8" s="25">
+        <v>3</v>
+      </c>
+      <c r="AL8" s="25">
+        <v>3</v>
+      </c>
+      <c r="AM8" s="25">
+        <v>3</v>
+      </c>
+      <c r="AN8" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="18">
+        <v>2</v>
+      </c>
+      <c r="B9" s="18">
+        <v>2</v>
+      </c>
+      <c r="C9" s="18">
+        <v>2</v>
+      </c>
+      <c r="D9" s="18">
+        <v>2</v>
+      </c>
+      <c r="E9" s="18">
+        <v>2</v>
+      </c>
+      <c r="F9" s="18">
+        <v>2</v>
+      </c>
+      <c r="G9" s="18">
+        <v>2</v>
+      </c>
+      <c r="H9" s="18">
+        <v>2</v>
+      </c>
+      <c r="I9" s="18">
+        <v>2</v>
+      </c>
+      <c r="J9" s="18">
+        <v>2</v>
+      </c>
+      <c r="K9" s="18">
+        <v>2</v>
+      </c>
+      <c r="L9" s="18">
+        <v>2</v>
+      </c>
+      <c r="M9" s="18">
+        <v>2</v>
+      </c>
+      <c r="N9" s="18">
+        <v>2</v>
+      </c>
+      <c r="O9" s="18">
+        <v>2</v>
+      </c>
+      <c r="P9" s="18">
+        <v>2</v>
+      </c>
+      <c r="Q9" s="18">
+        <v>2</v>
+      </c>
+      <c r="R9" s="18">
+        <v>2</v>
+      </c>
+      <c r="S9" s="18">
+        <v>2</v>
+      </c>
+      <c r="T9" s="18">
+        <v>2</v>
+      </c>
+      <c r="U9" s="25">
+        <v>3</v>
+      </c>
+      <c r="V9" s="25">
+        <v>3</v>
+      </c>
+      <c r="W9" s="25">
+        <v>3</v>
+      </c>
+      <c r="X9" s="25">
+        <v>3</v>
+      </c>
+      <c r="Y9" s="25">
+        <v>3</v>
+      </c>
+      <c r="Z9" s="25">
+        <v>3</v>
+      </c>
+      <c r="AA9" s="25">
+        <v>3</v>
+      </c>
+      <c r="AB9" s="25">
+        <v>3</v>
+      </c>
+      <c r="AC9" s="25">
+        <v>3</v>
+      </c>
+      <c r="AD9" s="25">
+        <v>3</v>
+      </c>
+      <c r="AE9" s="25">
+        <v>3</v>
+      </c>
+      <c r="AF9" s="25">
+        <v>3</v>
+      </c>
+      <c r="AG9" s="25">
+        <v>3</v>
+      </c>
+      <c r="AH9" s="25">
+        <v>3</v>
+      </c>
+      <c r="AI9" s="25">
+        <v>3</v>
+      </c>
+      <c r="AJ9" s="25">
+        <v>3</v>
+      </c>
+      <c r="AK9" s="25">
+        <v>3</v>
+      </c>
+      <c r="AL9" s="25">
+        <v>3</v>
+      </c>
+      <c r="AM9" s="25">
+        <v>3</v>
+      </c>
+      <c r="AN9" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="18">
+        <v>2</v>
+      </c>
+      <c r="B10" s="18">
+        <v>2</v>
+      </c>
+      <c r="C10" s="18">
+        <v>2</v>
+      </c>
+      <c r="D10" s="18">
+        <v>2</v>
+      </c>
+      <c r="E10" s="18">
+        <v>2</v>
+      </c>
+      <c r="F10" s="18">
+        <v>2</v>
+      </c>
+      <c r="G10" s="18">
+        <v>2</v>
+      </c>
+      <c r="H10" s="18">
+        <v>2</v>
+      </c>
+      <c r="I10" s="18">
+        <v>2</v>
+      </c>
+      <c r="J10" s="18">
+        <v>2</v>
+      </c>
+      <c r="K10" s="18">
+        <v>2</v>
+      </c>
+      <c r="L10" s="18">
+        <v>2</v>
+      </c>
+      <c r="M10" s="18">
+        <v>2</v>
+      </c>
+      <c r="N10" s="18">
+        <v>2</v>
+      </c>
+      <c r="O10" s="18">
+        <v>2</v>
+      </c>
+      <c r="P10" s="18">
+        <v>2</v>
+      </c>
+      <c r="Q10" s="18">
+        <v>2</v>
+      </c>
+      <c r="R10" s="18">
+        <v>2</v>
+      </c>
+      <c r="S10" s="18">
+        <v>2</v>
+      </c>
+      <c r="T10" s="18">
+        <v>2</v>
+      </c>
+      <c r="U10" s="25">
+        <v>3</v>
+      </c>
+      <c r="V10" s="25">
+        <v>3</v>
+      </c>
+      <c r="W10" s="25">
+        <v>3</v>
+      </c>
+      <c r="X10" s="25">
+        <v>3</v>
+      </c>
+      <c r="Y10" s="25">
+        <v>3</v>
+      </c>
+      <c r="Z10" s="25">
+        <v>3</v>
+      </c>
+      <c r="AA10" s="25">
+        <v>3</v>
+      </c>
+      <c r="AB10" s="25">
+        <v>3</v>
+      </c>
+      <c r="AC10" s="25">
+        <v>3</v>
+      </c>
+      <c r="AD10" s="25">
+        <v>3</v>
+      </c>
+      <c r="AE10" s="25">
+        <v>3</v>
+      </c>
+      <c r="AF10" s="25">
+        <v>3</v>
+      </c>
+      <c r="AG10" s="25">
+        <v>3</v>
+      </c>
+      <c r="AH10" s="25">
+        <v>3</v>
+      </c>
+      <c r="AI10" s="25">
+        <v>3</v>
+      </c>
+      <c r="AJ10" s="25">
+        <v>3</v>
+      </c>
+      <c r="AK10" s="25">
+        <v>3</v>
+      </c>
+      <c r="AL10" s="25">
+        <v>3</v>
+      </c>
+      <c r="AM10" s="25">
+        <v>3</v>
+      </c>
+      <c r="AN10" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="18">
+        <v>2</v>
+      </c>
+      <c r="B11" s="18">
+        <v>2</v>
+      </c>
+      <c r="C11" s="18">
+        <v>2</v>
+      </c>
+      <c r="D11" s="18">
+        <v>2</v>
+      </c>
+      <c r="E11" s="18">
+        <v>2</v>
+      </c>
+      <c r="F11" s="18">
+        <v>2</v>
+      </c>
+      <c r="G11" s="18">
+        <v>2</v>
+      </c>
+      <c r="H11" s="18">
+        <v>2</v>
+      </c>
+      <c r="I11" s="18">
+        <v>2</v>
+      </c>
+      <c r="J11" s="18">
+        <v>2</v>
+      </c>
+      <c r="K11" s="18">
+        <v>2</v>
+      </c>
+      <c r="L11" s="18">
+        <v>2</v>
+      </c>
+      <c r="M11" s="18">
+        <v>2</v>
+      </c>
+      <c r="N11" s="18">
+        <v>2</v>
+      </c>
+      <c r="O11" s="18">
+        <v>2</v>
+      </c>
+      <c r="P11" s="18">
+        <v>2</v>
+      </c>
+      <c r="Q11" s="18">
+        <v>2</v>
+      </c>
+      <c r="R11" s="18">
+        <v>2</v>
+      </c>
+      <c r="S11" s="18">
+        <v>2</v>
+      </c>
+      <c r="T11" s="18">
+        <v>2</v>
+      </c>
+      <c r="U11" s="25">
+        <v>3</v>
+      </c>
+      <c r="V11" s="25">
+        <v>3</v>
+      </c>
+      <c r="W11" s="25">
+        <v>3</v>
+      </c>
+      <c r="X11" s="25">
+        <v>3</v>
+      </c>
+      <c r="Y11" s="25">
+        <v>3</v>
+      </c>
+      <c r="Z11" s="25">
+        <v>3</v>
+      </c>
+      <c r="AA11" s="25">
+        <v>3</v>
+      </c>
+      <c r="AB11" s="25">
+        <v>3</v>
+      </c>
+      <c r="AC11" s="25">
+        <v>3</v>
+      </c>
+      <c r="AD11" s="25">
+        <v>3</v>
+      </c>
+      <c r="AE11" s="25">
+        <v>3</v>
+      </c>
+      <c r="AF11" s="25">
+        <v>3</v>
+      </c>
+      <c r="AG11" s="25">
+        <v>3</v>
+      </c>
+      <c r="AH11" s="25">
+        <v>3</v>
+      </c>
+      <c r="AI11" s="25">
+        <v>3</v>
+      </c>
+      <c r="AJ11" s="25">
+        <v>3</v>
+      </c>
+      <c r="AK11" s="25">
+        <v>3</v>
+      </c>
+      <c r="AL11" s="25">
+        <v>3</v>
+      </c>
+      <c r="AM11" s="25">
+        <v>3</v>
+      </c>
+      <c r="AN11" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="18">
+        <v>2</v>
+      </c>
+      <c r="B12" s="18">
+        <v>2</v>
+      </c>
+      <c r="C12" s="18">
+        <v>2</v>
+      </c>
+      <c r="D12" s="18">
+        <v>2</v>
+      </c>
+      <c r="E12" s="18">
+        <v>2</v>
+      </c>
+      <c r="F12" s="18">
+        <v>2</v>
+      </c>
+      <c r="G12" s="18">
+        <v>2</v>
+      </c>
+      <c r="H12" s="18">
+        <v>2</v>
+      </c>
+      <c r="I12" s="18">
+        <v>2</v>
+      </c>
+      <c r="J12" s="18">
+        <v>2</v>
+      </c>
+      <c r="K12" s="18">
+        <v>2</v>
+      </c>
+      <c r="L12" s="18">
+        <v>2</v>
+      </c>
+      <c r="M12" s="18">
+        <v>2</v>
+      </c>
+      <c r="N12" s="18">
+        <v>2</v>
+      </c>
+      <c r="O12" s="18">
+        <v>2</v>
+      </c>
+      <c r="P12" s="18">
+        <v>2</v>
+      </c>
+      <c r="Q12" s="18">
+        <v>2</v>
+      </c>
+      <c r="R12" s="18">
+        <v>2</v>
+      </c>
+      <c r="S12" s="18">
+        <v>2</v>
+      </c>
+      <c r="T12" s="18">
+        <v>2</v>
+      </c>
+      <c r="U12" s="25">
+        <v>3</v>
+      </c>
+      <c r="V12" s="25">
+        <v>3</v>
+      </c>
+      <c r="W12" s="25">
+        <v>3</v>
+      </c>
+      <c r="X12" s="25">
+        <v>3</v>
+      </c>
+      <c r="Y12" s="25">
+        <v>3</v>
+      </c>
+      <c r="Z12" s="25">
+        <v>3</v>
+      </c>
+      <c r="AA12" s="25">
+        <v>3</v>
+      </c>
+      <c r="AB12" s="25">
+        <v>3</v>
+      </c>
+      <c r="AC12" s="25">
+        <v>3</v>
+      </c>
+      <c r="AD12" s="25">
+        <v>3</v>
+      </c>
+      <c r="AE12" s="25">
+        <v>3</v>
+      </c>
+      <c r="AF12" s="25">
+        <v>3</v>
+      </c>
+      <c r="AG12" s="25">
+        <v>3</v>
+      </c>
+      <c r="AH12" s="25">
+        <v>3</v>
+      </c>
+      <c r="AI12" s="25">
+        <v>3</v>
+      </c>
+      <c r="AJ12" s="25">
+        <v>3</v>
+      </c>
+      <c r="AK12" s="25">
+        <v>3</v>
+      </c>
+      <c r="AL12" s="25">
+        <v>3</v>
+      </c>
+      <c r="AM12" s="25">
+        <v>3</v>
+      </c>
+      <c r="AN12" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="18">
+        <v>2</v>
+      </c>
+      <c r="B13" s="18">
+        <v>2</v>
+      </c>
+      <c r="C13" s="18">
+        <v>2</v>
+      </c>
+      <c r="D13" s="18">
+        <v>2</v>
+      </c>
+      <c r="E13" s="18">
+        <v>2</v>
+      </c>
+      <c r="F13" s="18">
+        <v>2</v>
+      </c>
+      <c r="G13" s="18">
+        <v>2</v>
+      </c>
+      <c r="H13" s="18">
+        <v>2</v>
+      </c>
+      <c r="I13" s="18">
+        <v>2</v>
+      </c>
+      <c r="J13" s="18">
+        <v>2</v>
+      </c>
+      <c r="K13" s="18">
+        <v>2</v>
+      </c>
+      <c r="L13" s="18">
+        <v>2</v>
+      </c>
+      <c r="M13" s="18">
+        <v>2</v>
+      </c>
+      <c r="N13" s="18">
+        <v>2</v>
+      </c>
+      <c r="O13" s="18">
+        <v>2</v>
+      </c>
+      <c r="P13" s="18">
+        <v>2</v>
+      </c>
+      <c r="Q13" s="18">
+        <v>2</v>
+      </c>
+      <c r="R13" s="18">
+        <v>2</v>
+      </c>
+      <c r="S13" s="18">
+        <v>2</v>
+      </c>
+      <c r="T13" s="18">
+        <v>2</v>
+      </c>
+      <c r="U13" s="25">
+        <v>3</v>
+      </c>
+      <c r="V13" s="25">
+        <v>3</v>
+      </c>
+      <c r="W13" s="25">
+        <v>3</v>
+      </c>
+      <c r="X13" s="25">
+        <v>3</v>
+      </c>
+      <c r="Y13" s="25">
+        <v>3</v>
+      </c>
+      <c r="Z13" s="25">
+        <v>3</v>
+      </c>
+      <c r="AA13" s="25">
+        <v>3</v>
+      </c>
+      <c r="AB13" s="25">
+        <v>3</v>
+      </c>
+      <c r="AC13" s="25">
+        <v>3</v>
+      </c>
+      <c r="AD13" s="25">
+        <v>3</v>
+      </c>
+      <c r="AE13" s="25">
+        <v>3</v>
+      </c>
+      <c r="AF13" s="25">
+        <v>3</v>
+      </c>
+      <c r="AG13" s="25">
+        <v>3</v>
+      </c>
+      <c r="AH13" s="25">
+        <v>3</v>
+      </c>
+      <c r="AI13" s="25">
+        <v>3</v>
+      </c>
+      <c r="AJ13" s="25">
+        <v>3</v>
+      </c>
+      <c r="AK13" s="25">
+        <v>3</v>
+      </c>
+      <c r="AL13" s="25">
+        <v>3</v>
+      </c>
+      <c r="AM13" s="25">
+        <v>3</v>
+      </c>
+      <c r="AN13" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="18">
+        <v>2</v>
+      </c>
+      <c r="B14" s="18">
+        <v>2</v>
+      </c>
+      <c r="C14" s="18">
+        <v>2</v>
+      </c>
+      <c r="D14" s="18">
+        <v>2</v>
+      </c>
+      <c r="E14" s="18">
+        <v>2</v>
+      </c>
+      <c r="F14" s="18">
+        <v>2</v>
+      </c>
+      <c r="G14" s="18">
+        <v>2</v>
+      </c>
+      <c r="H14" s="18">
+        <v>2</v>
+      </c>
+      <c r="I14" s="18">
+        <v>2</v>
+      </c>
+      <c r="J14" s="18">
+        <v>2</v>
+      </c>
+      <c r="K14" s="18">
+        <v>2</v>
+      </c>
+      <c r="L14" s="18">
+        <v>2</v>
+      </c>
+      <c r="M14" s="18">
+        <v>2</v>
+      </c>
+      <c r="N14" s="18">
+        <v>2</v>
+      </c>
+      <c r="O14" s="18">
+        <v>2</v>
+      </c>
+      <c r="P14" s="18">
+        <v>2</v>
+      </c>
+      <c r="Q14" s="18">
+        <v>2</v>
+      </c>
+      <c r="R14" s="18">
+        <v>2</v>
+      </c>
+      <c r="S14" s="18">
+        <v>2</v>
+      </c>
+      <c r="T14" s="18">
+        <v>2</v>
+      </c>
+      <c r="U14" s="25">
+        <v>3</v>
+      </c>
+      <c r="V14" s="25">
+        <v>3</v>
+      </c>
+      <c r="W14" s="25">
+        <v>3</v>
+      </c>
+      <c r="X14" s="25">
+        <v>3</v>
+      </c>
+      <c r="Y14" s="25">
+        <v>3</v>
+      </c>
+      <c r="Z14" s="25">
+        <v>3</v>
+      </c>
+      <c r="AA14" s="25">
+        <v>3</v>
+      </c>
+      <c r="AB14" s="25">
+        <v>3</v>
+      </c>
+      <c r="AC14" s="25">
+        <v>3</v>
+      </c>
+      <c r="AD14" s="25">
+        <v>3</v>
+      </c>
+      <c r="AE14" s="25">
+        <v>3</v>
+      </c>
+      <c r="AF14" s="25">
+        <v>3</v>
+      </c>
+      <c r="AG14" s="25">
+        <v>3</v>
+      </c>
+      <c r="AH14" s="25">
+        <v>3</v>
+      </c>
+      <c r="AI14" s="25">
+        <v>3</v>
+      </c>
+      <c r="AJ14" s="25">
+        <v>3</v>
+      </c>
+      <c r="AK14" s="25">
+        <v>3</v>
+      </c>
+      <c r="AL14" s="25">
+        <v>3</v>
+      </c>
+      <c r="AM14" s="25">
+        <v>3</v>
+      </c>
+      <c r="AN14" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="18">
+        <v>2</v>
+      </c>
+      <c r="B15" s="18">
+        <v>2</v>
+      </c>
+      <c r="C15" s="18">
+        <v>2</v>
+      </c>
+      <c r="D15" s="18">
+        <v>2</v>
+      </c>
+      <c r="E15" s="18">
+        <v>2</v>
+      </c>
+      <c r="F15" s="18">
+        <v>2</v>
+      </c>
+      <c r="G15" s="18">
+        <v>2</v>
+      </c>
+      <c r="H15" s="18">
+        <v>2</v>
+      </c>
+      <c r="I15" s="18">
+        <v>2</v>
+      </c>
+      <c r="J15" s="18">
+        <v>2</v>
+      </c>
+      <c r="K15" s="18">
+        <v>2</v>
+      </c>
+      <c r="L15" s="18">
+        <v>2</v>
+      </c>
+      <c r="M15" s="18">
+        <v>2</v>
+      </c>
+      <c r="N15" s="18">
+        <v>2</v>
+      </c>
+      <c r="O15" s="18">
+        <v>2</v>
+      </c>
+      <c r="P15" s="18">
+        <v>2</v>
+      </c>
+      <c r="Q15" s="18">
+        <v>2</v>
+      </c>
+      <c r="R15" s="18">
+        <v>2</v>
+      </c>
+      <c r="S15" s="18">
+        <v>2</v>
+      </c>
+      <c r="T15" s="18">
+        <v>2</v>
+      </c>
+      <c r="U15" s="25">
+        <v>3</v>
+      </c>
+      <c r="V15" s="25">
+        <v>3</v>
+      </c>
+      <c r="W15" s="25">
+        <v>3</v>
+      </c>
+      <c r="X15" s="25">
+        <v>3</v>
+      </c>
+      <c r="Y15" s="25">
+        <v>3</v>
+      </c>
+      <c r="Z15" s="25">
+        <v>3</v>
+      </c>
+      <c r="AA15" s="25">
+        <v>3</v>
+      </c>
+      <c r="AB15" s="25">
+        <v>3</v>
+      </c>
+      <c r="AC15" s="25">
+        <v>3</v>
+      </c>
+      <c r="AD15" s="25">
+        <v>3</v>
+      </c>
+      <c r="AE15" s="25">
+        <v>3</v>
+      </c>
+      <c r="AF15" s="25">
+        <v>3</v>
+      </c>
+      <c r="AG15" s="25">
+        <v>3</v>
+      </c>
+      <c r="AH15" s="25">
+        <v>3</v>
+      </c>
+      <c r="AI15" s="25">
+        <v>3</v>
+      </c>
+      <c r="AJ15" s="25">
+        <v>3</v>
+      </c>
+      <c r="AK15" s="25">
+        <v>3</v>
+      </c>
+      <c r="AL15" s="25">
+        <v>3</v>
+      </c>
+      <c r="AM15" s="25">
+        <v>3</v>
+      </c>
+      <c r="AN15" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="18">
+        <v>2</v>
+      </c>
+      <c r="B16" s="18">
+        <v>2</v>
+      </c>
+      <c r="C16" s="18">
+        <v>2</v>
+      </c>
+      <c r="D16" s="18">
+        <v>2</v>
+      </c>
+      <c r="E16" s="18">
+        <v>2</v>
+      </c>
+      <c r="F16" s="18">
+        <v>2</v>
+      </c>
+      <c r="G16" s="18">
+        <v>2</v>
+      </c>
+      <c r="H16" s="18">
+        <v>2</v>
+      </c>
+      <c r="I16" s="18">
+        <v>2</v>
+      </c>
+      <c r="J16" s="18">
+        <v>2</v>
+      </c>
+      <c r="K16" s="18">
+        <v>2</v>
+      </c>
+      <c r="L16" s="18">
+        <v>2</v>
+      </c>
+      <c r="M16" s="18">
+        <v>2</v>
+      </c>
+      <c r="N16" s="18">
+        <v>2</v>
+      </c>
+      <c r="O16" s="18">
+        <v>2</v>
+      </c>
+      <c r="P16" s="18">
+        <v>2</v>
+      </c>
+      <c r="Q16" s="18">
+        <v>2</v>
+      </c>
+      <c r="R16" s="18">
+        <v>2</v>
+      </c>
+      <c r="S16" s="18">
+        <v>2</v>
+      </c>
+      <c r="T16" s="18">
+        <v>2</v>
+      </c>
+      <c r="U16" s="25">
+        <v>3</v>
+      </c>
+      <c r="V16" s="25">
+        <v>3</v>
+      </c>
+      <c r="W16" s="25">
+        <v>3</v>
+      </c>
+      <c r="X16" s="25">
+        <v>3</v>
+      </c>
+      <c r="Y16" s="25">
+        <v>3</v>
+      </c>
+      <c r="Z16" s="25">
+        <v>3</v>
+      </c>
+      <c r="AA16" s="25">
+        <v>3</v>
+      </c>
+      <c r="AB16" s="25">
+        <v>3</v>
+      </c>
+      <c r="AC16" s="25">
+        <v>3</v>
+      </c>
+      <c r="AD16" s="25">
+        <v>3</v>
+      </c>
+      <c r="AE16" s="25">
+        <v>3</v>
+      </c>
+      <c r="AF16" s="25">
+        <v>3</v>
+      </c>
+      <c r="AG16" s="25">
+        <v>3</v>
+      </c>
+      <c r="AH16" s="25">
+        <v>3</v>
+      </c>
+      <c r="AI16" s="25">
+        <v>3</v>
+      </c>
+      <c r="AJ16" s="25">
+        <v>3</v>
+      </c>
+      <c r="AK16" s="25">
+        <v>3</v>
+      </c>
+      <c r="AL16" s="25">
+        <v>3</v>
+      </c>
+      <c r="AM16" s="25">
+        <v>3</v>
+      </c>
+      <c r="AN16" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="18">
+        <v>2</v>
+      </c>
+      <c r="B17" s="18">
+        <v>2</v>
+      </c>
+      <c r="C17" s="18">
+        <v>2</v>
+      </c>
+      <c r="D17" s="18">
+        <v>2</v>
+      </c>
+      <c r="E17" s="18">
+        <v>2</v>
+      </c>
+      <c r="F17" s="18">
+        <v>2</v>
+      </c>
+      <c r="G17" s="18">
+        <v>2</v>
+      </c>
+      <c r="H17" s="18">
+        <v>2</v>
+      </c>
+      <c r="I17" s="18">
+        <v>2</v>
+      </c>
+      <c r="J17" s="18">
+        <v>2</v>
+      </c>
+      <c r="K17" s="18">
+        <v>2</v>
+      </c>
+      <c r="L17" s="18">
+        <v>2</v>
+      </c>
+      <c r="M17" s="18">
+        <v>2</v>
+      </c>
+      <c r="N17" s="18">
+        <v>2</v>
+      </c>
+      <c r="O17" s="18">
+        <v>2</v>
+      </c>
+      <c r="P17" s="18">
+        <v>2</v>
+      </c>
+      <c r="Q17" s="18">
+        <v>2</v>
+      </c>
+      <c r="R17" s="18">
+        <v>2</v>
+      </c>
+      <c r="S17" s="18">
+        <v>2</v>
+      </c>
+      <c r="T17" s="18">
+        <v>2</v>
+      </c>
+      <c r="U17" s="25">
+        <v>3</v>
+      </c>
+      <c r="V17" s="25">
+        <v>3</v>
+      </c>
+      <c r="W17" s="25">
+        <v>3</v>
+      </c>
+      <c r="X17" s="25">
+        <v>3</v>
+      </c>
+      <c r="Y17" s="25">
+        <v>3</v>
+      </c>
+      <c r="Z17" s="25">
+        <v>3</v>
+      </c>
+      <c r="AA17" s="25">
+        <v>3</v>
+      </c>
+      <c r="AB17" s="25">
+        <v>3</v>
+      </c>
+      <c r="AC17" s="25">
+        <v>3</v>
+      </c>
+      <c r="AD17" s="25">
+        <v>3</v>
+      </c>
+      <c r="AE17" s="25">
+        <v>3</v>
+      </c>
+      <c r="AF17" s="25">
+        <v>3</v>
+      </c>
+      <c r="AG17" s="25">
+        <v>3</v>
+      </c>
+      <c r="AH17" s="25">
+        <v>3</v>
+      </c>
+      <c r="AI17" s="25">
+        <v>3</v>
+      </c>
+      <c r="AJ17" s="25">
+        <v>3</v>
+      </c>
+      <c r="AK17" s="25">
+        <v>3</v>
+      </c>
+      <c r="AL17" s="25">
+        <v>3</v>
+      </c>
+      <c r="AM17" s="25">
+        <v>3</v>
+      </c>
+      <c r="AN17" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="21">
+        <v>4</v>
+      </c>
+      <c r="B18" s="21">
+        <v>4</v>
+      </c>
+      <c r="C18" s="21">
+        <v>4</v>
+      </c>
+      <c r="D18" s="21">
+        <v>4</v>
+      </c>
+      <c r="E18" s="21">
+        <v>4</v>
+      </c>
+      <c r="F18" s="21">
+        <v>4</v>
+      </c>
+      <c r="G18" s="21">
+        <v>4</v>
+      </c>
+      <c r="H18" s="21">
+        <v>4</v>
+      </c>
+      <c r="I18" s="21">
+        <v>4</v>
+      </c>
+      <c r="J18" s="21">
+        <v>4</v>
+      </c>
+      <c r="K18" s="21">
+        <v>4</v>
+      </c>
+      <c r="L18" s="21">
+        <v>4</v>
+      </c>
+      <c r="M18" s="21">
+        <v>4</v>
+      </c>
+      <c r="N18" s="21">
+        <v>4</v>
+      </c>
+      <c r="O18" s="21">
+        <v>4</v>
+      </c>
+      <c r="P18" s="21">
+        <v>4</v>
+      </c>
+      <c r="Q18" s="21">
+        <v>4</v>
+      </c>
+      <c r="R18" s="21">
+        <v>4</v>
+      </c>
+      <c r="S18" s="21">
+        <v>4</v>
+      </c>
+      <c r="T18" s="21">
+        <v>4</v>
+      </c>
+      <c r="U18" s="20">
+        <v>5</v>
+      </c>
+      <c r="V18" s="20">
+        <v>5</v>
+      </c>
+      <c r="W18" s="20">
+        <v>5</v>
+      </c>
+      <c r="X18" s="20">
+        <v>5</v>
+      </c>
+      <c r="Y18" s="20">
+        <v>5</v>
+      </c>
+      <c r="Z18" s="20">
+        <v>5</v>
+      </c>
+      <c r="AA18" s="20">
+        <v>5</v>
+      </c>
+      <c r="AB18" s="20">
+        <v>5</v>
+      </c>
+      <c r="AC18" s="20">
+        <v>5</v>
+      </c>
+      <c r="AD18" s="20">
+        <v>5</v>
+      </c>
+      <c r="AE18" s="20">
+        <v>5</v>
+      </c>
+      <c r="AF18" s="20">
+        <v>5</v>
+      </c>
+      <c r="AG18" s="20">
+        <v>5</v>
+      </c>
+      <c r="AH18" s="20">
+        <v>5</v>
+      </c>
+      <c r="AI18" s="20">
+        <v>5</v>
+      </c>
+      <c r="AJ18" s="20">
+        <v>5</v>
+      </c>
+      <c r="AK18" s="20">
+        <v>5</v>
+      </c>
+      <c r="AL18" s="20">
+        <v>5</v>
+      </c>
+      <c r="AM18" s="20">
+        <v>5</v>
+      </c>
+      <c r="AN18" s="20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="21">
+        <v>4</v>
+      </c>
+      <c r="B19" s="21">
+        <v>4</v>
+      </c>
+      <c r="C19" s="21">
+        <v>4</v>
+      </c>
+      <c r="D19" s="21">
+        <v>4</v>
+      </c>
+      <c r="E19" s="21">
+        <v>4</v>
+      </c>
+      <c r="F19" s="21">
+        <v>4</v>
+      </c>
+      <c r="G19" s="21">
+        <v>4</v>
+      </c>
+      <c r="H19" s="21">
+        <v>4</v>
+      </c>
+      <c r="I19" s="21">
+        <v>4</v>
+      </c>
+      <c r="J19" s="21">
+        <v>4</v>
+      </c>
+      <c r="K19" s="21">
+        <v>4</v>
+      </c>
+      <c r="L19" s="21">
+        <v>4</v>
+      </c>
+      <c r="M19" s="21">
+        <v>4</v>
+      </c>
+      <c r="N19" s="21">
+        <v>4</v>
+      </c>
+      <c r="O19" s="21">
+        <v>4</v>
+      </c>
+      <c r="P19" s="21">
+        <v>4</v>
+      </c>
+      <c r="Q19" s="21">
+        <v>4</v>
+      </c>
+      <c r="R19" s="21">
+        <v>4</v>
+      </c>
+      <c r="S19" s="21">
+        <v>4</v>
+      </c>
+      <c r="T19" s="21">
+        <v>4</v>
+      </c>
+      <c r="U19" s="20">
+        <v>5</v>
+      </c>
+      <c r="V19" s="20">
+        <v>5</v>
+      </c>
+      <c r="W19" s="20">
+        <v>5</v>
+      </c>
+      <c r="X19" s="20">
+        <v>5</v>
+      </c>
+      <c r="Y19" s="20">
+        <v>5</v>
+      </c>
+      <c r="Z19" s="20">
+        <v>5</v>
+      </c>
+      <c r="AA19" s="20">
+        <v>5</v>
+      </c>
+      <c r="AB19" s="20">
+        <v>5</v>
+      </c>
+      <c r="AC19" s="20">
+        <v>5</v>
+      </c>
+      <c r="AD19" s="20">
+        <v>5</v>
+      </c>
+      <c r="AE19" s="20">
+        <v>5</v>
+      </c>
+      <c r="AF19" s="20">
+        <v>5</v>
+      </c>
+      <c r="AG19" s="20">
+        <v>5</v>
+      </c>
+      <c r="AH19" s="20">
+        <v>5</v>
+      </c>
+      <c r="AI19" s="20">
+        <v>5</v>
+      </c>
+      <c r="AJ19" s="20">
+        <v>5</v>
+      </c>
+      <c r="AK19" s="20">
+        <v>5</v>
+      </c>
+      <c r="AL19" s="20">
+        <v>5</v>
+      </c>
+      <c r="AM19" s="20">
+        <v>5</v>
+      </c>
+      <c r="AN19" s="20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="21">
+        <v>4</v>
+      </c>
+      <c r="B20" s="21">
+        <v>4</v>
+      </c>
+      <c r="C20" s="21">
+        <v>4</v>
+      </c>
+      <c r="D20" s="21">
+        <v>4</v>
+      </c>
+      <c r="E20" s="21">
+        <v>4</v>
+      </c>
+      <c r="F20" s="21">
+        <v>4</v>
+      </c>
+      <c r="G20" s="21">
+        <v>4</v>
+      </c>
+      <c r="H20" s="21">
+        <v>4</v>
+      </c>
+      <c r="I20" s="21">
+        <v>4</v>
+      </c>
+      <c r="J20" s="21">
+        <v>4</v>
+      </c>
+      <c r="K20" s="21">
+        <v>4</v>
+      </c>
+      <c r="L20" s="21">
+        <v>4</v>
+      </c>
+      <c r="M20" s="21">
+        <v>4</v>
+      </c>
+      <c r="N20" s="21">
+        <v>4</v>
+      </c>
+      <c r="O20" s="21">
+        <v>4</v>
+      </c>
+      <c r="P20" s="21">
+        <v>4</v>
+      </c>
+      <c r="Q20" s="21">
+        <v>4</v>
+      </c>
+      <c r="R20" s="21">
+        <v>4</v>
+      </c>
+      <c r="S20" s="21">
+        <v>4</v>
+      </c>
+      <c r="T20" s="21">
+        <v>4</v>
+      </c>
+      <c r="U20" s="20">
+        <v>5</v>
+      </c>
+      <c r="V20" s="20">
+        <v>5</v>
+      </c>
+      <c r="W20" s="20">
+        <v>5</v>
+      </c>
+      <c r="X20" s="20">
+        <v>5</v>
+      </c>
+      <c r="Y20" s="20">
+        <v>5</v>
+      </c>
+      <c r="Z20" s="20">
+        <v>5</v>
+      </c>
+      <c r="AA20" s="20">
+        <v>5</v>
+      </c>
+      <c r="AB20" s="20">
+        <v>5</v>
+      </c>
+      <c r="AC20" s="20">
+        <v>5</v>
+      </c>
+      <c r="AD20" s="20">
+        <v>5</v>
+      </c>
+      <c r="AE20" s="20">
+        <v>5</v>
+      </c>
+      <c r="AF20" s="20">
+        <v>5</v>
+      </c>
+      <c r="AG20" s="20">
+        <v>5</v>
+      </c>
+      <c r="AH20" s="20">
+        <v>5</v>
+      </c>
+      <c r="AI20" s="20">
+        <v>5</v>
+      </c>
+      <c r="AJ20" s="20">
+        <v>5</v>
+      </c>
+      <c r="AK20" s="20">
+        <v>5</v>
+      </c>
+      <c r="AL20" s="20">
+        <v>5</v>
+      </c>
+      <c r="AM20" s="20">
+        <v>5</v>
+      </c>
+      <c r="AN20" s="20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="21">
+        <v>4</v>
+      </c>
+      <c r="B21" s="21">
+        <v>4</v>
+      </c>
+      <c r="C21" s="21">
+        <v>4</v>
+      </c>
+      <c r="D21" s="21">
+        <v>4</v>
+      </c>
+      <c r="E21" s="21">
+        <v>4</v>
+      </c>
+      <c r="F21" s="21">
+        <v>4</v>
+      </c>
+      <c r="G21" s="21">
+        <v>4</v>
+      </c>
+      <c r="H21" s="21">
+        <v>4</v>
+      </c>
+      <c r="I21" s="21">
+        <v>4</v>
+      </c>
+      <c r="J21" s="21">
+        <v>4</v>
+      </c>
+      <c r="K21" s="21">
+        <v>4</v>
+      </c>
+      <c r="L21" s="21">
+        <v>4</v>
+      </c>
+      <c r="M21" s="21">
+        <v>4</v>
+      </c>
+      <c r="N21" s="21">
+        <v>4</v>
+      </c>
+      <c r="O21" s="21">
+        <v>4</v>
+      </c>
+      <c r="P21" s="21">
+        <v>4</v>
+      </c>
+      <c r="Q21" s="21">
+        <v>4</v>
+      </c>
+      <c r="R21" s="21">
+        <v>4</v>
+      </c>
+      <c r="S21" s="21">
+        <v>4</v>
+      </c>
+      <c r="T21" s="21">
+        <v>4</v>
+      </c>
+      <c r="U21" s="20">
+        <v>5</v>
+      </c>
+      <c r="V21" s="20">
+        <v>5</v>
+      </c>
+      <c r="W21" s="20">
+        <v>5</v>
+      </c>
+      <c r="X21" s="20">
+        <v>5</v>
+      </c>
+      <c r="Y21" s="20">
+        <v>5</v>
+      </c>
+      <c r="Z21" s="20">
+        <v>5</v>
+      </c>
+      <c r="AA21" s="20">
+        <v>5</v>
+      </c>
+      <c r="AB21" s="20">
+        <v>5</v>
+      </c>
+      <c r="AC21" s="20">
+        <v>5</v>
+      </c>
+      <c r="AD21" s="20">
+        <v>5</v>
+      </c>
+      <c r="AE21" s="20">
+        <v>5</v>
+      </c>
+      <c r="AF21" s="20">
+        <v>5</v>
+      </c>
+      <c r="AG21" s="20">
+        <v>5</v>
+      </c>
+      <c r="AH21" s="20">
+        <v>5</v>
+      </c>
+      <c r="AI21" s="20">
+        <v>5</v>
+      </c>
+      <c r="AJ21" s="20">
+        <v>5</v>
+      </c>
+      <c r="AK21" s="20">
+        <v>5</v>
+      </c>
+      <c r="AL21" s="20">
+        <v>5</v>
+      </c>
+      <c r="AM21" s="20">
+        <v>5</v>
+      </c>
+      <c r="AN21" s="20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="21">
+        <v>4</v>
+      </c>
+      <c r="B22" s="21">
+        <v>4</v>
+      </c>
+      <c r="C22" s="21">
+        <v>4</v>
+      </c>
+      <c r="D22" s="21">
+        <v>4</v>
+      </c>
+      <c r="E22" s="21">
+        <v>4</v>
+      </c>
+      <c r="F22" s="21">
+        <v>4</v>
+      </c>
+      <c r="G22" s="21">
+        <v>4</v>
+      </c>
+      <c r="H22" s="21">
+        <v>4</v>
+      </c>
+      <c r="I22" s="21">
+        <v>4</v>
+      </c>
+      <c r="J22" s="21">
+        <v>4</v>
+      </c>
+      <c r="K22" s="21">
+        <v>4</v>
+      </c>
+      <c r="L22" s="21">
+        <v>4</v>
+      </c>
+      <c r="M22" s="21">
+        <v>4</v>
+      </c>
+      <c r="N22" s="21">
+        <v>4</v>
+      </c>
+      <c r="O22" s="21">
+        <v>4</v>
+      </c>
+      <c r="P22" s="21">
+        <v>4</v>
+      </c>
+      <c r="Q22" s="21">
+        <v>4</v>
+      </c>
+      <c r="R22" s="21">
+        <v>4</v>
+      </c>
+      <c r="S22" s="21">
+        <v>4</v>
+      </c>
+      <c r="T22" s="21">
+        <v>4</v>
+      </c>
+      <c r="U22" s="20">
+        <v>5</v>
+      </c>
+      <c r="V22" s="20">
+        <v>5</v>
+      </c>
+      <c r="W22" s="20">
+        <v>5</v>
+      </c>
+      <c r="X22" s="20">
+        <v>5</v>
+      </c>
+      <c r="Y22" s="20">
+        <v>5</v>
+      </c>
+      <c r="Z22" s="20">
+        <v>5</v>
+      </c>
+      <c r="AA22" s="20">
+        <v>5</v>
+      </c>
+      <c r="AB22" s="20">
+        <v>5</v>
+      </c>
+      <c r="AC22" s="20">
+        <v>5</v>
+      </c>
+      <c r="AD22" s="20">
+        <v>5</v>
+      </c>
+      <c r="AE22" s="20">
+        <v>5</v>
+      </c>
+      <c r="AF22" s="20">
+        <v>5</v>
+      </c>
+      <c r="AG22" s="20">
+        <v>5</v>
+      </c>
+      <c r="AH22" s="20">
+        <v>5</v>
+      </c>
+      <c r="AI22" s="20">
+        <v>5</v>
+      </c>
+      <c r="AJ22" s="20">
+        <v>5</v>
+      </c>
+      <c r="AK22" s="20">
+        <v>5</v>
+      </c>
+      <c r="AL22" s="20">
+        <v>5</v>
+      </c>
+      <c r="AM22" s="20">
+        <v>5</v>
+      </c>
+      <c r="AN22" s="20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="21">
+        <v>4</v>
+      </c>
+      <c r="B23" s="21">
+        <v>4</v>
+      </c>
+      <c r="C23" s="21">
+        <v>4</v>
+      </c>
+      <c r="D23" s="21">
+        <v>4</v>
+      </c>
+      <c r="E23" s="21">
+        <v>4</v>
+      </c>
+      <c r="F23" s="21">
+        <v>4</v>
+      </c>
+      <c r="G23" s="21">
+        <v>4</v>
+      </c>
+      <c r="H23" s="21">
+        <v>4</v>
+      </c>
+      <c r="I23" s="21">
+        <v>4</v>
+      </c>
+      <c r="J23" s="21">
+        <v>4</v>
+      </c>
+      <c r="K23" s="21">
+        <v>4</v>
+      </c>
+      <c r="L23" s="21">
+        <v>4</v>
+      </c>
+      <c r="M23" s="21">
+        <v>4</v>
+      </c>
+      <c r="N23" s="21">
+        <v>4</v>
+      </c>
+      <c r="O23" s="21">
+        <v>4</v>
+      </c>
+      <c r="P23" s="21">
+        <v>4</v>
+      </c>
+      <c r="Q23" s="21">
+        <v>4</v>
+      </c>
+      <c r="R23" s="21">
+        <v>4</v>
+      </c>
+      <c r="S23" s="21">
+        <v>4</v>
+      </c>
+      <c r="T23" s="21">
+        <v>4</v>
+      </c>
+      <c r="U23" s="20">
+        <v>5</v>
+      </c>
+      <c r="V23" s="20">
+        <v>5</v>
+      </c>
+      <c r="W23" s="20">
+        <v>5</v>
+      </c>
+      <c r="X23" s="20">
+        <v>5</v>
+      </c>
+      <c r="Y23" s="20">
+        <v>5</v>
+      </c>
+      <c r="Z23" s="20">
+        <v>5</v>
+      </c>
+      <c r="AA23" s="20">
+        <v>5</v>
+      </c>
+      <c r="AB23" s="20">
+        <v>5</v>
+      </c>
+      <c r="AC23" s="20">
+        <v>5</v>
+      </c>
+      <c r="AD23" s="20">
+        <v>5</v>
+      </c>
+      <c r="AE23" s="20">
+        <v>5</v>
+      </c>
+      <c r="AF23" s="20">
+        <v>5</v>
+      </c>
+      <c r="AG23" s="20">
+        <v>5</v>
+      </c>
+      <c r="AH23" s="20">
+        <v>5</v>
+      </c>
+      <c r="AI23" s="20">
+        <v>5</v>
+      </c>
+      <c r="AJ23" s="20">
+        <v>5</v>
+      </c>
+      <c r="AK23" s="20">
+        <v>5</v>
+      </c>
+      <c r="AL23" s="20">
+        <v>5</v>
+      </c>
+      <c r="AM23" s="20">
+        <v>5</v>
+      </c>
+      <c r="AN23" s="20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="21">
+        <v>4</v>
+      </c>
+      <c r="B24" s="21">
+        <v>4</v>
+      </c>
+      <c r="C24" s="21">
+        <v>4</v>
+      </c>
+      <c r="D24" s="21">
+        <v>4</v>
+      </c>
+      <c r="E24" s="21">
+        <v>4</v>
+      </c>
+      <c r="F24" s="21">
+        <v>4</v>
+      </c>
+      <c r="G24" s="21">
+        <v>4</v>
+      </c>
+      <c r="H24" s="21">
+        <v>4</v>
+      </c>
+      <c r="I24" s="21">
+        <v>4</v>
+      </c>
+      <c r="J24" s="21">
+        <v>4</v>
+      </c>
+      <c r="K24" s="21">
+        <v>4</v>
+      </c>
+      <c r="L24" s="21">
+        <v>4</v>
+      </c>
+      <c r="M24" s="21">
+        <v>4</v>
+      </c>
+      <c r="N24" s="21">
+        <v>4</v>
+      </c>
+      <c r="O24" s="21">
+        <v>4</v>
+      </c>
+      <c r="P24" s="21">
+        <v>4</v>
+      </c>
+      <c r="Q24" s="21">
+        <v>4</v>
+      </c>
+      <c r="R24" s="21">
+        <v>4</v>
+      </c>
+      <c r="S24" s="21">
+        <v>4</v>
+      </c>
+      <c r="T24" s="21">
+        <v>4</v>
+      </c>
+      <c r="U24" s="20">
+        <v>5</v>
+      </c>
+      <c r="V24" s="20">
+        <v>5</v>
+      </c>
+      <c r="W24" s="20">
+        <v>5</v>
+      </c>
+      <c r="X24" s="20">
+        <v>5</v>
+      </c>
+      <c r="Y24" s="20">
+        <v>5</v>
+      </c>
+      <c r="Z24" s="20">
+        <v>5</v>
+      </c>
+      <c r="AA24" s="20">
+        <v>5</v>
+      </c>
+      <c r="AB24" s="20">
+        <v>5</v>
+      </c>
+      <c r="AC24" s="20">
+        <v>5</v>
+      </c>
+      <c r="AD24" s="20">
+        <v>5</v>
+      </c>
+      <c r="AE24" s="20">
+        <v>5</v>
+      </c>
+      <c r="AF24" s="20">
+        <v>5</v>
+      </c>
+      <c r="AG24" s="20">
+        <v>5</v>
+      </c>
+      <c r="AH24" s="20">
+        <v>5</v>
+      </c>
+      <c r="AI24" s="20">
+        <v>5</v>
+      </c>
+      <c r="AJ24" s="20">
+        <v>5</v>
+      </c>
+      <c r="AK24" s="20">
+        <v>5</v>
+      </c>
+      <c r="AL24" s="20">
+        <v>5</v>
+      </c>
+      <c r="AM24" s="20">
+        <v>5</v>
+      </c>
+      <c r="AN24" s="20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="21">
+        <v>4</v>
+      </c>
+      <c r="B25" s="21">
+        <v>4</v>
+      </c>
+      <c r="C25" s="21">
+        <v>4</v>
+      </c>
+      <c r="D25" s="21">
+        <v>4</v>
+      </c>
+      <c r="E25" s="21">
+        <v>4</v>
+      </c>
+      <c r="F25" s="21">
+        <v>4</v>
+      </c>
+      <c r="G25" s="21">
+        <v>4</v>
+      </c>
+      <c r="H25" s="21">
+        <v>4</v>
+      </c>
+      <c r="I25" s="21">
+        <v>4</v>
+      </c>
+      <c r="J25" s="21">
+        <v>4</v>
+      </c>
+      <c r="K25" s="21">
+        <v>4</v>
+      </c>
+      <c r="L25" s="21">
+        <v>4</v>
+      </c>
+      <c r="M25" s="21">
+        <v>4</v>
+      </c>
+      <c r="N25" s="21">
+        <v>4</v>
+      </c>
+      <c r="O25" s="21">
+        <v>4</v>
+      </c>
+      <c r="P25" s="21">
+        <v>4</v>
+      </c>
+      <c r="Q25" s="21">
+        <v>4</v>
+      </c>
+      <c r="R25" s="21">
+        <v>4</v>
+      </c>
+      <c r="S25" s="21">
+        <v>4</v>
+      </c>
+      <c r="T25" s="21">
+        <v>4</v>
+      </c>
+      <c r="U25" s="20">
+        <v>5</v>
+      </c>
+      <c r="V25" s="20">
+        <v>5</v>
+      </c>
+      <c r="W25" s="20">
+        <v>5</v>
+      </c>
+      <c r="X25" s="20">
+        <v>5</v>
+      </c>
+      <c r="Y25" s="20">
+        <v>5</v>
+      </c>
+      <c r="Z25" s="20">
+        <v>5</v>
+      </c>
+      <c r="AA25" s="20">
+        <v>5</v>
+      </c>
+      <c r="AB25" s="20">
+        <v>5</v>
+      </c>
+      <c r="AC25" s="20">
+        <v>5</v>
+      </c>
+      <c r="AD25" s="20">
+        <v>5</v>
+      </c>
+      <c r="AE25" s="20">
+        <v>5</v>
+      </c>
+      <c r="AF25" s="20">
+        <v>5</v>
+      </c>
+      <c r="AG25" s="20">
+        <v>5</v>
+      </c>
+      <c r="AH25" s="20">
+        <v>5</v>
+      </c>
+      <c r="AI25" s="20">
+        <v>5</v>
+      </c>
+      <c r="AJ25" s="20">
+        <v>5</v>
+      </c>
+      <c r="AK25" s="20">
+        <v>5</v>
+      </c>
+      <c r="AL25" s="20">
+        <v>5</v>
+      </c>
+      <c r="AM25" s="20">
+        <v>5</v>
+      </c>
+      <c r="AN25" s="20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="21">
+        <v>4</v>
+      </c>
+      <c r="B26" s="21">
+        <v>4</v>
+      </c>
+      <c r="C26" s="21">
+        <v>4</v>
+      </c>
+      <c r="D26" s="21">
+        <v>4</v>
+      </c>
+      <c r="E26" s="21">
+        <v>4</v>
+      </c>
+      <c r="F26" s="21">
+        <v>4</v>
+      </c>
+      <c r="G26" s="21">
+        <v>4</v>
+      </c>
+      <c r="H26" s="21">
+        <v>4</v>
+      </c>
+      <c r="I26" s="21">
+        <v>4</v>
+      </c>
+      <c r="J26" s="21">
+        <v>4</v>
+      </c>
+      <c r="K26" s="21">
+        <v>4</v>
+      </c>
+      <c r="L26" s="21">
+        <v>4</v>
+      </c>
+      <c r="M26" s="21">
+        <v>4</v>
+      </c>
+      <c r="N26" s="21">
+        <v>4</v>
+      </c>
+      <c r="O26" s="21">
+        <v>4</v>
+      </c>
+      <c r="P26" s="21">
+        <v>4</v>
+      </c>
+      <c r="Q26" s="21">
+        <v>4</v>
+      </c>
+      <c r="R26" s="21">
+        <v>4</v>
+      </c>
+      <c r="S26" s="21">
+        <v>4</v>
+      </c>
+      <c r="T26" s="21">
+        <v>4</v>
+      </c>
+      <c r="U26" s="20">
+        <v>5</v>
+      </c>
+      <c r="V26" s="20">
+        <v>5</v>
+      </c>
+      <c r="W26" s="20">
+        <v>5</v>
+      </c>
+      <c r="X26" s="20">
+        <v>5</v>
+      </c>
+      <c r="Y26" s="20">
+        <v>5</v>
+      </c>
+      <c r="Z26" s="20">
+        <v>5</v>
+      </c>
+      <c r="AA26" s="20">
+        <v>5</v>
+      </c>
+      <c r="AB26" s="20">
+        <v>5</v>
+      </c>
+      <c r="AC26" s="20">
+        <v>5</v>
+      </c>
+      <c r="AD26" s="20">
+        <v>5</v>
+      </c>
+      <c r="AE26" s="20">
+        <v>5</v>
+      </c>
+      <c r="AF26" s="20">
+        <v>5</v>
+      </c>
+      <c r="AG26" s="20">
+        <v>5</v>
+      </c>
+      <c r="AH26" s="20">
+        <v>5</v>
+      </c>
+      <c r="AI26" s="20">
+        <v>5</v>
+      </c>
+      <c r="AJ26" s="20">
+        <v>5</v>
+      </c>
+      <c r="AK26" s="20">
+        <v>5</v>
+      </c>
+      <c r="AL26" s="20">
+        <v>5</v>
+      </c>
+      <c r="AM26" s="20">
+        <v>5</v>
+      </c>
+      <c r="AN26" s="20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="21">
+        <v>4</v>
+      </c>
+      <c r="B27" s="21">
+        <v>4</v>
+      </c>
+      <c r="C27" s="21">
+        <v>4</v>
+      </c>
+      <c r="D27" s="21">
+        <v>4</v>
+      </c>
+      <c r="E27" s="21">
+        <v>4</v>
+      </c>
+      <c r="F27" s="21">
+        <v>4</v>
+      </c>
+      <c r="G27" s="21">
+        <v>4</v>
+      </c>
+      <c r="H27" s="21">
+        <v>4</v>
+      </c>
+      <c r="I27" s="21">
+        <v>4</v>
+      </c>
+      <c r="J27" s="21">
+        <v>4</v>
+      </c>
+      <c r="K27" s="21">
+        <v>4</v>
+      </c>
+      <c r="L27" s="21">
+        <v>4</v>
+      </c>
+      <c r="M27" s="21">
+        <v>4</v>
+      </c>
+      <c r="N27" s="21">
+        <v>4</v>
+      </c>
+      <c r="O27" s="21">
+        <v>4</v>
+      </c>
+      <c r="P27" s="21">
+        <v>4</v>
+      </c>
+      <c r="Q27" s="21">
+        <v>4</v>
+      </c>
+      <c r="R27" s="21">
+        <v>4</v>
+      </c>
+      <c r="S27" s="21">
+        <v>4</v>
+      </c>
+      <c r="T27" s="21">
+        <v>4</v>
+      </c>
+      <c r="U27" s="20">
+        <v>5</v>
+      </c>
+      <c r="V27" s="20">
+        <v>5</v>
+      </c>
+      <c r="W27" s="20">
+        <v>5</v>
+      </c>
+      <c r="X27" s="20">
+        <v>5</v>
+      </c>
+      <c r="Y27" s="20">
+        <v>5</v>
+      </c>
+      <c r="Z27" s="20">
+        <v>5</v>
+      </c>
+      <c r="AA27" s="20">
+        <v>5</v>
+      </c>
+      <c r="AB27" s="20">
+        <v>5</v>
+      </c>
+      <c r="AC27" s="20">
+        <v>5</v>
+      </c>
+      <c r="AD27" s="20">
+        <v>5</v>
+      </c>
+      <c r="AE27" s="20">
+        <v>5</v>
+      </c>
+      <c r="AF27" s="20">
+        <v>5</v>
+      </c>
+      <c r="AG27" s="20">
+        <v>5</v>
+      </c>
+      <c r="AH27" s="20">
+        <v>5</v>
+      </c>
+      <c r="AI27" s="20">
+        <v>5</v>
+      </c>
+      <c r="AJ27" s="20">
+        <v>5</v>
+      </c>
+      <c r="AK27" s="20">
+        <v>5</v>
+      </c>
+      <c r="AL27" s="20">
+        <v>5</v>
+      </c>
+      <c r="AM27" s="20">
+        <v>5</v>
+      </c>
+      <c r="AN27" s="20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="21">
+        <v>4</v>
+      </c>
+      <c r="B28" s="21">
+        <v>4</v>
+      </c>
+      <c r="C28" s="21">
+        <v>4</v>
+      </c>
+      <c r="D28" s="21">
+        <v>4</v>
+      </c>
+      <c r="E28" s="21">
+        <v>4</v>
+      </c>
+      <c r="F28" s="21">
+        <v>4</v>
+      </c>
+      <c r="G28" s="21">
+        <v>4</v>
+      </c>
+      <c r="H28" s="21">
+        <v>4</v>
+      </c>
+      <c r="I28" s="21">
+        <v>4</v>
+      </c>
+      <c r="J28" s="21">
+        <v>4</v>
+      </c>
+      <c r="K28" s="21">
+        <v>4</v>
+      </c>
+      <c r="L28" s="21">
+        <v>4</v>
+      </c>
+      <c r="M28" s="21">
+        <v>4</v>
+      </c>
+      <c r="N28" s="21">
+        <v>4</v>
+      </c>
+      <c r="O28" s="21">
+        <v>4</v>
+      </c>
+      <c r="P28" s="21">
+        <v>4</v>
+      </c>
+      <c r="Q28" s="21">
+        <v>4</v>
+      </c>
+      <c r="R28" s="21">
+        <v>4</v>
+      </c>
+      <c r="S28" s="21">
+        <v>4</v>
+      </c>
+      <c r="T28" s="21">
+        <v>4</v>
+      </c>
+      <c r="U28" s="20">
+        <v>5</v>
+      </c>
+      <c r="V28" s="20">
+        <v>5</v>
+      </c>
+      <c r="W28" s="20">
+        <v>5</v>
+      </c>
+      <c r="X28" s="20">
+        <v>5</v>
+      </c>
+      <c r="Y28" s="20">
+        <v>5</v>
+      </c>
+      <c r="Z28" s="20">
+        <v>5</v>
+      </c>
+      <c r="AA28" s="20">
+        <v>5</v>
+      </c>
+      <c r="AB28" s="20">
+        <v>5</v>
+      </c>
+      <c r="AC28" s="20">
+        <v>5</v>
+      </c>
+      <c r="AD28" s="20">
+        <v>5</v>
+      </c>
+      <c r="AE28" s="20">
+        <v>5</v>
+      </c>
+      <c r="AF28" s="20">
+        <v>5</v>
+      </c>
+      <c r="AG28" s="20">
+        <v>5</v>
+      </c>
+      <c r="AH28" s="20">
+        <v>5</v>
+      </c>
+      <c r="AI28" s="20">
+        <v>5</v>
+      </c>
+      <c r="AJ28" s="20">
+        <v>5</v>
+      </c>
+      <c r="AK28" s="20">
+        <v>5</v>
+      </c>
+      <c r="AL28" s="20">
+        <v>5</v>
+      </c>
+      <c r="AM28" s="20">
+        <v>5</v>
+      </c>
+      <c r="AN28" s="20">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add equity market pages
</commit_message>
<xml_diff>
--- a/layouts.xlsx
+++ b/layouts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/046b73b793af0aea/PAMGMT/projects/tamarac/economic-market-commentary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="364" documentId="8_{16FB9176-5700-CA44-8DDA-ADDCE61D2EC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{84A94ABD-011B-004C-9767-C5F012F0E50F}"/>
+  <xr:revisionPtr revIDLastSave="370" documentId="8_{16FB9176-5700-CA44-8DDA-ADDCE61D2EC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B0BCBCB8-CE17-4645-AB83-5D440F45D4AB}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="1600" windowWidth="28040" windowHeight="18100" firstSheet="1" activeTab="16" xr2:uid="{7344E464-CEB7-A74D-A529-F1BDE3AF96EC}"/>
+    <workbookView xWindow="3900" yWindow="1600" windowWidth="28040" windowHeight="18100" firstSheet="2" activeTab="17" xr2:uid="{7344E464-CEB7-A74D-A529-F1BDE3AF96EC}"/>
   </bookViews>
   <sheets>
     <sheet name="lay-1" sheetId="2" r:id="rId1"/>
@@ -30,6 +30,7 @@
     <sheet name="lay-15" sheetId="17" r:id="rId15"/>
     <sheet name="lay-16" sheetId="18" r:id="rId16"/>
     <sheet name="lay-17" sheetId="19" r:id="rId17"/>
+    <sheet name="lay-18" sheetId="20" r:id="rId18"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="41">
   <si>
     <t>a</t>
   </si>
@@ -27976,7 +27977,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5268B644-7A89-8D49-B8FB-D1817D32BA26}">
   <dimension ref="A1:AN28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L18" sqref="L18:AN28"/>
     </sheetView>
   </sheetViews>
@@ -30423,6 +30424,3440 @@
       </c>
       <c r="AN20" s="3">
         <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="3">
+        <v>4</v>
+      </c>
+      <c r="B21" s="3">
+        <v>4</v>
+      </c>
+      <c r="C21" s="3">
+        <v>4</v>
+      </c>
+      <c r="D21" s="3">
+        <v>4</v>
+      </c>
+      <c r="E21" s="3">
+        <v>4</v>
+      </c>
+      <c r="F21" s="3">
+        <v>4</v>
+      </c>
+      <c r="G21" s="3">
+        <v>4</v>
+      </c>
+      <c r="H21" s="3">
+        <v>4</v>
+      </c>
+      <c r="I21" s="3">
+        <v>4</v>
+      </c>
+      <c r="J21" s="3">
+        <v>4</v>
+      </c>
+      <c r="K21" s="3">
+        <v>4</v>
+      </c>
+      <c r="L21" s="3">
+        <v>4</v>
+      </c>
+      <c r="M21" s="3">
+        <v>4</v>
+      </c>
+      <c r="N21" s="3">
+        <v>4</v>
+      </c>
+      <c r="O21" s="3">
+        <v>4</v>
+      </c>
+      <c r="P21" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q21" s="3">
+        <v>4</v>
+      </c>
+      <c r="R21" s="3">
+        <v>4</v>
+      </c>
+      <c r="S21" s="3">
+        <v>4</v>
+      </c>
+      <c r="T21" s="3">
+        <v>4</v>
+      </c>
+      <c r="U21" s="3">
+        <v>4</v>
+      </c>
+      <c r="V21" s="3">
+        <v>4</v>
+      </c>
+      <c r="W21" s="3">
+        <v>4</v>
+      </c>
+      <c r="X21" s="3">
+        <v>4</v>
+      </c>
+      <c r="Y21" s="3">
+        <v>4</v>
+      </c>
+      <c r="Z21" s="3">
+        <v>4</v>
+      </c>
+      <c r="AA21" s="3">
+        <v>4</v>
+      </c>
+      <c r="AB21" s="3">
+        <v>4</v>
+      </c>
+      <c r="AC21" s="3">
+        <v>4</v>
+      </c>
+      <c r="AD21" s="3">
+        <v>4</v>
+      </c>
+      <c r="AE21" s="3">
+        <v>4</v>
+      </c>
+      <c r="AF21" s="3">
+        <v>4</v>
+      </c>
+      <c r="AG21" s="3">
+        <v>4</v>
+      </c>
+      <c r="AH21" s="3">
+        <v>4</v>
+      </c>
+      <c r="AI21" s="3">
+        <v>4</v>
+      </c>
+      <c r="AJ21" s="3">
+        <v>4</v>
+      </c>
+      <c r="AK21" s="3">
+        <v>4</v>
+      </c>
+      <c r="AL21" s="3">
+        <v>4</v>
+      </c>
+      <c r="AM21" s="3">
+        <v>4</v>
+      </c>
+      <c r="AN21" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="3">
+        <v>4</v>
+      </c>
+      <c r="B22" s="3">
+        <v>4</v>
+      </c>
+      <c r="C22" s="3">
+        <v>4</v>
+      </c>
+      <c r="D22" s="3">
+        <v>4</v>
+      </c>
+      <c r="E22" s="3">
+        <v>4</v>
+      </c>
+      <c r="F22" s="3">
+        <v>4</v>
+      </c>
+      <c r="G22" s="3">
+        <v>4</v>
+      </c>
+      <c r="H22" s="3">
+        <v>4</v>
+      </c>
+      <c r="I22" s="3">
+        <v>4</v>
+      </c>
+      <c r="J22" s="3">
+        <v>4</v>
+      </c>
+      <c r="K22" s="3">
+        <v>4</v>
+      </c>
+      <c r="L22" s="3">
+        <v>4</v>
+      </c>
+      <c r="M22" s="3">
+        <v>4</v>
+      </c>
+      <c r="N22" s="3">
+        <v>4</v>
+      </c>
+      <c r="O22" s="3">
+        <v>4</v>
+      </c>
+      <c r="P22" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q22" s="3">
+        <v>4</v>
+      </c>
+      <c r="R22" s="3">
+        <v>4</v>
+      </c>
+      <c r="S22" s="3">
+        <v>4</v>
+      </c>
+      <c r="T22" s="3">
+        <v>4</v>
+      </c>
+      <c r="U22" s="3">
+        <v>4</v>
+      </c>
+      <c r="V22" s="3">
+        <v>4</v>
+      </c>
+      <c r="W22" s="3">
+        <v>4</v>
+      </c>
+      <c r="X22" s="3">
+        <v>4</v>
+      </c>
+      <c r="Y22" s="3">
+        <v>4</v>
+      </c>
+      <c r="Z22" s="3">
+        <v>4</v>
+      </c>
+      <c r="AA22" s="3">
+        <v>4</v>
+      </c>
+      <c r="AB22" s="3">
+        <v>4</v>
+      </c>
+      <c r="AC22" s="3">
+        <v>4</v>
+      </c>
+      <c r="AD22" s="3">
+        <v>4</v>
+      </c>
+      <c r="AE22" s="3">
+        <v>4</v>
+      </c>
+      <c r="AF22" s="3">
+        <v>4</v>
+      </c>
+      <c r="AG22" s="3">
+        <v>4</v>
+      </c>
+      <c r="AH22" s="3">
+        <v>4</v>
+      </c>
+      <c r="AI22" s="3">
+        <v>4</v>
+      </c>
+      <c r="AJ22" s="3">
+        <v>4</v>
+      </c>
+      <c r="AK22" s="3">
+        <v>4</v>
+      </c>
+      <c r="AL22" s="3">
+        <v>4</v>
+      </c>
+      <c r="AM22" s="3">
+        <v>4</v>
+      </c>
+      <c r="AN22" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="3">
+        <v>4</v>
+      </c>
+      <c r="B23" s="3">
+        <v>4</v>
+      </c>
+      <c r="C23" s="3">
+        <v>4</v>
+      </c>
+      <c r="D23" s="3">
+        <v>4</v>
+      </c>
+      <c r="E23" s="3">
+        <v>4</v>
+      </c>
+      <c r="F23" s="3">
+        <v>4</v>
+      </c>
+      <c r="G23" s="3">
+        <v>4</v>
+      </c>
+      <c r="H23" s="3">
+        <v>4</v>
+      </c>
+      <c r="I23" s="3">
+        <v>4</v>
+      </c>
+      <c r="J23" s="3">
+        <v>4</v>
+      </c>
+      <c r="K23" s="3">
+        <v>4</v>
+      </c>
+      <c r="L23" s="3">
+        <v>4</v>
+      </c>
+      <c r="M23" s="3">
+        <v>4</v>
+      </c>
+      <c r="N23" s="3">
+        <v>4</v>
+      </c>
+      <c r="O23" s="3">
+        <v>4</v>
+      </c>
+      <c r="P23" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q23" s="3">
+        <v>4</v>
+      </c>
+      <c r="R23" s="3">
+        <v>4</v>
+      </c>
+      <c r="S23" s="3">
+        <v>4</v>
+      </c>
+      <c r="T23" s="3">
+        <v>4</v>
+      </c>
+      <c r="U23" s="3">
+        <v>4</v>
+      </c>
+      <c r="V23" s="3">
+        <v>4</v>
+      </c>
+      <c r="W23" s="3">
+        <v>4</v>
+      </c>
+      <c r="X23" s="3">
+        <v>4</v>
+      </c>
+      <c r="Y23" s="3">
+        <v>4</v>
+      </c>
+      <c r="Z23" s="3">
+        <v>4</v>
+      </c>
+      <c r="AA23" s="3">
+        <v>4</v>
+      </c>
+      <c r="AB23" s="3">
+        <v>4</v>
+      </c>
+      <c r="AC23" s="3">
+        <v>4</v>
+      </c>
+      <c r="AD23" s="3">
+        <v>4</v>
+      </c>
+      <c r="AE23" s="3">
+        <v>4</v>
+      </c>
+      <c r="AF23" s="3">
+        <v>4</v>
+      </c>
+      <c r="AG23" s="3">
+        <v>4</v>
+      </c>
+      <c r="AH23" s="3">
+        <v>4</v>
+      </c>
+      <c r="AI23" s="3">
+        <v>4</v>
+      </c>
+      <c r="AJ23" s="3">
+        <v>4</v>
+      </c>
+      <c r="AK23" s="3">
+        <v>4</v>
+      </c>
+      <c r="AL23" s="3">
+        <v>4</v>
+      </c>
+      <c r="AM23" s="3">
+        <v>4</v>
+      </c>
+      <c r="AN23" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="3">
+        <v>4</v>
+      </c>
+      <c r="B24" s="3">
+        <v>4</v>
+      </c>
+      <c r="C24" s="3">
+        <v>4</v>
+      </c>
+      <c r="D24" s="3">
+        <v>4</v>
+      </c>
+      <c r="E24" s="3">
+        <v>4</v>
+      </c>
+      <c r="F24" s="3">
+        <v>4</v>
+      </c>
+      <c r="G24" s="3">
+        <v>4</v>
+      </c>
+      <c r="H24" s="3">
+        <v>4</v>
+      </c>
+      <c r="I24" s="3">
+        <v>4</v>
+      </c>
+      <c r="J24" s="3">
+        <v>4</v>
+      </c>
+      <c r="K24" s="3">
+        <v>4</v>
+      </c>
+      <c r="L24" s="3">
+        <v>4</v>
+      </c>
+      <c r="M24" s="3">
+        <v>4</v>
+      </c>
+      <c r="N24" s="3">
+        <v>4</v>
+      </c>
+      <c r="O24" s="3">
+        <v>4</v>
+      </c>
+      <c r="P24" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q24" s="3">
+        <v>4</v>
+      </c>
+      <c r="R24" s="3">
+        <v>4</v>
+      </c>
+      <c r="S24" s="3">
+        <v>4</v>
+      </c>
+      <c r="T24" s="3">
+        <v>4</v>
+      </c>
+      <c r="U24" s="3">
+        <v>4</v>
+      </c>
+      <c r="V24" s="3">
+        <v>4</v>
+      </c>
+      <c r="W24" s="3">
+        <v>4</v>
+      </c>
+      <c r="X24" s="3">
+        <v>4</v>
+      </c>
+      <c r="Y24" s="3">
+        <v>4</v>
+      </c>
+      <c r="Z24" s="3">
+        <v>4</v>
+      </c>
+      <c r="AA24" s="3">
+        <v>4</v>
+      </c>
+      <c r="AB24" s="3">
+        <v>4</v>
+      </c>
+      <c r="AC24" s="3">
+        <v>4</v>
+      </c>
+      <c r="AD24" s="3">
+        <v>4</v>
+      </c>
+      <c r="AE24" s="3">
+        <v>4</v>
+      </c>
+      <c r="AF24" s="3">
+        <v>4</v>
+      </c>
+      <c r="AG24" s="3">
+        <v>4</v>
+      </c>
+      <c r="AH24" s="3">
+        <v>4</v>
+      </c>
+      <c r="AI24" s="3">
+        <v>4</v>
+      </c>
+      <c r="AJ24" s="3">
+        <v>4</v>
+      </c>
+      <c r="AK24" s="3">
+        <v>4</v>
+      </c>
+      <c r="AL24" s="3">
+        <v>4</v>
+      </c>
+      <c r="AM24" s="3">
+        <v>4</v>
+      </c>
+      <c r="AN24" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="3">
+        <v>4</v>
+      </c>
+      <c r="B25" s="3">
+        <v>4</v>
+      </c>
+      <c r="C25" s="3">
+        <v>4</v>
+      </c>
+      <c r="D25" s="3">
+        <v>4</v>
+      </c>
+      <c r="E25" s="3">
+        <v>4</v>
+      </c>
+      <c r="F25" s="3">
+        <v>4</v>
+      </c>
+      <c r="G25" s="3">
+        <v>4</v>
+      </c>
+      <c r="H25" s="3">
+        <v>4</v>
+      </c>
+      <c r="I25" s="3">
+        <v>4</v>
+      </c>
+      <c r="J25" s="3">
+        <v>4</v>
+      </c>
+      <c r="K25" s="3">
+        <v>4</v>
+      </c>
+      <c r="L25" s="3">
+        <v>4</v>
+      </c>
+      <c r="M25" s="3">
+        <v>4</v>
+      </c>
+      <c r="N25" s="3">
+        <v>4</v>
+      </c>
+      <c r="O25" s="3">
+        <v>4</v>
+      </c>
+      <c r="P25" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q25" s="3">
+        <v>4</v>
+      </c>
+      <c r="R25" s="3">
+        <v>4</v>
+      </c>
+      <c r="S25" s="3">
+        <v>4</v>
+      </c>
+      <c r="T25" s="3">
+        <v>4</v>
+      </c>
+      <c r="U25" s="3">
+        <v>4</v>
+      </c>
+      <c r="V25" s="3">
+        <v>4</v>
+      </c>
+      <c r="W25" s="3">
+        <v>4</v>
+      </c>
+      <c r="X25" s="3">
+        <v>4</v>
+      </c>
+      <c r="Y25" s="3">
+        <v>4</v>
+      </c>
+      <c r="Z25" s="3">
+        <v>4</v>
+      </c>
+      <c r="AA25" s="3">
+        <v>4</v>
+      </c>
+      <c r="AB25" s="3">
+        <v>4</v>
+      </c>
+      <c r="AC25" s="3">
+        <v>4</v>
+      </c>
+      <c r="AD25" s="3">
+        <v>4</v>
+      </c>
+      <c r="AE25" s="3">
+        <v>4</v>
+      </c>
+      <c r="AF25" s="3">
+        <v>4</v>
+      </c>
+      <c r="AG25" s="3">
+        <v>4</v>
+      </c>
+      <c r="AH25" s="3">
+        <v>4</v>
+      </c>
+      <c r="AI25" s="3">
+        <v>4</v>
+      </c>
+      <c r="AJ25" s="3">
+        <v>4</v>
+      </c>
+      <c r="AK25" s="3">
+        <v>4</v>
+      </c>
+      <c r="AL25" s="3">
+        <v>4</v>
+      </c>
+      <c r="AM25" s="3">
+        <v>4</v>
+      </c>
+      <c r="AN25" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="3">
+        <v>4</v>
+      </c>
+      <c r="B26" s="3">
+        <v>4</v>
+      </c>
+      <c r="C26" s="3">
+        <v>4</v>
+      </c>
+      <c r="D26" s="3">
+        <v>4</v>
+      </c>
+      <c r="E26" s="3">
+        <v>4</v>
+      </c>
+      <c r="F26" s="3">
+        <v>4</v>
+      </c>
+      <c r="G26" s="3">
+        <v>4</v>
+      </c>
+      <c r="H26" s="3">
+        <v>4</v>
+      </c>
+      <c r="I26" s="3">
+        <v>4</v>
+      </c>
+      <c r="J26" s="3">
+        <v>4</v>
+      </c>
+      <c r="K26" s="3">
+        <v>4</v>
+      </c>
+      <c r="L26" s="3">
+        <v>4</v>
+      </c>
+      <c r="M26" s="3">
+        <v>4</v>
+      </c>
+      <c r="N26" s="3">
+        <v>4</v>
+      </c>
+      <c r="O26" s="3">
+        <v>4</v>
+      </c>
+      <c r="P26" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q26" s="3">
+        <v>4</v>
+      </c>
+      <c r="R26" s="3">
+        <v>4</v>
+      </c>
+      <c r="S26" s="3">
+        <v>4</v>
+      </c>
+      <c r="T26" s="3">
+        <v>4</v>
+      </c>
+      <c r="U26" s="3">
+        <v>4</v>
+      </c>
+      <c r="V26" s="3">
+        <v>4</v>
+      </c>
+      <c r="W26" s="3">
+        <v>4</v>
+      </c>
+      <c r="X26" s="3">
+        <v>4</v>
+      </c>
+      <c r="Y26" s="3">
+        <v>4</v>
+      </c>
+      <c r="Z26" s="3">
+        <v>4</v>
+      </c>
+      <c r="AA26" s="3">
+        <v>4</v>
+      </c>
+      <c r="AB26" s="3">
+        <v>4</v>
+      </c>
+      <c r="AC26" s="3">
+        <v>4</v>
+      </c>
+      <c r="AD26" s="3">
+        <v>4</v>
+      </c>
+      <c r="AE26" s="3">
+        <v>4</v>
+      </c>
+      <c r="AF26" s="3">
+        <v>4</v>
+      </c>
+      <c r="AG26" s="3">
+        <v>4</v>
+      </c>
+      <c r="AH26" s="3">
+        <v>4</v>
+      </c>
+      <c r="AI26" s="3">
+        <v>4</v>
+      </c>
+      <c r="AJ26" s="3">
+        <v>4</v>
+      </c>
+      <c r="AK26" s="3">
+        <v>4</v>
+      </c>
+      <c r="AL26" s="3">
+        <v>4</v>
+      </c>
+      <c r="AM26" s="3">
+        <v>4</v>
+      </c>
+      <c r="AN26" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="3">
+        <v>4</v>
+      </c>
+      <c r="B27" s="3">
+        <v>4</v>
+      </c>
+      <c r="C27" s="3">
+        <v>4</v>
+      </c>
+      <c r="D27" s="3">
+        <v>4</v>
+      </c>
+      <c r="E27" s="3">
+        <v>4</v>
+      </c>
+      <c r="F27" s="3">
+        <v>4</v>
+      </c>
+      <c r="G27" s="3">
+        <v>4</v>
+      </c>
+      <c r="H27" s="3">
+        <v>4</v>
+      </c>
+      <c r="I27" s="3">
+        <v>4</v>
+      </c>
+      <c r="J27" s="3">
+        <v>4</v>
+      </c>
+      <c r="K27" s="3">
+        <v>4</v>
+      </c>
+      <c r="L27" s="3">
+        <v>4</v>
+      </c>
+      <c r="M27" s="3">
+        <v>4</v>
+      </c>
+      <c r="N27" s="3">
+        <v>4</v>
+      </c>
+      <c r="O27" s="3">
+        <v>4</v>
+      </c>
+      <c r="P27" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q27" s="3">
+        <v>4</v>
+      </c>
+      <c r="R27" s="3">
+        <v>4</v>
+      </c>
+      <c r="S27" s="3">
+        <v>4</v>
+      </c>
+      <c r="T27" s="3">
+        <v>4</v>
+      </c>
+      <c r="U27" s="3">
+        <v>4</v>
+      </c>
+      <c r="V27" s="3">
+        <v>4</v>
+      </c>
+      <c r="W27" s="3">
+        <v>4</v>
+      </c>
+      <c r="X27" s="3">
+        <v>4</v>
+      </c>
+      <c r="Y27" s="3">
+        <v>4</v>
+      </c>
+      <c r="Z27" s="3">
+        <v>4</v>
+      </c>
+      <c r="AA27" s="3">
+        <v>4</v>
+      </c>
+      <c r="AB27" s="3">
+        <v>4</v>
+      </c>
+      <c r="AC27" s="3">
+        <v>4</v>
+      </c>
+      <c r="AD27" s="3">
+        <v>4</v>
+      </c>
+      <c r="AE27" s="3">
+        <v>4</v>
+      </c>
+      <c r="AF27" s="3">
+        <v>4</v>
+      </c>
+      <c r="AG27" s="3">
+        <v>4</v>
+      </c>
+      <c r="AH27" s="3">
+        <v>4</v>
+      </c>
+      <c r="AI27" s="3">
+        <v>4</v>
+      </c>
+      <c r="AJ27" s="3">
+        <v>4</v>
+      </c>
+      <c r="AK27" s="3">
+        <v>4</v>
+      </c>
+      <c r="AL27" s="3">
+        <v>4</v>
+      </c>
+      <c r="AM27" s="3">
+        <v>4</v>
+      </c>
+      <c r="AN27" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="3">
+        <v>4</v>
+      </c>
+      <c r="B28" s="3">
+        <v>4</v>
+      </c>
+      <c r="C28" s="3">
+        <v>4</v>
+      </c>
+      <c r="D28" s="3">
+        <v>4</v>
+      </c>
+      <c r="E28" s="3">
+        <v>4</v>
+      </c>
+      <c r="F28" s="3">
+        <v>4</v>
+      </c>
+      <c r="G28" s="3">
+        <v>4</v>
+      </c>
+      <c r="H28" s="3">
+        <v>4</v>
+      </c>
+      <c r="I28" s="3">
+        <v>4</v>
+      </c>
+      <c r="J28" s="3">
+        <v>4</v>
+      </c>
+      <c r="K28" s="3">
+        <v>4</v>
+      </c>
+      <c r="L28" s="3">
+        <v>4</v>
+      </c>
+      <c r="M28" s="3">
+        <v>4</v>
+      </c>
+      <c r="N28" s="3">
+        <v>4</v>
+      </c>
+      <c r="O28" s="3">
+        <v>4</v>
+      </c>
+      <c r="P28" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q28" s="3">
+        <v>4</v>
+      </c>
+      <c r="R28" s="3">
+        <v>4</v>
+      </c>
+      <c r="S28" s="3">
+        <v>4</v>
+      </c>
+      <c r="T28" s="3">
+        <v>4</v>
+      </c>
+      <c r="U28" s="3">
+        <v>4</v>
+      </c>
+      <c r="V28" s="3">
+        <v>4</v>
+      </c>
+      <c r="W28" s="3">
+        <v>4</v>
+      </c>
+      <c r="X28" s="3">
+        <v>4</v>
+      </c>
+      <c r="Y28" s="3">
+        <v>4</v>
+      </c>
+      <c r="Z28" s="3">
+        <v>4</v>
+      </c>
+      <c r="AA28" s="3">
+        <v>4</v>
+      </c>
+      <c r="AB28" s="3">
+        <v>4</v>
+      </c>
+      <c r="AC28" s="3">
+        <v>4</v>
+      </c>
+      <c r="AD28" s="3">
+        <v>4</v>
+      </c>
+      <c r="AE28" s="3">
+        <v>4</v>
+      </c>
+      <c r="AF28" s="3">
+        <v>4</v>
+      </c>
+      <c r="AG28" s="3">
+        <v>4</v>
+      </c>
+      <c r="AH28" s="3">
+        <v>4</v>
+      </c>
+      <c r="AI28" s="3">
+        <v>4</v>
+      </c>
+      <c r="AJ28" s="3">
+        <v>4</v>
+      </c>
+      <c r="AK28" s="3">
+        <v>4</v>
+      </c>
+      <c r="AL28" s="3">
+        <v>4</v>
+      </c>
+      <c r="AM28" s="3">
+        <v>4</v>
+      </c>
+      <c r="AN28" s="3">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{593D7251-ED31-BA47-99DA-64FA455321D8}">
+  <dimension ref="A1:AN28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AR21" sqref="AR21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="40" width="3.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>40</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1">
+        <v>1</v>
+      </c>
+      <c r="I2" s="1">
+        <v>1</v>
+      </c>
+      <c r="J2" s="1">
+        <v>1</v>
+      </c>
+      <c r="K2" s="1">
+        <v>1</v>
+      </c>
+      <c r="L2" s="1">
+        <v>1</v>
+      </c>
+      <c r="M2" s="1">
+        <v>1</v>
+      </c>
+      <c r="N2" s="1">
+        <v>1</v>
+      </c>
+      <c r="O2" s="1">
+        <v>1</v>
+      </c>
+      <c r="P2" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>1</v>
+      </c>
+      <c r="R2" s="1">
+        <v>1</v>
+      </c>
+      <c r="S2" s="1">
+        <v>1</v>
+      </c>
+      <c r="T2" s="1">
+        <v>1</v>
+      </c>
+      <c r="U2" s="1">
+        <v>1</v>
+      </c>
+      <c r="V2" s="1">
+        <v>1</v>
+      </c>
+      <c r="W2" s="1">
+        <v>1</v>
+      </c>
+      <c r="X2" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AM2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1">
+        <v>1</v>
+      </c>
+      <c r="J3" s="1">
+        <v>1</v>
+      </c>
+      <c r="K3" s="1">
+        <v>1</v>
+      </c>
+      <c r="L3" s="1">
+        <v>1</v>
+      </c>
+      <c r="M3" s="1">
+        <v>1</v>
+      </c>
+      <c r="N3" s="1">
+        <v>1</v>
+      </c>
+      <c r="O3" s="1">
+        <v>1</v>
+      </c>
+      <c r="P3" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>1</v>
+      </c>
+      <c r="R3" s="1">
+        <v>1</v>
+      </c>
+      <c r="S3" s="1">
+        <v>1</v>
+      </c>
+      <c r="T3" s="1">
+        <v>1</v>
+      </c>
+      <c r="U3" s="1">
+        <v>1</v>
+      </c>
+      <c r="V3" s="1">
+        <v>1</v>
+      </c>
+      <c r="W3" s="1">
+        <v>1</v>
+      </c>
+      <c r="X3" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y3" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AM3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1</v>
+      </c>
+      <c r="I4" s="1">
+        <v>1</v>
+      </c>
+      <c r="J4" s="1">
+        <v>1</v>
+      </c>
+      <c r="K4" s="1">
+        <v>1</v>
+      </c>
+      <c r="L4" s="1">
+        <v>1</v>
+      </c>
+      <c r="M4" s="1">
+        <v>1</v>
+      </c>
+      <c r="N4" s="1">
+        <v>1</v>
+      </c>
+      <c r="O4" s="1">
+        <v>1</v>
+      </c>
+      <c r="P4" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>1</v>
+      </c>
+      <c r="R4" s="1">
+        <v>1</v>
+      </c>
+      <c r="S4" s="1">
+        <v>1</v>
+      </c>
+      <c r="T4" s="1">
+        <v>1</v>
+      </c>
+      <c r="U4" s="1">
+        <v>1</v>
+      </c>
+      <c r="V4" s="1">
+        <v>1</v>
+      </c>
+      <c r="W4" s="1">
+        <v>1</v>
+      </c>
+      <c r="X4" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y4" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AM4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="18">
+        <v>2</v>
+      </c>
+      <c r="B5" s="18">
+        <v>2</v>
+      </c>
+      <c r="C5" s="18">
+        <v>2</v>
+      </c>
+      <c r="D5" s="18">
+        <v>2</v>
+      </c>
+      <c r="E5" s="18">
+        <v>2</v>
+      </c>
+      <c r="F5" s="18">
+        <v>2</v>
+      </c>
+      <c r="G5" s="18">
+        <v>2</v>
+      </c>
+      <c r="H5" s="18">
+        <v>2</v>
+      </c>
+      <c r="I5" s="18">
+        <v>2</v>
+      </c>
+      <c r="J5" s="18">
+        <v>2</v>
+      </c>
+      <c r="K5" s="18">
+        <v>2</v>
+      </c>
+      <c r="L5" s="18">
+        <v>2</v>
+      </c>
+      <c r="M5" s="18">
+        <v>2</v>
+      </c>
+      <c r="N5" s="18">
+        <v>2</v>
+      </c>
+      <c r="O5" s="18">
+        <v>2</v>
+      </c>
+      <c r="P5" s="18">
+        <v>2</v>
+      </c>
+      <c r="Q5" s="18">
+        <v>2</v>
+      </c>
+      <c r="R5" s="18">
+        <v>2</v>
+      </c>
+      <c r="S5" s="18">
+        <v>2</v>
+      </c>
+      <c r="T5" s="18">
+        <v>2</v>
+      </c>
+      <c r="U5" s="18">
+        <v>2</v>
+      </c>
+      <c r="V5" s="18">
+        <v>2</v>
+      </c>
+      <c r="W5" s="18">
+        <v>2</v>
+      </c>
+      <c r="X5" s="18">
+        <v>2</v>
+      </c>
+      <c r="Y5" s="18">
+        <v>2</v>
+      </c>
+      <c r="Z5" s="18">
+        <v>2</v>
+      </c>
+      <c r="AA5" s="18">
+        <v>2</v>
+      </c>
+      <c r="AB5" s="18">
+        <v>2</v>
+      </c>
+      <c r="AC5" s="18">
+        <v>2</v>
+      </c>
+      <c r="AD5" s="18">
+        <v>2</v>
+      </c>
+      <c r="AE5" s="18">
+        <v>2</v>
+      </c>
+      <c r="AF5" s="18">
+        <v>2</v>
+      </c>
+      <c r="AG5" s="18">
+        <v>2</v>
+      </c>
+      <c r="AH5" s="18">
+        <v>2</v>
+      </c>
+      <c r="AI5" s="18">
+        <v>2</v>
+      </c>
+      <c r="AJ5" s="18">
+        <v>2</v>
+      </c>
+      <c r="AK5" s="18">
+        <v>2</v>
+      </c>
+      <c r="AL5" s="18">
+        <v>2</v>
+      </c>
+      <c r="AM5" s="18">
+        <v>2</v>
+      </c>
+      <c r="AN5" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="18">
+        <v>2</v>
+      </c>
+      <c r="B6" s="18">
+        <v>2</v>
+      </c>
+      <c r="C6" s="18">
+        <v>2</v>
+      </c>
+      <c r="D6" s="18">
+        <v>2</v>
+      </c>
+      <c r="E6" s="18">
+        <v>2</v>
+      </c>
+      <c r="F6" s="18">
+        <v>2</v>
+      </c>
+      <c r="G6" s="18">
+        <v>2</v>
+      </c>
+      <c r="H6" s="18">
+        <v>2</v>
+      </c>
+      <c r="I6" s="18">
+        <v>2</v>
+      </c>
+      <c r="J6" s="18">
+        <v>2</v>
+      </c>
+      <c r="K6" s="18">
+        <v>2</v>
+      </c>
+      <c r="L6" s="18">
+        <v>2</v>
+      </c>
+      <c r="M6" s="18">
+        <v>2</v>
+      </c>
+      <c r="N6" s="18">
+        <v>2</v>
+      </c>
+      <c r="O6" s="18">
+        <v>2</v>
+      </c>
+      <c r="P6" s="18">
+        <v>2</v>
+      </c>
+      <c r="Q6" s="18">
+        <v>2</v>
+      </c>
+      <c r="R6" s="18">
+        <v>2</v>
+      </c>
+      <c r="S6" s="18">
+        <v>2</v>
+      </c>
+      <c r="T6" s="18">
+        <v>2</v>
+      </c>
+      <c r="U6" s="18">
+        <v>2</v>
+      </c>
+      <c r="V6" s="18">
+        <v>2</v>
+      </c>
+      <c r="W6" s="18">
+        <v>2</v>
+      </c>
+      <c r="X6" s="18">
+        <v>2</v>
+      </c>
+      <c r="Y6" s="18">
+        <v>2</v>
+      </c>
+      <c r="Z6" s="18">
+        <v>2</v>
+      </c>
+      <c r="AA6" s="18">
+        <v>2</v>
+      </c>
+      <c r="AB6" s="18">
+        <v>2</v>
+      </c>
+      <c r="AC6" s="18">
+        <v>2</v>
+      </c>
+      <c r="AD6" s="18">
+        <v>2</v>
+      </c>
+      <c r="AE6" s="18">
+        <v>2</v>
+      </c>
+      <c r="AF6" s="18">
+        <v>2</v>
+      </c>
+      <c r="AG6" s="18">
+        <v>2</v>
+      </c>
+      <c r="AH6" s="18">
+        <v>2</v>
+      </c>
+      <c r="AI6" s="18">
+        <v>2</v>
+      </c>
+      <c r="AJ6" s="18">
+        <v>2</v>
+      </c>
+      <c r="AK6" s="18">
+        <v>2</v>
+      </c>
+      <c r="AL6" s="18">
+        <v>2</v>
+      </c>
+      <c r="AM6" s="18">
+        <v>2</v>
+      </c>
+      <c r="AN6" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="18">
+        <v>2</v>
+      </c>
+      <c r="B7" s="18">
+        <v>2</v>
+      </c>
+      <c r="C7" s="18">
+        <v>2</v>
+      </c>
+      <c r="D7" s="18">
+        <v>2</v>
+      </c>
+      <c r="E7" s="18">
+        <v>2</v>
+      </c>
+      <c r="F7" s="18">
+        <v>2</v>
+      </c>
+      <c r="G7" s="18">
+        <v>2</v>
+      </c>
+      <c r="H7" s="18">
+        <v>2</v>
+      </c>
+      <c r="I7" s="18">
+        <v>2</v>
+      </c>
+      <c r="J7" s="18">
+        <v>2</v>
+      </c>
+      <c r="K7" s="18">
+        <v>2</v>
+      </c>
+      <c r="L7" s="18">
+        <v>2</v>
+      </c>
+      <c r="M7" s="18">
+        <v>2</v>
+      </c>
+      <c r="N7" s="18">
+        <v>2</v>
+      </c>
+      <c r="O7" s="18">
+        <v>2</v>
+      </c>
+      <c r="P7" s="18">
+        <v>2</v>
+      </c>
+      <c r="Q7" s="18">
+        <v>2</v>
+      </c>
+      <c r="R7" s="18">
+        <v>2</v>
+      </c>
+      <c r="S7" s="18">
+        <v>2</v>
+      </c>
+      <c r="T7" s="18">
+        <v>2</v>
+      </c>
+      <c r="U7" s="18">
+        <v>2</v>
+      </c>
+      <c r="V7" s="18">
+        <v>2</v>
+      </c>
+      <c r="W7" s="18">
+        <v>2</v>
+      </c>
+      <c r="X7" s="18">
+        <v>2</v>
+      </c>
+      <c r="Y7" s="18">
+        <v>2</v>
+      </c>
+      <c r="Z7" s="18">
+        <v>2</v>
+      </c>
+      <c r="AA7" s="18">
+        <v>2</v>
+      </c>
+      <c r="AB7" s="18">
+        <v>2</v>
+      </c>
+      <c r="AC7" s="18">
+        <v>2</v>
+      </c>
+      <c r="AD7" s="18">
+        <v>2</v>
+      </c>
+      <c r="AE7" s="18">
+        <v>2</v>
+      </c>
+      <c r="AF7" s="18">
+        <v>2</v>
+      </c>
+      <c r="AG7" s="18">
+        <v>2</v>
+      </c>
+      <c r="AH7" s="18">
+        <v>2</v>
+      </c>
+      <c r="AI7" s="18">
+        <v>2</v>
+      </c>
+      <c r="AJ7" s="18">
+        <v>2</v>
+      </c>
+      <c r="AK7" s="18">
+        <v>2</v>
+      </c>
+      <c r="AL7" s="18">
+        <v>2</v>
+      </c>
+      <c r="AM7" s="18">
+        <v>2</v>
+      </c>
+      <c r="AN7" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="18">
+        <v>2</v>
+      </c>
+      <c r="B8" s="18">
+        <v>2</v>
+      </c>
+      <c r="C8" s="18">
+        <v>2</v>
+      </c>
+      <c r="D8" s="18">
+        <v>2</v>
+      </c>
+      <c r="E8" s="18">
+        <v>2</v>
+      </c>
+      <c r="F8" s="18">
+        <v>2</v>
+      </c>
+      <c r="G8" s="18">
+        <v>2</v>
+      </c>
+      <c r="H8" s="18">
+        <v>2</v>
+      </c>
+      <c r="I8" s="18">
+        <v>2</v>
+      </c>
+      <c r="J8" s="18">
+        <v>2</v>
+      </c>
+      <c r="K8" s="18">
+        <v>2</v>
+      </c>
+      <c r="L8" s="18">
+        <v>2</v>
+      </c>
+      <c r="M8" s="18">
+        <v>2</v>
+      </c>
+      <c r="N8" s="18">
+        <v>2</v>
+      </c>
+      <c r="O8" s="18">
+        <v>2</v>
+      </c>
+      <c r="P8" s="18">
+        <v>2</v>
+      </c>
+      <c r="Q8" s="18">
+        <v>2</v>
+      </c>
+      <c r="R8" s="18">
+        <v>2</v>
+      </c>
+      <c r="S8" s="18">
+        <v>2</v>
+      </c>
+      <c r="T8" s="18">
+        <v>2</v>
+      </c>
+      <c r="U8" s="18">
+        <v>2</v>
+      </c>
+      <c r="V8" s="18">
+        <v>2</v>
+      </c>
+      <c r="W8" s="18">
+        <v>2</v>
+      </c>
+      <c r="X8" s="18">
+        <v>2</v>
+      </c>
+      <c r="Y8" s="18">
+        <v>2</v>
+      </c>
+      <c r="Z8" s="18">
+        <v>2</v>
+      </c>
+      <c r="AA8" s="18">
+        <v>2</v>
+      </c>
+      <c r="AB8" s="18">
+        <v>2</v>
+      </c>
+      <c r="AC8" s="18">
+        <v>2</v>
+      </c>
+      <c r="AD8" s="18">
+        <v>2</v>
+      </c>
+      <c r="AE8" s="18">
+        <v>2</v>
+      </c>
+      <c r="AF8" s="18">
+        <v>2</v>
+      </c>
+      <c r="AG8" s="18">
+        <v>2</v>
+      </c>
+      <c r="AH8" s="18">
+        <v>2</v>
+      </c>
+      <c r="AI8" s="18">
+        <v>2</v>
+      </c>
+      <c r="AJ8" s="18">
+        <v>2</v>
+      </c>
+      <c r="AK8" s="18">
+        <v>2</v>
+      </c>
+      <c r="AL8" s="18">
+        <v>2</v>
+      </c>
+      <c r="AM8" s="18">
+        <v>2</v>
+      </c>
+      <c r="AN8" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="18">
+        <v>2</v>
+      </c>
+      <c r="B9" s="18">
+        <v>2</v>
+      </c>
+      <c r="C9" s="18">
+        <v>2</v>
+      </c>
+      <c r="D9" s="18">
+        <v>2</v>
+      </c>
+      <c r="E9" s="18">
+        <v>2</v>
+      </c>
+      <c r="F9" s="18">
+        <v>2</v>
+      </c>
+      <c r="G9" s="18">
+        <v>2</v>
+      </c>
+      <c r="H9" s="18">
+        <v>2</v>
+      </c>
+      <c r="I9" s="18">
+        <v>2</v>
+      </c>
+      <c r="J9" s="18">
+        <v>2</v>
+      </c>
+      <c r="K9" s="18">
+        <v>2</v>
+      </c>
+      <c r="L9" s="18">
+        <v>2</v>
+      </c>
+      <c r="M9" s="18">
+        <v>2</v>
+      </c>
+      <c r="N9" s="18">
+        <v>2</v>
+      </c>
+      <c r="O9" s="18">
+        <v>2</v>
+      </c>
+      <c r="P9" s="18">
+        <v>2</v>
+      </c>
+      <c r="Q9" s="18">
+        <v>2</v>
+      </c>
+      <c r="R9" s="18">
+        <v>2</v>
+      </c>
+      <c r="S9" s="18">
+        <v>2</v>
+      </c>
+      <c r="T9" s="18">
+        <v>2</v>
+      </c>
+      <c r="U9" s="18">
+        <v>2</v>
+      </c>
+      <c r="V9" s="18">
+        <v>2</v>
+      </c>
+      <c r="W9" s="18">
+        <v>2</v>
+      </c>
+      <c r="X9" s="18">
+        <v>2</v>
+      </c>
+      <c r="Y9" s="18">
+        <v>2</v>
+      </c>
+      <c r="Z9" s="18">
+        <v>2</v>
+      </c>
+      <c r="AA9" s="18">
+        <v>2</v>
+      </c>
+      <c r="AB9" s="18">
+        <v>2</v>
+      </c>
+      <c r="AC9" s="18">
+        <v>2</v>
+      </c>
+      <c r="AD9" s="18">
+        <v>2</v>
+      </c>
+      <c r="AE9" s="18">
+        <v>2</v>
+      </c>
+      <c r="AF9" s="18">
+        <v>2</v>
+      </c>
+      <c r="AG9" s="18">
+        <v>2</v>
+      </c>
+      <c r="AH9" s="18">
+        <v>2</v>
+      </c>
+      <c r="AI9" s="18">
+        <v>2</v>
+      </c>
+      <c r="AJ9" s="18">
+        <v>2</v>
+      </c>
+      <c r="AK9" s="18">
+        <v>2</v>
+      </c>
+      <c r="AL9" s="18">
+        <v>2</v>
+      </c>
+      <c r="AM9" s="18">
+        <v>2</v>
+      </c>
+      <c r="AN9" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="18">
+        <v>2</v>
+      </c>
+      <c r="B10" s="18">
+        <v>2</v>
+      </c>
+      <c r="C10" s="18">
+        <v>2</v>
+      </c>
+      <c r="D10" s="18">
+        <v>2</v>
+      </c>
+      <c r="E10" s="18">
+        <v>2</v>
+      </c>
+      <c r="F10" s="18">
+        <v>2</v>
+      </c>
+      <c r="G10" s="18">
+        <v>2</v>
+      </c>
+      <c r="H10" s="18">
+        <v>2</v>
+      </c>
+      <c r="I10" s="18">
+        <v>2</v>
+      </c>
+      <c r="J10" s="18">
+        <v>2</v>
+      </c>
+      <c r="K10" s="18">
+        <v>2</v>
+      </c>
+      <c r="L10" s="18">
+        <v>2</v>
+      </c>
+      <c r="M10" s="18">
+        <v>2</v>
+      </c>
+      <c r="N10" s="18">
+        <v>2</v>
+      </c>
+      <c r="O10" s="18">
+        <v>2</v>
+      </c>
+      <c r="P10" s="18">
+        <v>2</v>
+      </c>
+      <c r="Q10" s="18">
+        <v>2</v>
+      </c>
+      <c r="R10" s="18">
+        <v>2</v>
+      </c>
+      <c r="S10" s="18">
+        <v>2</v>
+      </c>
+      <c r="T10" s="18">
+        <v>2</v>
+      </c>
+      <c r="U10" s="18">
+        <v>2</v>
+      </c>
+      <c r="V10" s="18">
+        <v>2</v>
+      </c>
+      <c r="W10" s="18">
+        <v>2</v>
+      </c>
+      <c r="X10" s="18">
+        <v>2</v>
+      </c>
+      <c r="Y10" s="18">
+        <v>2</v>
+      </c>
+      <c r="Z10" s="18">
+        <v>2</v>
+      </c>
+      <c r="AA10" s="18">
+        <v>2</v>
+      </c>
+      <c r="AB10" s="18">
+        <v>2</v>
+      </c>
+      <c r="AC10" s="18">
+        <v>2</v>
+      </c>
+      <c r="AD10" s="18">
+        <v>2</v>
+      </c>
+      <c r="AE10" s="18">
+        <v>2</v>
+      </c>
+      <c r="AF10" s="18">
+        <v>2</v>
+      </c>
+      <c r="AG10" s="18">
+        <v>2</v>
+      </c>
+      <c r="AH10" s="18">
+        <v>2</v>
+      </c>
+      <c r="AI10" s="18">
+        <v>2</v>
+      </c>
+      <c r="AJ10" s="18">
+        <v>2</v>
+      </c>
+      <c r="AK10" s="18">
+        <v>2</v>
+      </c>
+      <c r="AL10" s="18">
+        <v>2</v>
+      </c>
+      <c r="AM10" s="18">
+        <v>2</v>
+      </c>
+      <c r="AN10" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="18">
+        <v>2</v>
+      </c>
+      <c r="B11" s="18">
+        <v>2</v>
+      </c>
+      <c r="C11" s="18">
+        <v>2</v>
+      </c>
+      <c r="D11" s="18">
+        <v>2</v>
+      </c>
+      <c r="E11" s="18">
+        <v>2</v>
+      </c>
+      <c r="F11" s="18">
+        <v>2</v>
+      </c>
+      <c r="G11" s="18">
+        <v>2</v>
+      </c>
+      <c r="H11" s="18">
+        <v>2</v>
+      </c>
+      <c r="I11" s="18">
+        <v>2</v>
+      </c>
+      <c r="J11" s="18">
+        <v>2</v>
+      </c>
+      <c r="K11" s="18">
+        <v>2</v>
+      </c>
+      <c r="L11" s="18">
+        <v>2</v>
+      </c>
+      <c r="M11" s="18">
+        <v>2</v>
+      </c>
+      <c r="N11" s="18">
+        <v>2</v>
+      </c>
+      <c r="O11" s="18">
+        <v>2</v>
+      </c>
+      <c r="P11" s="18">
+        <v>2</v>
+      </c>
+      <c r="Q11" s="18">
+        <v>2</v>
+      </c>
+      <c r="R11" s="18">
+        <v>2</v>
+      </c>
+      <c r="S11" s="18">
+        <v>2</v>
+      </c>
+      <c r="T11" s="18">
+        <v>2</v>
+      </c>
+      <c r="U11" s="18">
+        <v>2</v>
+      </c>
+      <c r="V11" s="18">
+        <v>2</v>
+      </c>
+      <c r="W11" s="18">
+        <v>2</v>
+      </c>
+      <c r="X11" s="18">
+        <v>2</v>
+      </c>
+      <c r="Y11" s="18">
+        <v>2</v>
+      </c>
+      <c r="Z11" s="18">
+        <v>2</v>
+      </c>
+      <c r="AA11" s="18">
+        <v>2</v>
+      </c>
+      <c r="AB11" s="18">
+        <v>2</v>
+      </c>
+      <c r="AC11" s="18">
+        <v>2</v>
+      </c>
+      <c r="AD11" s="18">
+        <v>2</v>
+      </c>
+      <c r="AE11" s="18">
+        <v>2</v>
+      </c>
+      <c r="AF11" s="18">
+        <v>2</v>
+      </c>
+      <c r="AG11" s="18">
+        <v>2</v>
+      </c>
+      <c r="AH11" s="18">
+        <v>2</v>
+      </c>
+      <c r="AI11" s="18">
+        <v>2</v>
+      </c>
+      <c r="AJ11" s="18">
+        <v>2</v>
+      </c>
+      <c r="AK11" s="18">
+        <v>2</v>
+      </c>
+      <c r="AL11" s="18">
+        <v>2</v>
+      </c>
+      <c r="AM11" s="18">
+        <v>2</v>
+      </c>
+      <c r="AN11" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="18">
+        <v>2</v>
+      </c>
+      <c r="B12" s="18">
+        <v>2</v>
+      </c>
+      <c r="C12" s="18">
+        <v>2</v>
+      </c>
+      <c r="D12" s="18">
+        <v>2</v>
+      </c>
+      <c r="E12" s="18">
+        <v>2</v>
+      </c>
+      <c r="F12" s="18">
+        <v>2</v>
+      </c>
+      <c r="G12" s="18">
+        <v>2</v>
+      </c>
+      <c r="H12" s="18">
+        <v>2</v>
+      </c>
+      <c r="I12" s="18">
+        <v>2</v>
+      </c>
+      <c r="J12" s="18">
+        <v>2</v>
+      </c>
+      <c r="K12" s="18">
+        <v>2</v>
+      </c>
+      <c r="L12" s="18">
+        <v>2</v>
+      </c>
+      <c r="M12" s="18">
+        <v>2</v>
+      </c>
+      <c r="N12" s="18">
+        <v>2</v>
+      </c>
+      <c r="O12" s="18">
+        <v>2</v>
+      </c>
+      <c r="P12" s="18">
+        <v>2</v>
+      </c>
+      <c r="Q12" s="18">
+        <v>2</v>
+      </c>
+      <c r="R12" s="18">
+        <v>2</v>
+      </c>
+      <c r="S12" s="18">
+        <v>2</v>
+      </c>
+      <c r="T12" s="18">
+        <v>2</v>
+      </c>
+      <c r="U12" s="18">
+        <v>2</v>
+      </c>
+      <c r="V12" s="18">
+        <v>2</v>
+      </c>
+      <c r="W12" s="18">
+        <v>2</v>
+      </c>
+      <c r="X12" s="18">
+        <v>2</v>
+      </c>
+      <c r="Y12" s="18">
+        <v>2</v>
+      </c>
+      <c r="Z12" s="18">
+        <v>2</v>
+      </c>
+      <c r="AA12" s="18">
+        <v>2</v>
+      </c>
+      <c r="AB12" s="18">
+        <v>2</v>
+      </c>
+      <c r="AC12" s="18">
+        <v>2</v>
+      </c>
+      <c r="AD12" s="18">
+        <v>2</v>
+      </c>
+      <c r="AE12" s="18">
+        <v>2</v>
+      </c>
+      <c r="AF12" s="18">
+        <v>2</v>
+      </c>
+      <c r="AG12" s="18">
+        <v>2</v>
+      </c>
+      <c r="AH12" s="18">
+        <v>2</v>
+      </c>
+      <c r="AI12" s="18">
+        <v>2</v>
+      </c>
+      <c r="AJ12" s="18">
+        <v>2</v>
+      </c>
+      <c r="AK12" s="18">
+        <v>2</v>
+      </c>
+      <c r="AL12" s="18">
+        <v>2</v>
+      </c>
+      <c r="AM12" s="18">
+        <v>2</v>
+      </c>
+      <c r="AN12" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>3</v>
+      </c>
+      <c r="B13" s="2">
+        <v>3</v>
+      </c>
+      <c r="C13" s="2">
+        <v>3</v>
+      </c>
+      <c r="D13" s="2">
+        <v>3</v>
+      </c>
+      <c r="E13" s="2">
+        <v>3</v>
+      </c>
+      <c r="F13" s="2">
+        <v>3</v>
+      </c>
+      <c r="G13" s="2">
+        <v>3</v>
+      </c>
+      <c r="H13" s="2">
+        <v>3</v>
+      </c>
+      <c r="I13" s="2">
+        <v>3</v>
+      </c>
+      <c r="J13" s="2">
+        <v>3</v>
+      </c>
+      <c r="K13" s="2">
+        <v>3</v>
+      </c>
+      <c r="L13" s="2">
+        <v>3</v>
+      </c>
+      <c r="M13" s="2">
+        <v>3</v>
+      </c>
+      <c r="N13" s="2">
+        <v>3</v>
+      </c>
+      <c r="O13" s="2">
+        <v>3</v>
+      </c>
+      <c r="P13" s="2">
+        <v>3</v>
+      </c>
+      <c r="Q13" s="2">
+        <v>3</v>
+      </c>
+      <c r="R13" s="2">
+        <v>3</v>
+      </c>
+      <c r="S13" s="2">
+        <v>3</v>
+      </c>
+      <c r="T13" s="2">
+        <v>3</v>
+      </c>
+      <c r="U13" s="2">
+        <v>3</v>
+      </c>
+      <c r="V13" s="2">
+        <v>3</v>
+      </c>
+      <c r="W13" s="2">
+        <v>3</v>
+      </c>
+      <c r="X13" s="2">
+        <v>3</v>
+      </c>
+      <c r="Y13" s="2">
+        <v>3</v>
+      </c>
+      <c r="Z13" s="2">
+        <v>3</v>
+      </c>
+      <c r="AA13" s="2">
+        <v>3</v>
+      </c>
+      <c r="AB13" s="2">
+        <v>3</v>
+      </c>
+      <c r="AC13" s="2">
+        <v>3</v>
+      </c>
+      <c r="AD13" s="2">
+        <v>3</v>
+      </c>
+      <c r="AE13" s="2">
+        <v>3</v>
+      </c>
+      <c r="AF13" s="2">
+        <v>3</v>
+      </c>
+      <c r="AG13" s="2">
+        <v>3</v>
+      </c>
+      <c r="AH13" s="2">
+        <v>3</v>
+      </c>
+      <c r="AI13" s="2">
+        <v>3</v>
+      </c>
+      <c r="AJ13" s="2">
+        <v>3</v>
+      </c>
+      <c r="AK13" s="2">
+        <v>3</v>
+      </c>
+      <c r="AL13" s="2">
+        <v>3</v>
+      </c>
+      <c r="AM13" s="2">
+        <v>3</v>
+      </c>
+      <c r="AN13" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>3</v>
+      </c>
+      <c r="B14" s="2">
+        <v>3</v>
+      </c>
+      <c r="C14" s="2">
+        <v>3</v>
+      </c>
+      <c r="D14" s="2">
+        <v>3</v>
+      </c>
+      <c r="E14" s="2">
+        <v>3</v>
+      </c>
+      <c r="F14" s="2">
+        <v>3</v>
+      </c>
+      <c r="G14" s="2">
+        <v>3</v>
+      </c>
+      <c r="H14" s="2">
+        <v>3</v>
+      </c>
+      <c r="I14" s="2">
+        <v>3</v>
+      </c>
+      <c r="J14" s="2">
+        <v>3</v>
+      </c>
+      <c r="K14" s="2">
+        <v>3</v>
+      </c>
+      <c r="L14" s="2">
+        <v>3</v>
+      </c>
+      <c r="M14" s="2">
+        <v>3</v>
+      </c>
+      <c r="N14" s="2">
+        <v>3</v>
+      </c>
+      <c r="O14" s="2">
+        <v>3</v>
+      </c>
+      <c r="P14" s="2">
+        <v>3</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>3</v>
+      </c>
+      <c r="R14" s="2">
+        <v>3</v>
+      </c>
+      <c r="S14" s="2">
+        <v>3</v>
+      </c>
+      <c r="T14" s="2">
+        <v>3</v>
+      </c>
+      <c r="U14" s="2">
+        <v>3</v>
+      </c>
+      <c r="V14" s="2">
+        <v>3</v>
+      </c>
+      <c r="W14" s="2">
+        <v>3</v>
+      </c>
+      <c r="X14" s="2">
+        <v>3</v>
+      </c>
+      <c r="Y14" s="2">
+        <v>3</v>
+      </c>
+      <c r="Z14" s="2">
+        <v>3</v>
+      </c>
+      <c r="AA14" s="2">
+        <v>3</v>
+      </c>
+      <c r="AB14" s="2">
+        <v>3</v>
+      </c>
+      <c r="AC14" s="2">
+        <v>3</v>
+      </c>
+      <c r="AD14" s="2">
+        <v>3</v>
+      </c>
+      <c r="AE14" s="2">
+        <v>3</v>
+      </c>
+      <c r="AF14" s="2">
+        <v>3</v>
+      </c>
+      <c r="AG14" s="2">
+        <v>3</v>
+      </c>
+      <c r="AH14" s="2">
+        <v>3</v>
+      </c>
+      <c r="AI14" s="2">
+        <v>3</v>
+      </c>
+      <c r="AJ14" s="2">
+        <v>3</v>
+      </c>
+      <c r="AK14" s="2">
+        <v>3</v>
+      </c>
+      <c r="AL14" s="2">
+        <v>3</v>
+      </c>
+      <c r="AM14" s="2">
+        <v>3</v>
+      </c>
+      <c r="AN14" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <v>3</v>
+      </c>
+      <c r="B15" s="2">
+        <v>3</v>
+      </c>
+      <c r="C15" s="2">
+        <v>3</v>
+      </c>
+      <c r="D15" s="2">
+        <v>3</v>
+      </c>
+      <c r="E15" s="2">
+        <v>3</v>
+      </c>
+      <c r="F15" s="2">
+        <v>3</v>
+      </c>
+      <c r="G15" s="2">
+        <v>3</v>
+      </c>
+      <c r="H15" s="2">
+        <v>3</v>
+      </c>
+      <c r="I15" s="2">
+        <v>3</v>
+      </c>
+      <c r="J15" s="2">
+        <v>3</v>
+      </c>
+      <c r="K15" s="2">
+        <v>3</v>
+      </c>
+      <c r="L15" s="2">
+        <v>3</v>
+      </c>
+      <c r="M15" s="2">
+        <v>3</v>
+      </c>
+      <c r="N15" s="2">
+        <v>3</v>
+      </c>
+      <c r="O15" s="2">
+        <v>3</v>
+      </c>
+      <c r="P15" s="2">
+        <v>3</v>
+      </c>
+      <c r="Q15" s="2">
+        <v>3</v>
+      </c>
+      <c r="R15" s="2">
+        <v>3</v>
+      </c>
+      <c r="S15" s="2">
+        <v>3</v>
+      </c>
+      <c r="T15" s="2">
+        <v>3</v>
+      </c>
+      <c r="U15" s="2">
+        <v>3</v>
+      </c>
+      <c r="V15" s="2">
+        <v>3</v>
+      </c>
+      <c r="W15" s="2">
+        <v>3</v>
+      </c>
+      <c r="X15" s="2">
+        <v>3</v>
+      </c>
+      <c r="Y15" s="2">
+        <v>3</v>
+      </c>
+      <c r="Z15" s="2">
+        <v>3</v>
+      </c>
+      <c r="AA15" s="2">
+        <v>3</v>
+      </c>
+      <c r="AB15" s="2">
+        <v>3</v>
+      </c>
+      <c r="AC15" s="2">
+        <v>3</v>
+      </c>
+      <c r="AD15" s="2">
+        <v>3</v>
+      </c>
+      <c r="AE15" s="2">
+        <v>3</v>
+      </c>
+      <c r="AF15" s="2">
+        <v>3</v>
+      </c>
+      <c r="AG15" s="2">
+        <v>3</v>
+      </c>
+      <c r="AH15" s="2">
+        <v>3</v>
+      </c>
+      <c r="AI15" s="2">
+        <v>3</v>
+      </c>
+      <c r="AJ15" s="2">
+        <v>3</v>
+      </c>
+      <c r="AK15" s="2">
+        <v>3</v>
+      </c>
+      <c r="AL15" s="2">
+        <v>3</v>
+      </c>
+      <c r="AM15" s="2">
+        <v>3</v>
+      </c>
+      <c r="AN15" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
+        <v>3</v>
+      </c>
+      <c r="B16" s="2">
+        <v>3</v>
+      </c>
+      <c r="C16" s="2">
+        <v>3</v>
+      </c>
+      <c r="D16" s="2">
+        <v>3</v>
+      </c>
+      <c r="E16" s="2">
+        <v>3</v>
+      </c>
+      <c r="F16" s="2">
+        <v>3</v>
+      </c>
+      <c r="G16" s="2">
+        <v>3</v>
+      </c>
+      <c r="H16" s="2">
+        <v>3</v>
+      </c>
+      <c r="I16" s="2">
+        <v>3</v>
+      </c>
+      <c r="J16" s="2">
+        <v>3</v>
+      </c>
+      <c r="K16" s="2">
+        <v>3</v>
+      </c>
+      <c r="L16" s="2">
+        <v>3</v>
+      </c>
+      <c r="M16" s="2">
+        <v>3</v>
+      </c>
+      <c r="N16" s="2">
+        <v>3</v>
+      </c>
+      <c r="O16" s="2">
+        <v>3</v>
+      </c>
+      <c r="P16" s="2">
+        <v>3</v>
+      </c>
+      <c r="Q16" s="2">
+        <v>3</v>
+      </c>
+      <c r="R16" s="2">
+        <v>3</v>
+      </c>
+      <c r="S16" s="2">
+        <v>3</v>
+      </c>
+      <c r="T16" s="2">
+        <v>3</v>
+      </c>
+      <c r="U16" s="2">
+        <v>3</v>
+      </c>
+      <c r="V16" s="2">
+        <v>3</v>
+      </c>
+      <c r="W16" s="2">
+        <v>3</v>
+      </c>
+      <c r="X16" s="2">
+        <v>3</v>
+      </c>
+      <c r="Y16" s="2">
+        <v>3</v>
+      </c>
+      <c r="Z16" s="2">
+        <v>3</v>
+      </c>
+      <c r="AA16" s="2">
+        <v>3</v>
+      </c>
+      <c r="AB16" s="2">
+        <v>3</v>
+      </c>
+      <c r="AC16" s="2">
+        <v>3</v>
+      </c>
+      <c r="AD16" s="2">
+        <v>3</v>
+      </c>
+      <c r="AE16" s="2">
+        <v>3</v>
+      </c>
+      <c r="AF16" s="2">
+        <v>3</v>
+      </c>
+      <c r="AG16" s="2">
+        <v>3</v>
+      </c>
+      <c r="AH16" s="2">
+        <v>3</v>
+      </c>
+      <c r="AI16" s="2">
+        <v>3</v>
+      </c>
+      <c r="AJ16" s="2">
+        <v>3</v>
+      </c>
+      <c r="AK16" s="2">
+        <v>3</v>
+      </c>
+      <c r="AL16" s="2">
+        <v>3</v>
+      </c>
+      <c r="AM16" s="2">
+        <v>3</v>
+      </c>
+      <c r="AN16" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <v>3</v>
+      </c>
+      <c r="B17" s="2">
+        <v>3</v>
+      </c>
+      <c r="C17" s="2">
+        <v>3</v>
+      </c>
+      <c r="D17" s="2">
+        <v>3</v>
+      </c>
+      <c r="E17" s="2">
+        <v>3</v>
+      </c>
+      <c r="F17" s="2">
+        <v>3</v>
+      </c>
+      <c r="G17" s="2">
+        <v>3</v>
+      </c>
+      <c r="H17" s="2">
+        <v>3</v>
+      </c>
+      <c r="I17" s="2">
+        <v>3</v>
+      </c>
+      <c r="J17" s="2">
+        <v>3</v>
+      </c>
+      <c r="K17" s="2">
+        <v>3</v>
+      </c>
+      <c r="L17" s="2">
+        <v>3</v>
+      </c>
+      <c r="M17" s="2">
+        <v>3</v>
+      </c>
+      <c r="N17" s="2">
+        <v>3</v>
+      </c>
+      <c r="O17" s="2">
+        <v>3</v>
+      </c>
+      <c r="P17" s="2">
+        <v>3</v>
+      </c>
+      <c r="Q17" s="2">
+        <v>3</v>
+      </c>
+      <c r="R17" s="2">
+        <v>3</v>
+      </c>
+      <c r="S17" s="2">
+        <v>3</v>
+      </c>
+      <c r="T17" s="2">
+        <v>3</v>
+      </c>
+      <c r="U17" s="2">
+        <v>3</v>
+      </c>
+      <c r="V17" s="2">
+        <v>3</v>
+      </c>
+      <c r="W17" s="2">
+        <v>3</v>
+      </c>
+      <c r="X17" s="2">
+        <v>3</v>
+      </c>
+      <c r="Y17" s="2">
+        <v>3</v>
+      </c>
+      <c r="Z17" s="2">
+        <v>3</v>
+      </c>
+      <c r="AA17" s="2">
+        <v>3</v>
+      </c>
+      <c r="AB17" s="2">
+        <v>3</v>
+      </c>
+      <c r="AC17" s="2">
+        <v>3</v>
+      </c>
+      <c r="AD17" s="2">
+        <v>3</v>
+      </c>
+      <c r="AE17" s="2">
+        <v>3</v>
+      </c>
+      <c r="AF17" s="2">
+        <v>3</v>
+      </c>
+      <c r="AG17" s="2">
+        <v>3</v>
+      </c>
+      <c r="AH17" s="2">
+        <v>3</v>
+      </c>
+      <c r="AI17" s="2">
+        <v>3</v>
+      </c>
+      <c r="AJ17" s="2">
+        <v>3</v>
+      </c>
+      <c r="AK17" s="2">
+        <v>3</v>
+      </c>
+      <c r="AL17" s="2">
+        <v>3</v>
+      </c>
+      <c r="AM17" s="2">
+        <v>3</v>
+      </c>
+      <c r="AN17" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <v>3</v>
+      </c>
+      <c r="B18" s="2">
+        <v>3</v>
+      </c>
+      <c r="C18" s="2">
+        <v>3</v>
+      </c>
+      <c r="D18" s="2">
+        <v>3</v>
+      </c>
+      <c r="E18" s="2">
+        <v>3</v>
+      </c>
+      <c r="F18" s="2">
+        <v>3</v>
+      </c>
+      <c r="G18" s="2">
+        <v>3</v>
+      </c>
+      <c r="H18" s="2">
+        <v>3</v>
+      </c>
+      <c r="I18" s="2">
+        <v>3</v>
+      </c>
+      <c r="J18" s="2">
+        <v>3</v>
+      </c>
+      <c r="K18" s="2">
+        <v>3</v>
+      </c>
+      <c r="L18" s="2">
+        <v>3</v>
+      </c>
+      <c r="M18" s="2">
+        <v>3</v>
+      </c>
+      <c r="N18" s="2">
+        <v>3</v>
+      </c>
+      <c r="O18" s="2">
+        <v>3</v>
+      </c>
+      <c r="P18" s="2">
+        <v>3</v>
+      </c>
+      <c r="Q18" s="2">
+        <v>3</v>
+      </c>
+      <c r="R18" s="2">
+        <v>3</v>
+      </c>
+      <c r="S18" s="2">
+        <v>3</v>
+      </c>
+      <c r="T18" s="2">
+        <v>3</v>
+      </c>
+      <c r="U18" s="2">
+        <v>3</v>
+      </c>
+      <c r="V18" s="2">
+        <v>3</v>
+      </c>
+      <c r="W18" s="2">
+        <v>3</v>
+      </c>
+      <c r="X18" s="2">
+        <v>3</v>
+      </c>
+      <c r="Y18" s="2">
+        <v>3</v>
+      </c>
+      <c r="Z18" s="2">
+        <v>3</v>
+      </c>
+      <c r="AA18" s="2">
+        <v>3</v>
+      </c>
+      <c r="AB18" s="2">
+        <v>3</v>
+      </c>
+      <c r="AC18" s="2">
+        <v>3</v>
+      </c>
+      <c r="AD18" s="2">
+        <v>3</v>
+      </c>
+      <c r="AE18" s="2">
+        <v>3</v>
+      </c>
+      <c r="AF18" s="2">
+        <v>3</v>
+      </c>
+      <c r="AG18" s="2">
+        <v>3</v>
+      </c>
+      <c r="AH18" s="2">
+        <v>3</v>
+      </c>
+      <c r="AI18" s="2">
+        <v>3</v>
+      </c>
+      <c r="AJ18" s="2">
+        <v>3</v>
+      </c>
+      <c r="AK18" s="2">
+        <v>3</v>
+      </c>
+      <c r="AL18" s="2">
+        <v>3</v>
+      </c>
+      <c r="AM18" s="2">
+        <v>3</v>
+      </c>
+      <c r="AN18" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
+        <v>3</v>
+      </c>
+      <c r="B19" s="2">
+        <v>3</v>
+      </c>
+      <c r="C19" s="2">
+        <v>3</v>
+      </c>
+      <c r="D19" s="2">
+        <v>3</v>
+      </c>
+      <c r="E19" s="2">
+        <v>3</v>
+      </c>
+      <c r="F19" s="2">
+        <v>3</v>
+      </c>
+      <c r="G19" s="2">
+        <v>3</v>
+      </c>
+      <c r="H19" s="2">
+        <v>3</v>
+      </c>
+      <c r="I19" s="2">
+        <v>3</v>
+      </c>
+      <c r="J19" s="2">
+        <v>3</v>
+      </c>
+      <c r="K19" s="2">
+        <v>3</v>
+      </c>
+      <c r="L19" s="2">
+        <v>3</v>
+      </c>
+      <c r="M19" s="2">
+        <v>3</v>
+      </c>
+      <c r="N19" s="2">
+        <v>3</v>
+      </c>
+      <c r="O19" s="2">
+        <v>3</v>
+      </c>
+      <c r="P19" s="2">
+        <v>3</v>
+      </c>
+      <c r="Q19" s="2">
+        <v>3</v>
+      </c>
+      <c r="R19" s="2">
+        <v>3</v>
+      </c>
+      <c r="S19" s="2">
+        <v>3</v>
+      </c>
+      <c r="T19" s="2">
+        <v>3</v>
+      </c>
+      <c r="U19" s="2">
+        <v>3</v>
+      </c>
+      <c r="V19" s="2">
+        <v>3</v>
+      </c>
+      <c r="W19" s="2">
+        <v>3</v>
+      </c>
+      <c r="X19" s="2">
+        <v>3</v>
+      </c>
+      <c r="Y19" s="2">
+        <v>3</v>
+      </c>
+      <c r="Z19" s="2">
+        <v>3</v>
+      </c>
+      <c r="AA19" s="2">
+        <v>3</v>
+      </c>
+      <c r="AB19" s="2">
+        <v>3</v>
+      </c>
+      <c r="AC19" s="2">
+        <v>3</v>
+      </c>
+      <c r="AD19" s="2">
+        <v>3</v>
+      </c>
+      <c r="AE19" s="2">
+        <v>3</v>
+      </c>
+      <c r="AF19" s="2">
+        <v>3</v>
+      </c>
+      <c r="AG19" s="2">
+        <v>3</v>
+      </c>
+      <c r="AH19" s="2">
+        <v>3</v>
+      </c>
+      <c r="AI19" s="2">
+        <v>3</v>
+      </c>
+      <c r="AJ19" s="2">
+        <v>3</v>
+      </c>
+      <c r="AK19" s="2">
+        <v>3</v>
+      </c>
+      <c r="AL19" s="2">
+        <v>3</v>
+      </c>
+      <c r="AM19" s="2">
+        <v>3</v>
+      </c>
+      <c r="AN19" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
+        <v>3</v>
+      </c>
+      <c r="B20" s="2">
+        <v>3</v>
+      </c>
+      <c r="C20" s="2">
+        <v>3</v>
+      </c>
+      <c r="D20" s="2">
+        <v>3</v>
+      </c>
+      <c r="E20" s="2">
+        <v>3</v>
+      </c>
+      <c r="F20" s="2">
+        <v>3</v>
+      </c>
+      <c r="G20" s="2">
+        <v>3</v>
+      </c>
+      <c r="H20" s="2">
+        <v>3</v>
+      </c>
+      <c r="I20" s="2">
+        <v>3</v>
+      </c>
+      <c r="J20" s="2">
+        <v>3</v>
+      </c>
+      <c r="K20" s="2">
+        <v>3</v>
+      </c>
+      <c r="L20" s="2">
+        <v>3</v>
+      </c>
+      <c r="M20" s="2">
+        <v>3</v>
+      </c>
+      <c r="N20" s="2">
+        <v>3</v>
+      </c>
+      <c r="O20" s="2">
+        <v>3</v>
+      </c>
+      <c r="P20" s="2">
+        <v>3</v>
+      </c>
+      <c r="Q20" s="2">
+        <v>3</v>
+      </c>
+      <c r="R20" s="2">
+        <v>3</v>
+      </c>
+      <c r="S20" s="2">
+        <v>3</v>
+      </c>
+      <c r="T20" s="2">
+        <v>3</v>
+      </c>
+      <c r="U20" s="2">
+        <v>3</v>
+      </c>
+      <c r="V20" s="2">
+        <v>3</v>
+      </c>
+      <c r="W20" s="2">
+        <v>3</v>
+      </c>
+      <c r="X20" s="2">
+        <v>3</v>
+      </c>
+      <c r="Y20" s="2">
+        <v>3</v>
+      </c>
+      <c r="Z20" s="2">
+        <v>3</v>
+      </c>
+      <c r="AA20" s="2">
+        <v>3</v>
+      </c>
+      <c r="AB20" s="2">
+        <v>3</v>
+      </c>
+      <c r="AC20" s="2">
+        <v>3</v>
+      </c>
+      <c r="AD20" s="2">
+        <v>3</v>
+      </c>
+      <c r="AE20" s="2">
+        <v>3</v>
+      </c>
+      <c r="AF20" s="2">
+        <v>3</v>
+      </c>
+      <c r="AG20" s="2">
+        <v>3</v>
+      </c>
+      <c r="AH20" s="2">
+        <v>3</v>
+      </c>
+      <c r="AI20" s="2">
+        <v>3</v>
+      </c>
+      <c r="AJ20" s="2">
+        <v>3</v>
+      </c>
+      <c r="AK20" s="2">
+        <v>3</v>
+      </c>
+      <c r="AL20" s="2">
+        <v>3</v>
+      </c>
+      <c r="AM20" s="2">
+        <v>3</v>
+      </c>
+      <c r="AN20" s="2">
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
update housing market and jobless claims charts
</commit_message>
<xml_diff>
--- a/layouts.xlsx
+++ b/layouts.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="370" documentId="8_{16FB9176-5700-CA44-8DDA-ADDCE61D2EC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B0BCBCB8-CE17-4645-AB83-5D440F45D4AB}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="1600" windowWidth="28040" windowHeight="18100" firstSheet="2" activeTab="17" xr2:uid="{7344E464-CEB7-A74D-A529-F1BDE3AF96EC}"/>
+    <workbookView xWindow="3900" yWindow="1600" windowWidth="28040" windowHeight="18100" activeTab="4" xr2:uid="{7344E464-CEB7-A74D-A529-F1BDE3AF96EC}"/>
   </bookViews>
   <sheets>
     <sheet name="lay-1" sheetId="2" r:id="rId1"/>
@@ -31411,7 +31411,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{593D7251-ED31-BA47-99DA-64FA455321D8}">
   <dimension ref="A1:AN28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AR21" sqref="AR21"/>
     </sheetView>
   </sheetViews>
@@ -34846,7 +34846,7 @@
   <dimension ref="A1:AN27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:AN27"/>
+      <selection activeCell="AN4" sqref="AN4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -44905,7 +44905,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E1D5664-FD82-904C-987A-24EAE06E9377}">
   <dimension ref="A1:AN27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="AP13" sqref="AP13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
new gdp chart for JW
</commit_message>
<xml_diff>
--- a/layouts.xlsx
+++ b/layouts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/046b73b793af0aea/PAMGMT/projects/tamarac/economic-market-commentary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="370" documentId="8_{16FB9176-5700-CA44-8DDA-ADDCE61D2EC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B0BCBCB8-CE17-4645-AB83-5D440F45D4AB}"/>
+  <xr:revisionPtr revIDLastSave="378" documentId="8_{16FB9176-5700-CA44-8DDA-ADDCE61D2EC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DA0E3993-952E-9E4A-9D95-38EA3D69AC82}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="1600" windowWidth="28040" windowHeight="18100" activeTab="4" xr2:uid="{7344E464-CEB7-A74D-A529-F1BDE3AF96EC}"/>
+    <workbookView xWindow="3900" yWindow="1600" windowWidth="28040" windowHeight="18100" firstSheet="3" activeTab="18" xr2:uid="{7344E464-CEB7-A74D-A529-F1BDE3AF96EC}"/>
   </bookViews>
   <sheets>
     <sheet name="lay-1" sheetId="2" r:id="rId1"/>
@@ -31,6 +31,7 @@
     <sheet name="lay-16" sheetId="18" r:id="rId16"/>
     <sheet name="lay-17" sheetId="19" r:id="rId17"/>
     <sheet name="lay-18" sheetId="20" r:id="rId18"/>
+    <sheet name="lay-19" sheetId="21" r:id="rId19"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -50,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="41">
   <si>
     <t>a</t>
   </si>
@@ -34841,6 +34842,3440 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50B44203-84DE-C949-99C4-30E10F45EAA1}">
+  <dimension ref="A1:AN28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AN17" sqref="A16:AN17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="40" width="3.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>40</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1">
+        <v>1</v>
+      </c>
+      <c r="I2" s="1">
+        <v>1</v>
+      </c>
+      <c r="J2" s="1">
+        <v>1</v>
+      </c>
+      <c r="K2" s="1">
+        <v>1</v>
+      </c>
+      <c r="L2" s="1">
+        <v>1</v>
+      </c>
+      <c r="M2" s="1">
+        <v>1</v>
+      </c>
+      <c r="N2" s="1">
+        <v>1</v>
+      </c>
+      <c r="O2" s="1">
+        <v>1</v>
+      </c>
+      <c r="P2" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>1</v>
+      </c>
+      <c r="R2" s="1">
+        <v>1</v>
+      </c>
+      <c r="S2" s="1">
+        <v>1</v>
+      </c>
+      <c r="T2" s="1">
+        <v>1</v>
+      </c>
+      <c r="U2" s="1">
+        <v>1</v>
+      </c>
+      <c r="V2" s="1">
+        <v>1</v>
+      </c>
+      <c r="W2" s="1">
+        <v>1</v>
+      </c>
+      <c r="X2" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AM2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1">
+        <v>1</v>
+      </c>
+      <c r="J3" s="1">
+        <v>1</v>
+      </c>
+      <c r="K3" s="1">
+        <v>1</v>
+      </c>
+      <c r="L3" s="1">
+        <v>1</v>
+      </c>
+      <c r="M3" s="1">
+        <v>1</v>
+      </c>
+      <c r="N3" s="1">
+        <v>1</v>
+      </c>
+      <c r="O3" s="1">
+        <v>1</v>
+      </c>
+      <c r="P3" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>1</v>
+      </c>
+      <c r="R3" s="1">
+        <v>1</v>
+      </c>
+      <c r="S3" s="1">
+        <v>1</v>
+      </c>
+      <c r="T3" s="1">
+        <v>1</v>
+      </c>
+      <c r="U3" s="1">
+        <v>1</v>
+      </c>
+      <c r="V3" s="1">
+        <v>1</v>
+      </c>
+      <c r="W3" s="1">
+        <v>1</v>
+      </c>
+      <c r="X3" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y3" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AM3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1</v>
+      </c>
+      <c r="I4" s="1">
+        <v>1</v>
+      </c>
+      <c r="J4" s="1">
+        <v>1</v>
+      </c>
+      <c r="K4" s="1">
+        <v>1</v>
+      </c>
+      <c r="L4" s="1">
+        <v>1</v>
+      </c>
+      <c r="M4" s="1">
+        <v>1</v>
+      </c>
+      <c r="N4" s="1">
+        <v>1</v>
+      </c>
+      <c r="O4" s="1">
+        <v>1</v>
+      </c>
+      <c r="P4" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>1</v>
+      </c>
+      <c r="R4" s="1">
+        <v>1</v>
+      </c>
+      <c r="S4" s="1">
+        <v>1</v>
+      </c>
+      <c r="T4" s="1">
+        <v>1</v>
+      </c>
+      <c r="U4" s="1">
+        <v>1</v>
+      </c>
+      <c r="V4" s="1">
+        <v>1</v>
+      </c>
+      <c r="W4" s="1">
+        <v>1</v>
+      </c>
+      <c r="X4" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y4" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AM4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2">
+        <v>2</v>
+      </c>
+      <c r="C5" s="2">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2">
+        <v>2</v>
+      </c>
+      <c r="E5" s="2">
+        <v>2</v>
+      </c>
+      <c r="F5" s="2">
+        <v>2</v>
+      </c>
+      <c r="G5" s="2">
+        <v>2</v>
+      </c>
+      <c r="H5" s="2">
+        <v>2</v>
+      </c>
+      <c r="I5" s="2">
+        <v>2</v>
+      </c>
+      <c r="J5" s="2">
+        <v>2</v>
+      </c>
+      <c r="K5" s="2">
+        <v>2</v>
+      </c>
+      <c r="L5" s="2">
+        <v>2</v>
+      </c>
+      <c r="M5" s="2">
+        <v>2</v>
+      </c>
+      <c r="N5" s="2">
+        <v>2</v>
+      </c>
+      <c r="O5" s="2">
+        <v>2</v>
+      </c>
+      <c r="P5" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>2</v>
+      </c>
+      <c r="R5" s="2">
+        <v>2</v>
+      </c>
+      <c r="S5" s="2">
+        <v>2</v>
+      </c>
+      <c r="T5" s="2">
+        <v>2</v>
+      </c>
+      <c r="U5" s="2">
+        <v>2</v>
+      </c>
+      <c r="V5" s="2">
+        <v>2</v>
+      </c>
+      <c r="W5" s="2">
+        <v>2</v>
+      </c>
+      <c r="X5" s="2">
+        <v>2</v>
+      </c>
+      <c r="Y5" s="2">
+        <v>2</v>
+      </c>
+      <c r="Z5" s="2">
+        <v>2</v>
+      </c>
+      <c r="AA5" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB5" s="2">
+        <v>2</v>
+      </c>
+      <c r="AC5" s="2">
+        <v>2</v>
+      </c>
+      <c r="AD5" s="2">
+        <v>2</v>
+      </c>
+      <c r="AE5" s="2">
+        <v>2</v>
+      </c>
+      <c r="AF5" s="2">
+        <v>2</v>
+      </c>
+      <c r="AG5" s="2">
+        <v>2</v>
+      </c>
+      <c r="AH5" s="2">
+        <v>2</v>
+      </c>
+      <c r="AI5" s="2">
+        <v>2</v>
+      </c>
+      <c r="AJ5" s="2">
+        <v>2</v>
+      </c>
+      <c r="AK5" s="2">
+        <v>2</v>
+      </c>
+      <c r="AL5" s="2">
+        <v>2</v>
+      </c>
+      <c r="AM5" s="2">
+        <v>2</v>
+      </c>
+      <c r="AN5" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>2</v>
+      </c>
+      <c r="B6" s="2">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2">
+        <v>2</v>
+      </c>
+      <c r="D6" s="2">
+        <v>2</v>
+      </c>
+      <c r="E6" s="2">
+        <v>2</v>
+      </c>
+      <c r="F6" s="2">
+        <v>2</v>
+      </c>
+      <c r="G6" s="2">
+        <v>2</v>
+      </c>
+      <c r="H6" s="2">
+        <v>2</v>
+      </c>
+      <c r="I6" s="2">
+        <v>2</v>
+      </c>
+      <c r="J6" s="2">
+        <v>2</v>
+      </c>
+      <c r="K6" s="2">
+        <v>2</v>
+      </c>
+      <c r="L6" s="2">
+        <v>2</v>
+      </c>
+      <c r="M6" s="2">
+        <v>2</v>
+      </c>
+      <c r="N6" s="2">
+        <v>2</v>
+      </c>
+      <c r="O6" s="2">
+        <v>2</v>
+      </c>
+      <c r="P6" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>2</v>
+      </c>
+      <c r="R6" s="2">
+        <v>2</v>
+      </c>
+      <c r="S6" s="2">
+        <v>2</v>
+      </c>
+      <c r="T6" s="2">
+        <v>2</v>
+      </c>
+      <c r="U6" s="2">
+        <v>2</v>
+      </c>
+      <c r="V6" s="2">
+        <v>2</v>
+      </c>
+      <c r="W6" s="2">
+        <v>2</v>
+      </c>
+      <c r="X6" s="2">
+        <v>2</v>
+      </c>
+      <c r="Y6" s="2">
+        <v>2</v>
+      </c>
+      <c r="Z6" s="2">
+        <v>2</v>
+      </c>
+      <c r="AA6" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB6" s="2">
+        <v>2</v>
+      </c>
+      <c r="AC6" s="2">
+        <v>2</v>
+      </c>
+      <c r="AD6" s="2">
+        <v>2</v>
+      </c>
+      <c r="AE6" s="2">
+        <v>2</v>
+      </c>
+      <c r="AF6" s="2">
+        <v>2</v>
+      </c>
+      <c r="AG6" s="2">
+        <v>2</v>
+      </c>
+      <c r="AH6" s="2">
+        <v>2</v>
+      </c>
+      <c r="AI6" s="2">
+        <v>2</v>
+      </c>
+      <c r="AJ6" s="2">
+        <v>2</v>
+      </c>
+      <c r="AK6" s="2">
+        <v>2</v>
+      </c>
+      <c r="AL6" s="2">
+        <v>2</v>
+      </c>
+      <c r="AM6" s="2">
+        <v>2</v>
+      </c>
+      <c r="AN6" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>2</v>
+      </c>
+      <c r="B7" s="2">
+        <v>2</v>
+      </c>
+      <c r="C7" s="2">
+        <v>2</v>
+      </c>
+      <c r="D7" s="2">
+        <v>2</v>
+      </c>
+      <c r="E7" s="2">
+        <v>2</v>
+      </c>
+      <c r="F7" s="2">
+        <v>2</v>
+      </c>
+      <c r="G7" s="2">
+        <v>2</v>
+      </c>
+      <c r="H7" s="2">
+        <v>2</v>
+      </c>
+      <c r="I7" s="2">
+        <v>2</v>
+      </c>
+      <c r="J7" s="2">
+        <v>2</v>
+      </c>
+      <c r="K7" s="2">
+        <v>2</v>
+      </c>
+      <c r="L7" s="2">
+        <v>2</v>
+      </c>
+      <c r="M7" s="2">
+        <v>2</v>
+      </c>
+      <c r="N7" s="2">
+        <v>2</v>
+      </c>
+      <c r="O7" s="2">
+        <v>2</v>
+      </c>
+      <c r="P7" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>2</v>
+      </c>
+      <c r="R7" s="2">
+        <v>2</v>
+      </c>
+      <c r="S7" s="2">
+        <v>2</v>
+      </c>
+      <c r="T7" s="2">
+        <v>2</v>
+      </c>
+      <c r="U7" s="2">
+        <v>2</v>
+      </c>
+      <c r="V7" s="2">
+        <v>2</v>
+      </c>
+      <c r="W7" s="2">
+        <v>2</v>
+      </c>
+      <c r="X7" s="2">
+        <v>2</v>
+      </c>
+      <c r="Y7" s="2">
+        <v>2</v>
+      </c>
+      <c r="Z7" s="2">
+        <v>2</v>
+      </c>
+      <c r="AA7" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB7" s="2">
+        <v>2</v>
+      </c>
+      <c r="AC7" s="2">
+        <v>2</v>
+      </c>
+      <c r="AD7" s="2">
+        <v>2</v>
+      </c>
+      <c r="AE7" s="2">
+        <v>2</v>
+      </c>
+      <c r="AF7" s="2">
+        <v>2</v>
+      </c>
+      <c r="AG7" s="2">
+        <v>2</v>
+      </c>
+      <c r="AH7" s="2">
+        <v>2</v>
+      </c>
+      <c r="AI7" s="2">
+        <v>2</v>
+      </c>
+      <c r="AJ7" s="2">
+        <v>2</v>
+      </c>
+      <c r="AK7" s="2">
+        <v>2</v>
+      </c>
+      <c r="AL7" s="2">
+        <v>2</v>
+      </c>
+      <c r="AM7" s="2">
+        <v>2</v>
+      </c>
+      <c r="AN7" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>2</v>
+      </c>
+      <c r="B8" s="2">
+        <v>2</v>
+      </c>
+      <c r="C8" s="2">
+        <v>2</v>
+      </c>
+      <c r="D8" s="2">
+        <v>2</v>
+      </c>
+      <c r="E8" s="2">
+        <v>2</v>
+      </c>
+      <c r="F8" s="2">
+        <v>2</v>
+      </c>
+      <c r="G8" s="2">
+        <v>2</v>
+      </c>
+      <c r="H8" s="2">
+        <v>2</v>
+      </c>
+      <c r="I8" s="2">
+        <v>2</v>
+      </c>
+      <c r="J8" s="2">
+        <v>2</v>
+      </c>
+      <c r="K8" s="2">
+        <v>2</v>
+      </c>
+      <c r="L8" s="2">
+        <v>2</v>
+      </c>
+      <c r="M8" s="2">
+        <v>2</v>
+      </c>
+      <c r="N8" s="2">
+        <v>2</v>
+      </c>
+      <c r="O8" s="2">
+        <v>2</v>
+      </c>
+      <c r="P8" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>2</v>
+      </c>
+      <c r="R8" s="2">
+        <v>2</v>
+      </c>
+      <c r="S8" s="2">
+        <v>2</v>
+      </c>
+      <c r="T8" s="2">
+        <v>2</v>
+      </c>
+      <c r="U8" s="2">
+        <v>2</v>
+      </c>
+      <c r="V8" s="2">
+        <v>2</v>
+      </c>
+      <c r="W8" s="2">
+        <v>2</v>
+      </c>
+      <c r="X8" s="2">
+        <v>2</v>
+      </c>
+      <c r="Y8" s="2">
+        <v>2</v>
+      </c>
+      <c r="Z8" s="2">
+        <v>2</v>
+      </c>
+      <c r="AA8" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB8" s="2">
+        <v>2</v>
+      </c>
+      <c r="AC8" s="2">
+        <v>2</v>
+      </c>
+      <c r="AD8" s="2">
+        <v>2</v>
+      </c>
+      <c r="AE8" s="2">
+        <v>2</v>
+      </c>
+      <c r="AF8" s="2">
+        <v>2</v>
+      </c>
+      <c r="AG8" s="2">
+        <v>2</v>
+      </c>
+      <c r="AH8" s="2">
+        <v>2</v>
+      </c>
+      <c r="AI8" s="2">
+        <v>2</v>
+      </c>
+      <c r="AJ8" s="2">
+        <v>2</v>
+      </c>
+      <c r="AK8" s="2">
+        <v>2</v>
+      </c>
+      <c r="AL8" s="2">
+        <v>2</v>
+      </c>
+      <c r="AM8" s="2">
+        <v>2</v>
+      </c>
+      <c r="AN8" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>2</v>
+      </c>
+      <c r="B9" s="2">
+        <v>2</v>
+      </c>
+      <c r="C9" s="2">
+        <v>2</v>
+      </c>
+      <c r="D9" s="2">
+        <v>2</v>
+      </c>
+      <c r="E9" s="2">
+        <v>2</v>
+      </c>
+      <c r="F9" s="2">
+        <v>2</v>
+      </c>
+      <c r="G9" s="2">
+        <v>2</v>
+      </c>
+      <c r="H9" s="2">
+        <v>2</v>
+      </c>
+      <c r="I9" s="2">
+        <v>2</v>
+      </c>
+      <c r="J9" s="2">
+        <v>2</v>
+      </c>
+      <c r="K9" s="2">
+        <v>2</v>
+      </c>
+      <c r="L9" s="2">
+        <v>2</v>
+      </c>
+      <c r="M9" s="2">
+        <v>2</v>
+      </c>
+      <c r="N9" s="2">
+        <v>2</v>
+      </c>
+      <c r="O9" s="2">
+        <v>2</v>
+      </c>
+      <c r="P9" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>2</v>
+      </c>
+      <c r="R9" s="2">
+        <v>2</v>
+      </c>
+      <c r="S9" s="2">
+        <v>2</v>
+      </c>
+      <c r="T9" s="2">
+        <v>2</v>
+      </c>
+      <c r="U9" s="2">
+        <v>2</v>
+      </c>
+      <c r="V9" s="2">
+        <v>2</v>
+      </c>
+      <c r="W9" s="2">
+        <v>2</v>
+      </c>
+      <c r="X9" s="2">
+        <v>2</v>
+      </c>
+      <c r="Y9" s="2">
+        <v>2</v>
+      </c>
+      <c r="Z9" s="2">
+        <v>2</v>
+      </c>
+      <c r="AA9" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB9" s="2">
+        <v>2</v>
+      </c>
+      <c r="AC9" s="2">
+        <v>2</v>
+      </c>
+      <c r="AD9" s="2">
+        <v>2</v>
+      </c>
+      <c r="AE9" s="2">
+        <v>2</v>
+      </c>
+      <c r="AF9" s="2">
+        <v>2</v>
+      </c>
+      <c r="AG9" s="2">
+        <v>2</v>
+      </c>
+      <c r="AH9" s="2">
+        <v>2</v>
+      </c>
+      <c r="AI9" s="2">
+        <v>2</v>
+      </c>
+      <c r="AJ9" s="2">
+        <v>2</v>
+      </c>
+      <c r="AK9" s="2">
+        <v>2</v>
+      </c>
+      <c r="AL9" s="2">
+        <v>2</v>
+      </c>
+      <c r="AM9" s="2">
+        <v>2</v>
+      </c>
+      <c r="AN9" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>2</v>
+      </c>
+      <c r="B10" s="2">
+        <v>2</v>
+      </c>
+      <c r="C10" s="2">
+        <v>2</v>
+      </c>
+      <c r="D10" s="2">
+        <v>2</v>
+      </c>
+      <c r="E10" s="2">
+        <v>2</v>
+      </c>
+      <c r="F10" s="2">
+        <v>2</v>
+      </c>
+      <c r="G10" s="2">
+        <v>2</v>
+      </c>
+      <c r="H10" s="2">
+        <v>2</v>
+      </c>
+      <c r="I10" s="2">
+        <v>2</v>
+      </c>
+      <c r="J10" s="2">
+        <v>2</v>
+      </c>
+      <c r="K10" s="2">
+        <v>2</v>
+      </c>
+      <c r="L10" s="2">
+        <v>2</v>
+      </c>
+      <c r="M10" s="2">
+        <v>2</v>
+      </c>
+      <c r="N10" s="2">
+        <v>2</v>
+      </c>
+      <c r="O10" s="2">
+        <v>2</v>
+      </c>
+      <c r="P10" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>2</v>
+      </c>
+      <c r="R10" s="2">
+        <v>2</v>
+      </c>
+      <c r="S10" s="2">
+        <v>2</v>
+      </c>
+      <c r="T10" s="2">
+        <v>2</v>
+      </c>
+      <c r="U10" s="2">
+        <v>2</v>
+      </c>
+      <c r="V10" s="2">
+        <v>2</v>
+      </c>
+      <c r="W10" s="2">
+        <v>2</v>
+      </c>
+      <c r="X10" s="2">
+        <v>2</v>
+      </c>
+      <c r="Y10" s="2">
+        <v>2</v>
+      </c>
+      <c r="Z10" s="2">
+        <v>2</v>
+      </c>
+      <c r="AA10" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB10" s="2">
+        <v>2</v>
+      </c>
+      <c r="AC10" s="2">
+        <v>2</v>
+      </c>
+      <c r="AD10" s="2">
+        <v>2</v>
+      </c>
+      <c r="AE10" s="2">
+        <v>2</v>
+      </c>
+      <c r="AF10" s="2">
+        <v>2</v>
+      </c>
+      <c r="AG10" s="2">
+        <v>2</v>
+      </c>
+      <c r="AH10" s="2">
+        <v>2</v>
+      </c>
+      <c r="AI10" s="2">
+        <v>2</v>
+      </c>
+      <c r="AJ10" s="2">
+        <v>2</v>
+      </c>
+      <c r="AK10" s="2">
+        <v>2</v>
+      </c>
+      <c r="AL10" s="2">
+        <v>2</v>
+      </c>
+      <c r="AM10" s="2">
+        <v>2</v>
+      </c>
+      <c r="AN10" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>2</v>
+      </c>
+      <c r="B11" s="2">
+        <v>2</v>
+      </c>
+      <c r="C11" s="2">
+        <v>2</v>
+      </c>
+      <c r="D11" s="2">
+        <v>2</v>
+      </c>
+      <c r="E11" s="2">
+        <v>2</v>
+      </c>
+      <c r="F11" s="2">
+        <v>2</v>
+      </c>
+      <c r="G11" s="2">
+        <v>2</v>
+      </c>
+      <c r="H11" s="2">
+        <v>2</v>
+      </c>
+      <c r="I11" s="2">
+        <v>2</v>
+      </c>
+      <c r="J11" s="2">
+        <v>2</v>
+      </c>
+      <c r="K11" s="2">
+        <v>2</v>
+      </c>
+      <c r="L11" s="2">
+        <v>2</v>
+      </c>
+      <c r="M11" s="2">
+        <v>2</v>
+      </c>
+      <c r="N11" s="2">
+        <v>2</v>
+      </c>
+      <c r="O11" s="2">
+        <v>2</v>
+      </c>
+      <c r="P11" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>2</v>
+      </c>
+      <c r="R11" s="2">
+        <v>2</v>
+      </c>
+      <c r="S11" s="2">
+        <v>2</v>
+      </c>
+      <c r="T11" s="2">
+        <v>2</v>
+      </c>
+      <c r="U11" s="2">
+        <v>2</v>
+      </c>
+      <c r="V11" s="2">
+        <v>2</v>
+      </c>
+      <c r="W11" s="2">
+        <v>2</v>
+      </c>
+      <c r="X11" s="2">
+        <v>2</v>
+      </c>
+      <c r="Y11" s="2">
+        <v>2</v>
+      </c>
+      <c r="Z11" s="2">
+        <v>2</v>
+      </c>
+      <c r="AA11" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB11" s="2">
+        <v>2</v>
+      </c>
+      <c r="AC11" s="2">
+        <v>2</v>
+      </c>
+      <c r="AD11" s="2">
+        <v>2</v>
+      </c>
+      <c r="AE11" s="2">
+        <v>2</v>
+      </c>
+      <c r="AF11" s="2">
+        <v>2</v>
+      </c>
+      <c r="AG11" s="2">
+        <v>2</v>
+      </c>
+      <c r="AH11" s="2">
+        <v>2</v>
+      </c>
+      <c r="AI11" s="2">
+        <v>2</v>
+      </c>
+      <c r="AJ11" s="2">
+        <v>2</v>
+      </c>
+      <c r="AK11" s="2">
+        <v>2</v>
+      </c>
+      <c r="AL11" s="2">
+        <v>2</v>
+      </c>
+      <c r="AM11" s="2">
+        <v>2</v>
+      </c>
+      <c r="AN11" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>2</v>
+      </c>
+      <c r="B12" s="2">
+        <v>2</v>
+      </c>
+      <c r="C12" s="2">
+        <v>2</v>
+      </c>
+      <c r="D12" s="2">
+        <v>2</v>
+      </c>
+      <c r="E12" s="2">
+        <v>2</v>
+      </c>
+      <c r="F12" s="2">
+        <v>2</v>
+      </c>
+      <c r="G12" s="2">
+        <v>2</v>
+      </c>
+      <c r="H12" s="2">
+        <v>2</v>
+      </c>
+      <c r="I12" s="2">
+        <v>2</v>
+      </c>
+      <c r="J12" s="2">
+        <v>2</v>
+      </c>
+      <c r="K12" s="2">
+        <v>2</v>
+      </c>
+      <c r="L12" s="2">
+        <v>2</v>
+      </c>
+      <c r="M12" s="2">
+        <v>2</v>
+      </c>
+      <c r="N12" s="2">
+        <v>2</v>
+      </c>
+      <c r="O12" s="2">
+        <v>2</v>
+      </c>
+      <c r="P12" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q12" s="2">
+        <v>2</v>
+      </c>
+      <c r="R12" s="2">
+        <v>2</v>
+      </c>
+      <c r="S12" s="2">
+        <v>2</v>
+      </c>
+      <c r="T12" s="2">
+        <v>2</v>
+      </c>
+      <c r="U12" s="2">
+        <v>2</v>
+      </c>
+      <c r="V12" s="2">
+        <v>2</v>
+      </c>
+      <c r="W12" s="2">
+        <v>2</v>
+      </c>
+      <c r="X12" s="2">
+        <v>2</v>
+      </c>
+      <c r="Y12" s="2">
+        <v>2</v>
+      </c>
+      <c r="Z12" s="2">
+        <v>2</v>
+      </c>
+      <c r="AA12" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB12" s="2">
+        <v>2</v>
+      </c>
+      <c r="AC12" s="2">
+        <v>2</v>
+      </c>
+      <c r="AD12" s="2">
+        <v>2</v>
+      </c>
+      <c r="AE12" s="2">
+        <v>2</v>
+      </c>
+      <c r="AF12" s="2">
+        <v>2</v>
+      </c>
+      <c r="AG12" s="2">
+        <v>2</v>
+      </c>
+      <c r="AH12" s="2">
+        <v>2</v>
+      </c>
+      <c r="AI12" s="2">
+        <v>2</v>
+      </c>
+      <c r="AJ12" s="2">
+        <v>2</v>
+      </c>
+      <c r="AK12" s="2">
+        <v>2</v>
+      </c>
+      <c r="AL12" s="2">
+        <v>2</v>
+      </c>
+      <c r="AM12" s="2">
+        <v>2</v>
+      </c>
+      <c r="AN12" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>2</v>
+      </c>
+      <c r="B13" s="2">
+        <v>2</v>
+      </c>
+      <c r="C13" s="2">
+        <v>2</v>
+      </c>
+      <c r="D13" s="2">
+        <v>2</v>
+      </c>
+      <c r="E13" s="2">
+        <v>2</v>
+      </c>
+      <c r="F13" s="2">
+        <v>2</v>
+      </c>
+      <c r="G13" s="2">
+        <v>2</v>
+      </c>
+      <c r="H13" s="2">
+        <v>2</v>
+      </c>
+      <c r="I13" s="2">
+        <v>2</v>
+      </c>
+      <c r="J13" s="2">
+        <v>2</v>
+      </c>
+      <c r="K13" s="2">
+        <v>2</v>
+      </c>
+      <c r="L13" s="2">
+        <v>2</v>
+      </c>
+      <c r="M13" s="2">
+        <v>2</v>
+      </c>
+      <c r="N13" s="2">
+        <v>2</v>
+      </c>
+      <c r="O13" s="2">
+        <v>2</v>
+      </c>
+      <c r="P13" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q13" s="2">
+        <v>2</v>
+      </c>
+      <c r="R13" s="2">
+        <v>2</v>
+      </c>
+      <c r="S13" s="2">
+        <v>2</v>
+      </c>
+      <c r="T13" s="2">
+        <v>2</v>
+      </c>
+      <c r="U13" s="2">
+        <v>2</v>
+      </c>
+      <c r="V13" s="2">
+        <v>2</v>
+      </c>
+      <c r="W13" s="2">
+        <v>2</v>
+      </c>
+      <c r="X13" s="2">
+        <v>2</v>
+      </c>
+      <c r="Y13" s="2">
+        <v>2</v>
+      </c>
+      <c r="Z13" s="2">
+        <v>2</v>
+      </c>
+      <c r="AA13" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB13" s="2">
+        <v>2</v>
+      </c>
+      <c r="AC13" s="2">
+        <v>2</v>
+      </c>
+      <c r="AD13" s="2">
+        <v>2</v>
+      </c>
+      <c r="AE13" s="2">
+        <v>2</v>
+      </c>
+      <c r="AF13" s="2">
+        <v>2</v>
+      </c>
+      <c r="AG13" s="2">
+        <v>2</v>
+      </c>
+      <c r="AH13" s="2">
+        <v>2</v>
+      </c>
+      <c r="AI13" s="2">
+        <v>2</v>
+      </c>
+      <c r="AJ13" s="2">
+        <v>2</v>
+      </c>
+      <c r="AK13" s="2">
+        <v>2</v>
+      </c>
+      <c r="AL13" s="2">
+        <v>2</v>
+      </c>
+      <c r="AM13" s="2">
+        <v>2</v>
+      </c>
+      <c r="AN13" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>2</v>
+      </c>
+      <c r="B14" s="2">
+        <v>2</v>
+      </c>
+      <c r="C14" s="2">
+        <v>2</v>
+      </c>
+      <c r="D14" s="2">
+        <v>2</v>
+      </c>
+      <c r="E14" s="2">
+        <v>2</v>
+      </c>
+      <c r="F14" s="2">
+        <v>2</v>
+      </c>
+      <c r="G14" s="2">
+        <v>2</v>
+      </c>
+      <c r="H14" s="2">
+        <v>2</v>
+      </c>
+      <c r="I14" s="2">
+        <v>2</v>
+      </c>
+      <c r="J14" s="2">
+        <v>2</v>
+      </c>
+      <c r="K14" s="2">
+        <v>2</v>
+      </c>
+      <c r="L14" s="2">
+        <v>2</v>
+      </c>
+      <c r="M14" s="2">
+        <v>2</v>
+      </c>
+      <c r="N14" s="2">
+        <v>2</v>
+      </c>
+      <c r="O14" s="2">
+        <v>2</v>
+      </c>
+      <c r="P14" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>2</v>
+      </c>
+      <c r="R14" s="2">
+        <v>2</v>
+      </c>
+      <c r="S14" s="2">
+        <v>2</v>
+      </c>
+      <c r="T14" s="2">
+        <v>2</v>
+      </c>
+      <c r="U14" s="2">
+        <v>2</v>
+      </c>
+      <c r="V14" s="2">
+        <v>2</v>
+      </c>
+      <c r="W14" s="2">
+        <v>2</v>
+      </c>
+      <c r="X14" s="2">
+        <v>2</v>
+      </c>
+      <c r="Y14" s="2">
+        <v>2</v>
+      </c>
+      <c r="Z14" s="2">
+        <v>2</v>
+      </c>
+      <c r="AA14" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB14" s="2">
+        <v>2</v>
+      </c>
+      <c r="AC14" s="2">
+        <v>2</v>
+      </c>
+      <c r="AD14" s="2">
+        <v>2</v>
+      </c>
+      <c r="AE14" s="2">
+        <v>2</v>
+      </c>
+      <c r="AF14" s="2">
+        <v>2</v>
+      </c>
+      <c r="AG14" s="2">
+        <v>2</v>
+      </c>
+      <c r="AH14" s="2">
+        <v>2</v>
+      </c>
+      <c r="AI14" s="2">
+        <v>2</v>
+      </c>
+      <c r="AJ14" s="2">
+        <v>2</v>
+      </c>
+      <c r="AK14" s="2">
+        <v>2</v>
+      </c>
+      <c r="AL14" s="2">
+        <v>2</v>
+      </c>
+      <c r="AM14" s="2">
+        <v>2</v>
+      </c>
+      <c r="AN14" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <v>2</v>
+      </c>
+      <c r="B15" s="2">
+        <v>2</v>
+      </c>
+      <c r="C15" s="2">
+        <v>2</v>
+      </c>
+      <c r="D15" s="2">
+        <v>2</v>
+      </c>
+      <c r="E15" s="2">
+        <v>2</v>
+      </c>
+      <c r="F15" s="2">
+        <v>2</v>
+      </c>
+      <c r="G15" s="2">
+        <v>2</v>
+      </c>
+      <c r="H15" s="2">
+        <v>2</v>
+      </c>
+      <c r="I15" s="2">
+        <v>2</v>
+      </c>
+      <c r="J15" s="2">
+        <v>2</v>
+      </c>
+      <c r="K15" s="2">
+        <v>2</v>
+      </c>
+      <c r="L15" s="2">
+        <v>2</v>
+      </c>
+      <c r="M15" s="2">
+        <v>2</v>
+      </c>
+      <c r="N15" s="2">
+        <v>2</v>
+      </c>
+      <c r="O15" s="2">
+        <v>2</v>
+      </c>
+      <c r="P15" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q15" s="2">
+        <v>2</v>
+      </c>
+      <c r="R15" s="2">
+        <v>2</v>
+      </c>
+      <c r="S15" s="2">
+        <v>2</v>
+      </c>
+      <c r="T15" s="2">
+        <v>2</v>
+      </c>
+      <c r="U15" s="2">
+        <v>2</v>
+      </c>
+      <c r="V15" s="2">
+        <v>2</v>
+      </c>
+      <c r="W15" s="2">
+        <v>2</v>
+      </c>
+      <c r="X15" s="2">
+        <v>2</v>
+      </c>
+      <c r="Y15" s="2">
+        <v>2</v>
+      </c>
+      <c r="Z15" s="2">
+        <v>2</v>
+      </c>
+      <c r="AA15" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB15" s="2">
+        <v>2</v>
+      </c>
+      <c r="AC15" s="2">
+        <v>2</v>
+      </c>
+      <c r="AD15" s="2">
+        <v>2</v>
+      </c>
+      <c r="AE15" s="2">
+        <v>2</v>
+      </c>
+      <c r="AF15" s="2">
+        <v>2</v>
+      </c>
+      <c r="AG15" s="2">
+        <v>2</v>
+      </c>
+      <c r="AH15" s="2">
+        <v>2</v>
+      </c>
+      <c r="AI15" s="2">
+        <v>2</v>
+      </c>
+      <c r="AJ15" s="2">
+        <v>2</v>
+      </c>
+      <c r="AK15" s="2">
+        <v>2</v>
+      </c>
+      <c r="AL15" s="2">
+        <v>2</v>
+      </c>
+      <c r="AM15" s="2">
+        <v>2</v>
+      </c>
+      <c r="AN15" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
+        <v>3</v>
+      </c>
+      <c r="B16" s="3">
+        <v>3</v>
+      </c>
+      <c r="C16" s="3">
+        <v>3</v>
+      </c>
+      <c r="D16" s="3">
+        <v>3</v>
+      </c>
+      <c r="E16" s="3">
+        <v>3</v>
+      </c>
+      <c r="F16" s="3">
+        <v>3</v>
+      </c>
+      <c r="G16" s="3">
+        <v>3</v>
+      </c>
+      <c r="H16" s="3">
+        <v>3</v>
+      </c>
+      <c r="I16" s="3">
+        <v>3</v>
+      </c>
+      <c r="J16" s="3">
+        <v>3</v>
+      </c>
+      <c r="K16" s="3">
+        <v>3</v>
+      </c>
+      <c r="L16" s="3">
+        <v>3</v>
+      </c>
+      <c r="M16" s="3">
+        <v>3</v>
+      </c>
+      <c r="N16" s="3">
+        <v>3</v>
+      </c>
+      <c r="O16" s="3">
+        <v>3</v>
+      </c>
+      <c r="P16" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q16" s="3">
+        <v>3</v>
+      </c>
+      <c r="R16" s="3">
+        <v>3</v>
+      </c>
+      <c r="S16" s="3">
+        <v>3</v>
+      </c>
+      <c r="T16" s="3">
+        <v>3</v>
+      </c>
+      <c r="U16" s="3">
+        <v>3</v>
+      </c>
+      <c r="V16" s="3">
+        <v>3</v>
+      </c>
+      <c r="W16" s="3">
+        <v>3</v>
+      </c>
+      <c r="X16" s="3">
+        <v>3</v>
+      </c>
+      <c r="Y16" s="3">
+        <v>3</v>
+      </c>
+      <c r="Z16" s="3">
+        <v>3</v>
+      </c>
+      <c r="AA16" s="3">
+        <v>3</v>
+      </c>
+      <c r="AB16" s="3">
+        <v>3</v>
+      </c>
+      <c r="AC16" s="3">
+        <v>3</v>
+      </c>
+      <c r="AD16" s="3">
+        <v>3</v>
+      </c>
+      <c r="AE16" s="3">
+        <v>3</v>
+      </c>
+      <c r="AF16" s="3">
+        <v>3</v>
+      </c>
+      <c r="AG16" s="3">
+        <v>3</v>
+      </c>
+      <c r="AH16" s="3">
+        <v>3</v>
+      </c>
+      <c r="AI16" s="3">
+        <v>3</v>
+      </c>
+      <c r="AJ16" s="3">
+        <v>3</v>
+      </c>
+      <c r="AK16" s="3">
+        <v>3</v>
+      </c>
+      <c r="AL16" s="3">
+        <v>3</v>
+      </c>
+      <c r="AM16" s="3">
+        <v>3</v>
+      </c>
+      <c r="AN16" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
+        <v>3</v>
+      </c>
+      <c r="B17" s="3">
+        <v>3</v>
+      </c>
+      <c r="C17" s="3">
+        <v>3</v>
+      </c>
+      <c r="D17" s="3">
+        <v>3</v>
+      </c>
+      <c r="E17" s="3">
+        <v>3</v>
+      </c>
+      <c r="F17" s="3">
+        <v>3</v>
+      </c>
+      <c r="G17" s="3">
+        <v>3</v>
+      </c>
+      <c r="H17" s="3">
+        <v>3</v>
+      </c>
+      <c r="I17" s="3">
+        <v>3</v>
+      </c>
+      <c r="J17" s="3">
+        <v>3</v>
+      </c>
+      <c r="K17" s="3">
+        <v>3</v>
+      </c>
+      <c r="L17" s="3">
+        <v>3</v>
+      </c>
+      <c r="M17" s="3">
+        <v>3</v>
+      </c>
+      <c r="N17" s="3">
+        <v>3</v>
+      </c>
+      <c r="O17" s="3">
+        <v>3</v>
+      </c>
+      <c r="P17" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q17" s="3">
+        <v>3</v>
+      </c>
+      <c r="R17" s="3">
+        <v>3</v>
+      </c>
+      <c r="S17" s="3">
+        <v>3</v>
+      </c>
+      <c r="T17" s="3">
+        <v>3</v>
+      </c>
+      <c r="U17" s="3">
+        <v>3</v>
+      </c>
+      <c r="V17" s="3">
+        <v>3</v>
+      </c>
+      <c r="W17" s="3">
+        <v>3</v>
+      </c>
+      <c r="X17" s="3">
+        <v>3</v>
+      </c>
+      <c r="Y17" s="3">
+        <v>3</v>
+      </c>
+      <c r="Z17" s="3">
+        <v>3</v>
+      </c>
+      <c r="AA17" s="3">
+        <v>3</v>
+      </c>
+      <c r="AB17" s="3">
+        <v>3</v>
+      </c>
+      <c r="AC17" s="3">
+        <v>3</v>
+      </c>
+      <c r="AD17" s="3">
+        <v>3</v>
+      </c>
+      <c r="AE17" s="3">
+        <v>3</v>
+      </c>
+      <c r="AF17" s="3">
+        <v>3</v>
+      </c>
+      <c r="AG17" s="3">
+        <v>3</v>
+      </c>
+      <c r="AH17" s="3">
+        <v>3</v>
+      </c>
+      <c r="AI17" s="3">
+        <v>3</v>
+      </c>
+      <c r="AJ17" s="3">
+        <v>3</v>
+      </c>
+      <c r="AK17" s="3">
+        <v>3</v>
+      </c>
+      <c r="AL17" s="3">
+        <v>3</v>
+      </c>
+      <c r="AM17" s="3">
+        <v>3</v>
+      </c>
+      <c r="AN17" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="3">
+        <v>3</v>
+      </c>
+      <c r="B18" s="3">
+        <v>3</v>
+      </c>
+      <c r="C18" s="3">
+        <v>3</v>
+      </c>
+      <c r="D18" s="3">
+        <v>3</v>
+      </c>
+      <c r="E18" s="3">
+        <v>3</v>
+      </c>
+      <c r="F18" s="3">
+        <v>3</v>
+      </c>
+      <c r="G18" s="3">
+        <v>3</v>
+      </c>
+      <c r="H18" s="3">
+        <v>3</v>
+      </c>
+      <c r="I18" s="3">
+        <v>3</v>
+      </c>
+      <c r="J18" s="3">
+        <v>3</v>
+      </c>
+      <c r="K18" s="3">
+        <v>3</v>
+      </c>
+      <c r="L18" s="3">
+        <v>3</v>
+      </c>
+      <c r="M18" s="3">
+        <v>3</v>
+      </c>
+      <c r="N18" s="3">
+        <v>3</v>
+      </c>
+      <c r="O18" s="3">
+        <v>3</v>
+      </c>
+      <c r="P18" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q18" s="3">
+        <v>3</v>
+      </c>
+      <c r="R18" s="3">
+        <v>3</v>
+      </c>
+      <c r="S18" s="3">
+        <v>3</v>
+      </c>
+      <c r="T18" s="3">
+        <v>3</v>
+      </c>
+      <c r="U18" s="3">
+        <v>3</v>
+      </c>
+      <c r="V18" s="3">
+        <v>3</v>
+      </c>
+      <c r="W18" s="3">
+        <v>3</v>
+      </c>
+      <c r="X18" s="3">
+        <v>3</v>
+      </c>
+      <c r="Y18" s="3">
+        <v>3</v>
+      </c>
+      <c r="Z18" s="3">
+        <v>3</v>
+      </c>
+      <c r="AA18" s="3">
+        <v>3</v>
+      </c>
+      <c r="AB18" s="3">
+        <v>3</v>
+      </c>
+      <c r="AC18" s="3">
+        <v>3</v>
+      </c>
+      <c r="AD18" s="3">
+        <v>3</v>
+      </c>
+      <c r="AE18" s="3">
+        <v>3</v>
+      </c>
+      <c r="AF18" s="3">
+        <v>3</v>
+      </c>
+      <c r="AG18" s="3">
+        <v>3</v>
+      </c>
+      <c r="AH18" s="3">
+        <v>3</v>
+      </c>
+      <c r="AI18" s="3">
+        <v>3</v>
+      </c>
+      <c r="AJ18" s="3">
+        <v>3</v>
+      </c>
+      <c r="AK18" s="3">
+        <v>3</v>
+      </c>
+      <c r="AL18" s="3">
+        <v>3</v>
+      </c>
+      <c r="AM18" s="3">
+        <v>3</v>
+      </c>
+      <c r="AN18" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="3">
+        <v>3</v>
+      </c>
+      <c r="B19" s="3">
+        <v>3</v>
+      </c>
+      <c r="C19" s="3">
+        <v>3</v>
+      </c>
+      <c r="D19" s="3">
+        <v>3</v>
+      </c>
+      <c r="E19" s="3">
+        <v>3</v>
+      </c>
+      <c r="F19" s="3">
+        <v>3</v>
+      </c>
+      <c r="G19" s="3">
+        <v>3</v>
+      </c>
+      <c r="H19" s="3">
+        <v>3</v>
+      </c>
+      <c r="I19" s="3">
+        <v>3</v>
+      </c>
+      <c r="J19" s="3">
+        <v>3</v>
+      </c>
+      <c r="K19" s="3">
+        <v>3</v>
+      </c>
+      <c r="L19" s="3">
+        <v>3</v>
+      </c>
+      <c r="M19" s="3">
+        <v>3</v>
+      </c>
+      <c r="N19" s="3">
+        <v>3</v>
+      </c>
+      <c r="O19" s="3">
+        <v>3</v>
+      </c>
+      <c r="P19" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q19" s="3">
+        <v>3</v>
+      </c>
+      <c r="R19" s="3">
+        <v>3</v>
+      </c>
+      <c r="S19" s="3">
+        <v>3</v>
+      </c>
+      <c r="T19" s="3">
+        <v>3</v>
+      </c>
+      <c r="U19" s="3">
+        <v>3</v>
+      </c>
+      <c r="V19" s="3">
+        <v>3</v>
+      </c>
+      <c r="W19" s="3">
+        <v>3</v>
+      </c>
+      <c r="X19" s="3">
+        <v>3</v>
+      </c>
+      <c r="Y19" s="3">
+        <v>3</v>
+      </c>
+      <c r="Z19" s="3">
+        <v>3</v>
+      </c>
+      <c r="AA19" s="3">
+        <v>3</v>
+      </c>
+      <c r="AB19" s="3">
+        <v>3</v>
+      </c>
+      <c r="AC19" s="3">
+        <v>3</v>
+      </c>
+      <c r="AD19" s="3">
+        <v>3</v>
+      </c>
+      <c r="AE19" s="3">
+        <v>3</v>
+      </c>
+      <c r="AF19" s="3">
+        <v>3</v>
+      </c>
+      <c r="AG19" s="3">
+        <v>3</v>
+      </c>
+      <c r="AH19" s="3">
+        <v>3</v>
+      </c>
+      <c r="AI19" s="3">
+        <v>3</v>
+      </c>
+      <c r="AJ19" s="3">
+        <v>3</v>
+      </c>
+      <c r="AK19" s="3">
+        <v>3</v>
+      </c>
+      <c r="AL19" s="3">
+        <v>3</v>
+      </c>
+      <c r="AM19" s="3">
+        <v>3</v>
+      </c>
+      <c r="AN19" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="3">
+        <v>3</v>
+      </c>
+      <c r="B20" s="3">
+        <v>3</v>
+      </c>
+      <c r="C20" s="3">
+        <v>3</v>
+      </c>
+      <c r="D20" s="3">
+        <v>3</v>
+      </c>
+      <c r="E20" s="3">
+        <v>3</v>
+      </c>
+      <c r="F20" s="3">
+        <v>3</v>
+      </c>
+      <c r="G20" s="3">
+        <v>3</v>
+      </c>
+      <c r="H20" s="3">
+        <v>3</v>
+      </c>
+      <c r="I20" s="3">
+        <v>3</v>
+      </c>
+      <c r="J20" s="3">
+        <v>3</v>
+      </c>
+      <c r="K20" s="3">
+        <v>3</v>
+      </c>
+      <c r="L20" s="3">
+        <v>3</v>
+      </c>
+      <c r="M20" s="3">
+        <v>3</v>
+      </c>
+      <c r="N20" s="3">
+        <v>3</v>
+      </c>
+      <c r="O20" s="3">
+        <v>3</v>
+      </c>
+      <c r="P20" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q20" s="3">
+        <v>3</v>
+      </c>
+      <c r="R20" s="3">
+        <v>3</v>
+      </c>
+      <c r="S20" s="3">
+        <v>3</v>
+      </c>
+      <c r="T20" s="3">
+        <v>3</v>
+      </c>
+      <c r="U20" s="3">
+        <v>3</v>
+      </c>
+      <c r="V20" s="3">
+        <v>3</v>
+      </c>
+      <c r="W20" s="3">
+        <v>3</v>
+      </c>
+      <c r="X20" s="3">
+        <v>3</v>
+      </c>
+      <c r="Y20" s="3">
+        <v>3</v>
+      </c>
+      <c r="Z20" s="3">
+        <v>3</v>
+      </c>
+      <c r="AA20" s="3">
+        <v>3</v>
+      </c>
+      <c r="AB20" s="3">
+        <v>3</v>
+      </c>
+      <c r="AC20" s="3">
+        <v>3</v>
+      </c>
+      <c r="AD20" s="3">
+        <v>3</v>
+      </c>
+      <c r="AE20" s="3">
+        <v>3</v>
+      </c>
+      <c r="AF20" s="3">
+        <v>3</v>
+      </c>
+      <c r="AG20" s="3">
+        <v>3</v>
+      </c>
+      <c r="AH20" s="3">
+        <v>3</v>
+      </c>
+      <c r="AI20" s="3">
+        <v>3</v>
+      </c>
+      <c r="AJ20" s="3">
+        <v>3</v>
+      </c>
+      <c r="AK20" s="3">
+        <v>3</v>
+      </c>
+      <c r="AL20" s="3">
+        <v>3</v>
+      </c>
+      <c r="AM20" s="3">
+        <v>3</v>
+      </c>
+      <c r="AN20" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="3">
+        <v>3</v>
+      </c>
+      <c r="B21" s="3">
+        <v>3</v>
+      </c>
+      <c r="C21" s="3">
+        <v>3</v>
+      </c>
+      <c r="D21" s="3">
+        <v>3</v>
+      </c>
+      <c r="E21" s="3">
+        <v>3</v>
+      </c>
+      <c r="F21" s="3">
+        <v>3</v>
+      </c>
+      <c r="G21" s="3">
+        <v>3</v>
+      </c>
+      <c r="H21" s="3">
+        <v>3</v>
+      </c>
+      <c r="I21" s="3">
+        <v>3</v>
+      </c>
+      <c r="J21" s="3">
+        <v>3</v>
+      </c>
+      <c r="K21" s="3">
+        <v>3</v>
+      </c>
+      <c r="L21" s="3">
+        <v>3</v>
+      </c>
+      <c r="M21" s="3">
+        <v>3</v>
+      </c>
+      <c r="N21" s="3">
+        <v>3</v>
+      </c>
+      <c r="O21" s="3">
+        <v>3</v>
+      </c>
+      <c r="P21" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q21" s="3">
+        <v>3</v>
+      </c>
+      <c r="R21" s="3">
+        <v>3</v>
+      </c>
+      <c r="S21" s="3">
+        <v>3</v>
+      </c>
+      <c r="T21" s="3">
+        <v>3</v>
+      </c>
+      <c r="U21" s="3">
+        <v>3</v>
+      </c>
+      <c r="V21" s="3">
+        <v>3</v>
+      </c>
+      <c r="W21" s="3">
+        <v>3</v>
+      </c>
+      <c r="X21" s="3">
+        <v>3</v>
+      </c>
+      <c r="Y21" s="3">
+        <v>3</v>
+      </c>
+      <c r="Z21" s="3">
+        <v>3</v>
+      </c>
+      <c r="AA21" s="3">
+        <v>3</v>
+      </c>
+      <c r="AB21" s="3">
+        <v>3</v>
+      </c>
+      <c r="AC21" s="3">
+        <v>3</v>
+      </c>
+      <c r="AD21" s="3">
+        <v>3</v>
+      </c>
+      <c r="AE21" s="3">
+        <v>3</v>
+      </c>
+      <c r="AF21" s="3">
+        <v>3</v>
+      </c>
+      <c r="AG21" s="3">
+        <v>3</v>
+      </c>
+      <c r="AH21" s="3">
+        <v>3</v>
+      </c>
+      <c r="AI21" s="3">
+        <v>3</v>
+      </c>
+      <c r="AJ21" s="3">
+        <v>3</v>
+      </c>
+      <c r="AK21" s="3">
+        <v>3</v>
+      </c>
+      <c r="AL21" s="3">
+        <v>3</v>
+      </c>
+      <c r="AM21" s="3">
+        <v>3</v>
+      </c>
+      <c r="AN21" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="3">
+        <v>3</v>
+      </c>
+      <c r="B22" s="3">
+        <v>3</v>
+      </c>
+      <c r="C22" s="3">
+        <v>3</v>
+      </c>
+      <c r="D22" s="3">
+        <v>3</v>
+      </c>
+      <c r="E22" s="3">
+        <v>3</v>
+      </c>
+      <c r="F22" s="3">
+        <v>3</v>
+      </c>
+      <c r="G22" s="3">
+        <v>3</v>
+      </c>
+      <c r="H22" s="3">
+        <v>3</v>
+      </c>
+      <c r="I22" s="3">
+        <v>3</v>
+      </c>
+      <c r="J22" s="3">
+        <v>3</v>
+      </c>
+      <c r="K22" s="3">
+        <v>3</v>
+      </c>
+      <c r="L22" s="3">
+        <v>3</v>
+      </c>
+      <c r="M22" s="3">
+        <v>3</v>
+      </c>
+      <c r="N22" s="3">
+        <v>3</v>
+      </c>
+      <c r="O22" s="3">
+        <v>3</v>
+      </c>
+      <c r="P22" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q22" s="3">
+        <v>3</v>
+      </c>
+      <c r="R22" s="3">
+        <v>3</v>
+      </c>
+      <c r="S22" s="3">
+        <v>3</v>
+      </c>
+      <c r="T22" s="3">
+        <v>3</v>
+      </c>
+      <c r="U22" s="3">
+        <v>3</v>
+      </c>
+      <c r="V22" s="3">
+        <v>3</v>
+      </c>
+      <c r="W22" s="3">
+        <v>3</v>
+      </c>
+      <c r="X22" s="3">
+        <v>3</v>
+      </c>
+      <c r="Y22" s="3">
+        <v>3</v>
+      </c>
+      <c r="Z22" s="3">
+        <v>3</v>
+      </c>
+      <c r="AA22" s="3">
+        <v>3</v>
+      </c>
+      <c r="AB22" s="3">
+        <v>3</v>
+      </c>
+      <c r="AC22" s="3">
+        <v>3</v>
+      </c>
+      <c r="AD22" s="3">
+        <v>3</v>
+      </c>
+      <c r="AE22" s="3">
+        <v>3</v>
+      </c>
+      <c r="AF22" s="3">
+        <v>3</v>
+      </c>
+      <c r="AG22" s="3">
+        <v>3</v>
+      </c>
+      <c r="AH22" s="3">
+        <v>3</v>
+      </c>
+      <c r="AI22" s="3">
+        <v>3</v>
+      </c>
+      <c r="AJ22" s="3">
+        <v>3</v>
+      </c>
+      <c r="AK22" s="3">
+        <v>3</v>
+      </c>
+      <c r="AL22" s="3">
+        <v>3</v>
+      </c>
+      <c r="AM22" s="3">
+        <v>3</v>
+      </c>
+      <c r="AN22" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="3">
+        <v>3</v>
+      </c>
+      <c r="B23" s="3">
+        <v>3</v>
+      </c>
+      <c r="C23" s="3">
+        <v>3</v>
+      </c>
+      <c r="D23" s="3">
+        <v>3</v>
+      </c>
+      <c r="E23" s="3">
+        <v>3</v>
+      </c>
+      <c r="F23" s="3">
+        <v>3</v>
+      </c>
+      <c r="G23" s="3">
+        <v>3</v>
+      </c>
+      <c r="H23" s="3">
+        <v>3</v>
+      </c>
+      <c r="I23" s="3">
+        <v>3</v>
+      </c>
+      <c r="J23" s="3">
+        <v>3</v>
+      </c>
+      <c r="K23" s="3">
+        <v>3</v>
+      </c>
+      <c r="L23" s="3">
+        <v>3</v>
+      </c>
+      <c r="M23" s="3">
+        <v>3</v>
+      </c>
+      <c r="N23" s="3">
+        <v>3</v>
+      </c>
+      <c r="O23" s="3">
+        <v>3</v>
+      </c>
+      <c r="P23" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q23" s="3">
+        <v>3</v>
+      </c>
+      <c r="R23" s="3">
+        <v>3</v>
+      </c>
+      <c r="S23" s="3">
+        <v>3</v>
+      </c>
+      <c r="T23" s="3">
+        <v>3</v>
+      </c>
+      <c r="U23" s="3">
+        <v>3</v>
+      </c>
+      <c r="V23" s="3">
+        <v>3</v>
+      </c>
+      <c r="W23" s="3">
+        <v>3</v>
+      </c>
+      <c r="X23" s="3">
+        <v>3</v>
+      </c>
+      <c r="Y23" s="3">
+        <v>3</v>
+      </c>
+      <c r="Z23" s="3">
+        <v>3</v>
+      </c>
+      <c r="AA23" s="3">
+        <v>3</v>
+      </c>
+      <c r="AB23" s="3">
+        <v>3</v>
+      </c>
+      <c r="AC23" s="3">
+        <v>3</v>
+      </c>
+      <c r="AD23" s="3">
+        <v>3</v>
+      </c>
+      <c r="AE23" s="3">
+        <v>3</v>
+      </c>
+      <c r="AF23" s="3">
+        <v>3</v>
+      </c>
+      <c r="AG23" s="3">
+        <v>3</v>
+      </c>
+      <c r="AH23" s="3">
+        <v>3</v>
+      </c>
+      <c r="AI23" s="3">
+        <v>3</v>
+      </c>
+      <c r="AJ23" s="3">
+        <v>3</v>
+      </c>
+      <c r="AK23" s="3">
+        <v>3</v>
+      </c>
+      <c r="AL23" s="3">
+        <v>3</v>
+      </c>
+      <c r="AM23" s="3">
+        <v>3</v>
+      </c>
+      <c r="AN23" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="3">
+        <v>3</v>
+      </c>
+      <c r="B24" s="3">
+        <v>3</v>
+      </c>
+      <c r="C24" s="3">
+        <v>3</v>
+      </c>
+      <c r="D24" s="3">
+        <v>3</v>
+      </c>
+      <c r="E24" s="3">
+        <v>3</v>
+      </c>
+      <c r="F24" s="3">
+        <v>3</v>
+      </c>
+      <c r="G24" s="3">
+        <v>3</v>
+      </c>
+      <c r="H24" s="3">
+        <v>3</v>
+      </c>
+      <c r="I24" s="3">
+        <v>3</v>
+      </c>
+      <c r="J24" s="3">
+        <v>3</v>
+      </c>
+      <c r="K24" s="3">
+        <v>3</v>
+      </c>
+      <c r="L24" s="3">
+        <v>3</v>
+      </c>
+      <c r="M24" s="3">
+        <v>3</v>
+      </c>
+      <c r="N24" s="3">
+        <v>3</v>
+      </c>
+      <c r="O24" s="3">
+        <v>3</v>
+      </c>
+      <c r="P24" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q24" s="3">
+        <v>3</v>
+      </c>
+      <c r="R24" s="3">
+        <v>3</v>
+      </c>
+      <c r="S24" s="3">
+        <v>3</v>
+      </c>
+      <c r="T24" s="3">
+        <v>3</v>
+      </c>
+      <c r="U24" s="3">
+        <v>3</v>
+      </c>
+      <c r="V24" s="3">
+        <v>3</v>
+      </c>
+      <c r="W24" s="3">
+        <v>3</v>
+      </c>
+      <c r="X24" s="3">
+        <v>3</v>
+      </c>
+      <c r="Y24" s="3">
+        <v>3</v>
+      </c>
+      <c r="Z24" s="3">
+        <v>3</v>
+      </c>
+      <c r="AA24" s="3">
+        <v>3</v>
+      </c>
+      <c r="AB24" s="3">
+        <v>3</v>
+      </c>
+      <c r="AC24" s="3">
+        <v>3</v>
+      </c>
+      <c r="AD24" s="3">
+        <v>3</v>
+      </c>
+      <c r="AE24" s="3">
+        <v>3</v>
+      </c>
+      <c r="AF24" s="3">
+        <v>3</v>
+      </c>
+      <c r="AG24" s="3">
+        <v>3</v>
+      </c>
+      <c r="AH24" s="3">
+        <v>3</v>
+      </c>
+      <c r="AI24" s="3">
+        <v>3</v>
+      </c>
+      <c r="AJ24" s="3">
+        <v>3</v>
+      </c>
+      <c r="AK24" s="3">
+        <v>3</v>
+      </c>
+      <c r="AL24" s="3">
+        <v>3</v>
+      </c>
+      <c r="AM24" s="3">
+        <v>3</v>
+      </c>
+      <c r="AN24" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="3">
+        <v>3</v>
+      </c>
+      <c r="B25" s="3">
+        <v>3</v>
+      </c>
+      <c r="C25" s="3">
+        <v>3</v>
+      </c>
+      <c r="D25" s="3">
+        <v>3</v>
+      </c>
+      <c r="E25" s="3">
+        <v>3</v>
+      </c>
+      <c r="F25" s="3">
+        <v>3</v>
+      </c>
+      <c r="G25" s="3">
+        <v>3</v>
+      </c>
+      <c r="H25" s="3">
+        <v>3</v>
+      </c>
+      <c r="I25" s="3">
+        <v>3</v>
+      </c>
+      <c r="J25" s="3">
+        <v>3</v>
+      </c>
+      <c r="K25" s="3">
+        <v>3</v>
+      </c>
+      <c r="L25" s="3">
+        <v>3</v>
+      </c>
+      <c r="M25" s="3">
+        <v>3</v>
+      </c>
+      <c r="N25" s="3">
+        <v>3</v>
+      </c>
+      <c r="O25" s="3">
+        <v>3</v>
+      </c>
+      <c r="P25" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q25" s="3">
+        <v>3</v>
+      </c>
+      <c r="R25" s="3">
+        <v>3</v>
+      </c>
+      <c r="S25" s="3">
+        <v>3</v>
+      </c>
+      <c r="T25" s="3">
+        <v>3</v>
+      </c>
+      <c r="U25" s="3">
+        <v>3</v>
+      </c>
+      <c r="V25" s="3">
+        <v>3</v>
+      </c>
+      <c r="W25" s="3">
+        <v>3</v>
+      </c>
+      <c r="X25" s="3">
+        <v>3</v>
+      </c>
+      <c r="Y25" s="3">
+        <v>3</v>
+      </c>
+      <c r="Z25" s="3">
+        <v>3</v>
+      </c>
+      <c r="AA25" s="3">
+        <v>3</v>
+      </c>
+      <c r="AB25" s="3">
+        <v>3</v>
+      </c>
+      <c r="AC25" s="3">
+        <v>3</v>
+      </c>
+      <c r="AD25" s="3">
+        <v>3</v>
+      </c>
+      <c r="AE25" s="3">
+        <v>3</v>
+      </c>
+      <c r="AF25" s="3">
+        <v>3</v>
+      </c>
+      <c r="AG25" s="3">
+        <v>3</v>
+      </c>
+      <c r="AH25" s="3">
+        <v>3</v>
+      </c>
+      <c r="AI25" s="3">
+        <v>3</v>
+      </c>
+      <c r="AJ25" s="3">
+        <v>3</v>
+      </c>
+      <c r="AK25" s="3">
+        <v>3</v>
+      </c>
+      <c r="AL25" s="3">
+        <v>3</v>
+      </c>
+      <c r="AM25" s="3">
+        <v>3</v>
+      </c>
+      <c r="AN25" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="3">
+        <v>3</v>
+      </c>
+      <c r="B26" s="3">
+        <v>3</v>
+      </c>
+      <c r="C26" s="3">
+        <v>3</v>
+      </c>
+      <c r="D26" s="3">
+        <v>3</v>
+      </c>
+      <c r="E26" s="3">
+        <v>3</v>
+      </c>
+      <c r="F26" s="3">
+        <v>3</v>
+      </c>
+      <c r="G26" s="3">
+        <v>3</v>
+      </c>
+      <c r="H26" s="3">
+        <v>3</v>
+      </c>
+      <c r="I26" s="3">
+        <v>3</v>
+      </c>
+      <c r="J26" s="3">
+        <v>3</v>
+      </c>
+      <c r="K26" s="3">
+        <v>3</v>
+      </c>
+      <c r="L26" s="3">
+        <v>3</v>
+      </c>
+      <c r="M26" s="3">
+        <v>3</v>
+      </c>
+      <c r="N26" s="3">
+        <v>3</v>
+      </c>
+      <c r="O26" s="3">
+        <v>3</v>
+      </c>
+      <c r="P26" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q26" s="3">
+        <v>3</v>
+      </c>
+      <c r="R26" s="3">
+        <v>3</v>
+      </c>
+      <c r="S26" s="3">
+        <v>3</v>
+      </c>
+      <c r="T26" s="3">
+        <v>3</v>
+      </c>
+      <c r="U26" s="3">
+        <v>3</v>
+      </c>
+      <c r="V26" s="3">
+        <v>3</v>
+      </c>
+      <c r="W26" s="3">
+        <v>3</v>
+      </c>
+      <c r="X26" s="3">
+        <v>3</v>
+      </c>
+      <c r="Y26" s="3">
+        <v>3</v>
+      </c>
+      <c r="Z26" s="3">
+        <v>3</v>
+      </c>
+      <c r="AA26" s="3">
+        <v>3</v>
+      </c>
+      <c r="AB26" s="3">
+        <v>3</v>
+      </c>
+      <c r="AC26" s="3">
+        <v>3</v>
+      </c>
+      <c r="AD26" s="3">
+        <v>3</v>
+      </c>
+      <c r="AE26" s="3">
+        <v>3</v>
+      </c>
+      <c r="AF26" s="3">
+        <v>3</v>
+      </c>
+      <c r="AG26" s="3">
+        <v>3</v>
+      </c>
+      <c r="AH26" s="3">
+        <v>3</v>
+      </c>
+      <c r="AI26" s="3">
+        <v>3</v>
+      </c>
+      <c r="AJ26" s="3">
+        <v>3</v>
+      </c>
+      <c r="AK26" s="3">
+        <v>3</v>
+      </c>
+      <c r="AL26" s="3">
+        <v>3</v>
+      </c>
+      <c r="AM26" s="3">
+        <v>3</v>
+      </c>
+      <c r="AN26" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="18">
+        <v>4</v>
+      </c>
+      <c r="B27" s="18">
+        <v>4</v>
+      </c>
+      <c r="C27" s="18">
+        <v>4</v>
+      </c>
+      <c r="D27" s="18">
+        <v>4</v>
+      </c>
+      <c r="E27" s="18">
+        <v>4</v>
+      </c>
+      <c r="F27" s="18">
+        <v>4</v>
+      </c>
+      <c r="G27" s="18">
+        <v>4</v>
+      </c>
+      <c r="H27" s="18">
+        <v>4</v>
+      </c>
+      <c r="I27" s="18">
+        <v>4</v>
+      </c>
+      <c r="J27" s="18">
+        <v>4</v>
+      </c>
+      <c r="K27" s="18">
+        <v>4</v>
+      </c>
+      <c r="L27" s="18">
+        <v>4</v>
+      </c>
+      <c r="M27" s="18">
+        <v>4</v>
+      </c>
+      <c r="N27" s="18">
+        <v>4</v>
+      </c>
+      <c r="O27" s="18">
+        <v>4</v>
+      </c>
+      <c r="P27" s="18">
+        <v>4</v>
+      </c>
+      <c r="Q27" s="18">
+        <v>4</v>
+      </c>
+      <c r="R27" s="18">
+        <v>4</v>
+      </c>
+      <c r="S27" s="18">
+        <v>4</v>
+      </c>
+      <c r="T27" s="18">
+        <v>4</v>
+      </c>
+      <c r="U27" s="18">
+        <v>4</v>
+      </c>
+      <c r="V27" s="18">
+        <v>4</v>
+      </c>
+      <c r="W27" s="18">
+        <v>4</v>
+      </c>
+      <c r="X27" s="18">
+        <v>4</v>
+      </c>
+      <c r="Y27" s="18">
+        <v>4</v>
+      </c>
+      <c r="Z27" s="18">
+        <v>4</v>
+      </c>
+      <c r="AA27" s="18">
+        <v>4</v>
+      </c>
+      <c r="AB27" s="18">
+        <v>4</v>
+      </c>
+      <c r="AC27" s="18">
+        <v>4</v>
+      </c>
+      <c r="AD27" s="18">
+        <v>4</v>
+      </c>
+      <c r="AE27" s="18">
+        <v>4</v>
+      </c>
+      <c r="AF27" s="18">
+        <v>4</v>
+      </c>
+      <c r="AG27" s="18">
+        <v>4</v>
+      </c>
+      <c r="AH27" s="18">
+        <v>4</v>
+      </c>
+      <c r="AI27" s="18">
+        <v>4</v>
+      </c>
+      <c r="AJ27" s="18">
+        <v>4</v>
+      </c>
+      <c r="AK27" s="18">
+        <v>4</v>
+      </c>
+      <c r="AL27" s="18">
+        <v>4</v>
+      </c>
+      <c r="AM27" s="18">
+        <v>4</v>
+      </c>
+      <c r="AN27" s="18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="18">
+        <v>4</v>
+      </c>
+      <c r="B28" s="18">
+        <v>4</v>
+      </c>
+      <c r="C28" s="18">
+        <v>4</v>
+      </c>
+      <c r="D28" s="18">
+        <v>4</v>
+      </c>
+      <c r="E28" s="18">
+        <v>4</v>
+      </c>
+      <c r="F28" s="18">
+        <v>4</v>
+      </c>
+      <c r="G28" s="18">
+        <v>4</v>
+      </c>
+      <c r="H28" s="18">
+        <v>4</v>
+      </c>
+      <c r="I28" s="18">
+        <v>4</v>
+      </c>
+      <c r="J28" s="18">
+        <v>4</v>
+      </c>
+      <c r="K28" s="18">
+        <v>4</v>
+      </c>
+      <c r="L28" s="18">
+        <v>4</v>
+      </c>
+      <c r="M28" s="18">
+        <v>4</v>
+      </c>
+      <c r="N28" s="18">
+        <v>4</v>
+      </c>
+      <c r="O28" s="18">
+        <v>4</v>
+      </c>
+      <c r="P28" s="18">
+        <v>4</v>
+      </c>
+      <c r="Q28" s="18">
+        <v>4</v>
+      </c>
+      <c r="R28" s="18">
+        <v>4</v>
+      </c>
+      <c r="S28" s="18">
+        <v>4</v>
+      </c>
+      <c r="T28" s="18">
+        <v>4</v>
+      </c>
+      <c r="U28" s="18">
+        <v>4</v>
+      </c>
+      <c r="V28" s="18">
+        <v>4</v>
+      </c>
+      <c r="W28" s="18">
+        <v>4</v>
+      </c>
+      <c r="X28" s="18">
+        <v>4</v>
+      </c>
+      <c r="Y28" s="18">
+        <v>4</v>
+      </c>
+      <c r="Z28" s="18">
+        <v>4</v>
+      </c>
+      <c r="AA28" s="18">
+        <v>4</v>
+      </c>
+      <c r="AB28" s="18">
+        <v>4</v>
+      </c>
+      <c r="AC28" s="18">
+        <v>4</v>
+      </c>
+      <c r="AD28" s="18">
+        <v>4</v>
+      </c>
+      <c r="AE28" s="18">
+        <v>4</v>
+      </c>
+      <c r="AF28" s="18">
+        <v>4</v>
+      </c>
+      <c r="AG28" s="18">
+        <v>4</v>
+      </c>
+      <c r="AH28" s="18">
+        <v>4</v>
+      </c>
+      <c r="AI28" s="18">
+        <v>4</v>
+      </c>
+      <c r="AJ28" s="18">
+        <v>4</v>
+      </c>
+      <c r="AK28" s="18">
+        <v>4</v>
+      </c>
+      <c r="AL28" s="18">
+        <v>4</v>
+      </c>
+      <c r="AM28" s="18">
+        <v>4</v>
+      </c>
+      <c r="AN28" s="18">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F28B1C7F-4EC7-B549-BE8D-0AB0CF2912E7}">
   <dimension ref="A1:AN27"/>
@@ -44905,7 +48340,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E1D5664-FD82-904C-987A-24EAE06E9377}">
   <dimension ref="A1:AN27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AP13" sqref="AP13"/>
     </sheetView>
   </sheetViews>

</xml_diff>